<commit_message>
Tech WIP + Layout fixes
</commit_message>
<xml_diff>
--- a/Template_Data.xlsx
+++ b/Template_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12165" tabRatio="796" firstSheet="7" activeTab="16"/>
+    <workbookView windowWidth="14400" windowHeight="12255" tabRatio="796" firstSheet="7" activeTab="16"/>
   </bookViews>
   <sheets>
     <sheet name="Actions" sheetId="14" r:id="rId1"/>
@@ -7028,7 +7028,7 @@
     <t>DFDA23</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Экстренное развёртывание&lt;/fs&gt;</t>
+    <t>&lt;fs=56&gt;Экстренное развёртывание&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;f=Myriad Pro Light;50;1;0;0;0&gt;&lt;ls=75&gt;&lt;/f&gt;&lt;f=Myriad Pro;50;1;0;0;0&gt;ДЕЙСТВИЕ: &lt;/f&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt;переверните эту карту, чтобы разместить или переместить вашу базу на подконтрольную вам планету, на которой нет базы.&lt;/ls&gt;&lt;/f&gt;</t>
@@ -7058,7 +7058,7 @@
     <t>B61FCE</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Объединённые Репликаторы&lt;/fs&gt;</t>
+    <t>&lt;fs=56&gt;Объединённые Репликаторы&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;f=Myriad Pro Light;50;1;0;0;0&gt;&lt;ls=75&gt;Когда хотя бы 1 ваш отряд использует способность &lt;/f&gt;&lt;push=0;17&gt;&lt;f=Russo One;40;0;0;0;0&gt;«ПРОИЗВОДСТВО»&lt;/f&gt;&lt;push=0;-17&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt;, можете перевернуть эту карту, чтобы поменять значение производства этого отряда со значением производства другого отряда на игровом поле, или добавлять +2 к общему значению производства этих отрядов.&lt;/ls&gt;&lt;/f&gt;</t>
@@ -7067,10 +7067,10 @@
     <t>Келдарская Торговая Конфедерация</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Экстренная Мобилизация&lt;/fs&gt;</t>
-  </si>
-  <si>
-    <t>&lt;fs=40&gt;Келдарская Торговая Конфедерация&lt;/fs&gt;</t>
+    <t>&lt;fs=56&gt;Экстренная Мобилизация&lt;/fs&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fs=32&gt;Келдарская Торговая Конфедерация&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;f=Myriad Pro Light;50;1;0;0;0&gt;&lt;ls=75&gt;В конце вашего хода можете перевернуть эту карту и потратить 1 жетон из вашего стратегического резерва, чтобы убрать жетон приказа из системы, в которой есть хотя бы 1 ваша база.&lt;/ls&gt;&lt;/f&gt;</t>
@@ -7136,7 +7136,7 @@
     <t>Флотилия Ди-Мон</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Программы принудительной мобилизации&lt;/fs&gt;</t>
+    <t>&lt;fs=36&gt;Программы принудительной мобилизации&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;fs=40&gt;Флотилия Ди-Мон&lt;/fs&gt;</t>
@@ -7175,7 +7175,7 @@
     <t>DDD143</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Зашифрованный Торговый Узел&lt;/fs&gt;</t>
+    <t>&lt;fs=44&gt;Зашифрованный Торговый Узел&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;f=Myriad Pro Light;50;1;0;0;0&gt;&lt;ls=75&gt;Можете перевернуть эту карту, чтобы позволить игроку обменять 1 из его реликвий или карт политики в рамках сделки.&lt;/ls&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;&lt;ls=75&gt;Вы всегда голосуете последним во время фазы политики. После принятия решения, за которое вы проголосовали или которое вы предсказали, каждый игрок, проголосовавший за этот результат, получает 1 продукцию.&lt;/ls&gt;&lt;/f&gt;</t>
@@ -7208,7 +7208,7 @@
     <t>&lt;fs=64&gt;Сеть послов&lt;/fs&gt;</t>
   </si>
   <si>
-    <t>&lt;fs=40&gt;Содружество Свободных Систем&lt;/fs&gt;</t>
+    <t>&lt;fs=36&gt;Содружество Свободных Систем&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;f=Myriad Pro Light;50;1;0;0;0&gt;&lt;ls=75&gt;В начале фазы политики вы можете выбрать и перевернуть 1 культурную, 1 опасную и 1 промышленную планету любых игроков.&lt;/ls&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;&lt;ls=75&gt;Когда вы отдаёте хотя бы 1 голос и переворачиваете для голосования хотя бы по 1 планете каждого из 3 типов, можете отдать 4 дополнительных голоса.&lt;/ls&gt;&lt;/f&gt;</t>
@@ -7223,7 +7223,7 @@
     <t>8247AC</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Оперативная ударная группа&lt;/fs&gt;</t>
+    <t>&lt;fs=44&gt;Оперативная ударная группа&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;f=Myriad Pro Light;50;1;0;0;0&gt;&lt;ls=75&gt;В начале наземного боя вы можете бросить 1 кубик за каждый из ваших наземных отрядов (не более 2) на этой планете. За каждый результат, равный или превышающий значение боя этого отряда, нанесите 1 попадание, которое ваш противник должен присвоить одному из своих наземных отрядов.&lt;/ls&gt;&lt;/f&gt;</t>
@@ -7232,7 +7232,7 @@
     <t>Рейдеры Гемины</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Импланты Боевых Маршей&lt;/fs&gt;</t>
+    <t>&lt;fs=56&gt;Импланты Боевых Маршей&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;fs=40&gt;Рейдеры Гемины&lt;/fs&gt;</t>
@@ -7256,7 +7256,7 @@
     <t>Странники Готи</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Сетевая система управления&lt;/fs&gt;</t>
+    <t>&lt;fs=56&gt;Сетевая система управления&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;fs=40&gt;Странники Готи&lt;/fs&gt;</t>
@@ -7268,7 +7268,7 @@
     <t>CB662E</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Параллельное Производство&lt;/fs&gt;</t>
+    <t>&lt;fs=55&gt;Параллельное Производство&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;f=Myriad Pro Light;50;1;0;0;0&gt;&lt;ls=75&gt;Когда вы производите хотя бы 1 отряд, можете произвести 1 дополнительный отряд в каждой из 2 систем, в которых есть хотя бы 1 ваш корабль и хотя бы 1 ваш жетон приказа.&lt;/ls&gt;&lt;/f&gt;</t>
@@ -7277,10 +7277,10 @@
     <t>Горнодобывающий консорциум «ПРГ»</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Сверхскоростные двигатели&lt;/fs&gt;</t>
-  </si>
-  <si>
-    <t>&lt;fs=40&gt;Горнодобывающий консорциум «ПРГ»&lt;/fs&gt;</t>
+    <t>&lt;fs=56&gt;Сверхскоростные двигатели&lt;/fs&gt;</t>
+  </si>
+  <si>
+    <t>&lt;fs=30&gt;Горнодобывающий консорциум «ПРГ»&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;f=Myriad Pro Light;50;1;0;0;0&gt;&lt;ls=75&gt;Во время передвижения, можете добавить +1 к значению полёта каждого вашего корабля, который не перевозит отряды.&lt;/ls&gt;&lt;/f&gt;</t>
@@ -7313,7 +7313,7 @@
     <t>F6DF8E</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Когнитивное хранилище данных&lt;/fs&gt;</t>
+    <t>&lt;fs=44&gt;Когнитивное хранилище данных&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;f=Myriad Pro Light;50;1;0;0;0&gt;&lt;ls=75&gt;В начале фазы статуса вы можете потратить 3 товара, чтобы исследовать 1 технологию.&lt;/ls&gt;&lt;/f&gt;</t>
@@ -7358,7 +7358,7 @@
     <t>D53815</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Замаскированные Застрельщики&lt;/fs&gt;</t>
+    <t>&lt;fs=44&gt;Замаскированные Застрельщики&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;f=Myriad Pro Light;50;1;0;0;0&gt;&lt;ls=75&gt;В начале космического боя вы можете выбрать 1 ваш корабль в активной системе, который не начинал действие в этой системе; бросьте кубик. При результате, равном или превышающем значение боя этого корабля, нанесите 1 попадание, которое ваш противник должен присвоить 1 из своих кораблей.&lt;/ls&gt;&lt;/f&gt;</t>
@@ -7367,7 +7367,7 @@
     <t>Орден Колума</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Прикладная Биотермодинамика&lt;/fs&gt;</t>
+    <t>&lt;fs=44&gt;Прикладная Биотермодинамика&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;fs=40&gt;Орден Колума&lt;/fs&gt;</t>
@@ -7469,7 +7469,7 @@
     <t>C4662C</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Передовые Тактические Системы&lt;/fs&gt;</t>
+    <t>&lt;fs=44&gt;Передовые Тактические Системы&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;f=Myriad Pro Light;50;1;0;0;0&gt;&lt;ls=75&gt;После того как вы изгнали хотя бы 1 фрагмент реликвии, разведали планету или жетон пограничья, положите 1 продукцию на эту карту.&lt;/ls&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;&lt;ls=75&gt;В начале раунда боя уберите любое количество продукции с этой карты, чтобы перебросить такое же количество или меньше кубиков во время этого раунда боя.&lt;/ls&gt;&lt;/f&gt;</t>
@@ -7520,7 +7520,7 @@
     <t>Протекторат Мирведы</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Орбитальная защитная сеть&lt;/fs&gt;</t>
+    <t>&lt;fs=56&gt;Орбитальная защитная сеть&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;fs=40&gt;Протекторат Мирведы&lt;/fs&gt;</t>
@@ -7565,7 +7565,7 @@
     <t>Мико-Ментори</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Психоактивное Вооружение&lt;/fs&gt;</t>
+    <t>&lt;fs=56&gt;Психоактивное Вооружение&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;fs=40&gt;Мико-Ментори&lt;/fs&gt;</t>
@@ -7589,7 +7589,7 @@
     <t>Звёздные Короли Нивин</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Ракеты пробуждения пустоты&lt;/fs&gt;</t>
+    <t>&lt;fs=44&gt;Ракеты пробуждения пустоты&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;fs=40&gt;Звёздные Короли Нивин&lt;/fs&gt;</t>
@@ -7628,7 +7628,7 @@
     <t>Лига Олрадинов</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Операции под чужим флагом&lt;/fs&gt;</t>
+    <t>&lt;fs=54&gt;Операции под чужим флагом&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;fs=40&gt;Лига Олрадинов&lt;/fs&gt;</t>
@@ -7643,7 +7643,7 @@
     <t>06EFF3</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Геосимпатический Ускоритель&lt;/fs&gt;</t>
+    <t>&lt;fs=44&gt;Геосимпатический Ускоритель&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;f=Myriad Pro Light;50;1;0;0;0&gt;&lt;ls=75&gt;После того как вы активировали систему, можете перевернуть подконтрольную вам планету того же типа, что и планета в активной системе, чтобы добавить +1 к значению полёта каждого вашего корабля во время этого тактического действия.&lt;/ls&gt;&lt;/f&gt;</t>
@@ -7679,7 +7679,7 @@
     <t>Мехатроника Ро’Дна</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Контрактные обязательства&lt;/fs&gt;</t>
+    <t>&lt;fs=56&gt;Контрактные обязательства&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;fs=40&gt;Мехатроника Ро’Дна&lt;/fs&gt;</t>
@@ -7697,7 +7697,7 @@
     <t>Синдикат Тнелис</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Полётная система Дедалона&lt;/fs&gt;</t>
+    <t>&lt;fs=56&gt;Полётная система Дедалона&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;fs=40&gt;Синдикат Тнелис&lt;/fs&gt;</t>
@@ -7736,7 +7736,7 @@
     <t>D6EF3D</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Ударные отряды Кровоза&lt;/fs&gt;</t>
+    <t>&lt;fs=56&gt;Ударные отряды Кровоза&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;f=Myriad Pro Light;50;1;0;0;0&gt;&lt;ls=75&gt;После того как корабль другого игрока использовал способность &lt;/f&gt;&lt;push=0;17&gt;&lt;f=Russo One;40;0;0;0;0&gt;«ПОГЛОЩЕНИЕ УРОНА»&lt;/f&gt;&lt;push=0;-17&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt; для отмены попадания, нанесённого вашими отрядами или способностями, можете перевернуть эту карту, чтобы уничтожить этот отряд.&lt;/ls&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;&lt;ls=75&gt;После того как вы наносите хотя бы 1 попадание во время раунда боя, можете потратить 1 товар, чтобы нанести 1 дополнительное попадание.&lt;/ls&gt;&lt;/f&gt;</t>
@@ -8267,13 +8267,13 @@
     <t>&lt;f=Myriad Pro Light;50;1;0;0;0&gt;&lt;ls=75&gt;Этот отряд может быть уничтожен только присвоенным ему попаданием.&lt;/ls&gt;&lt;/f&gt;</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Тяжёлый бомбардировщик I&lt;/fs&gt;</t>
+    <t>&lt;fs=54&gt;Тяжёлый бомбардировщик I&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;fs=40&gt;Истребитель Ли-Джо&lt;/fs&gt;</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Тяжёлый бомбардировщик II&lt;/fs&gt;</t>
+    <t>&lt;fs=54&gt;Тяжёлый бомбардировщик II&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;fs=64&gt;Элита Оро-Жин&lt;/fs&gt;</t>
@@ -8403,7 +8403,7 @@
     <t>&lt;f=Myriad Pro Light;50;1;0;0;0&gt;&lt;ls=75&gt;Когда отряд в этой системе должен быть уничтожен, вы можете вместо этого убрать его с игрового поля.&lt;/ls&gt;&lt;/f&gt;</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Хранитель Вспышки Пустоты I&lt;/fs&gt;</t>
+    <t>&lt;fs=44&gt;Хранитель Вспышки Пустоты I&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;fs=40&gt;Мех Нивин&lt;/fs&gt;</t>
@@ -8412,7 +8412,7 @@
     <t>&lt;f=Myriad Pro Light;50;1;0;0;0&gt;&lt;ls=75&gt;После того как игрок активировал систему, вы можете выбрать этот отряд в активной системе, чтобы он стал повреждённым. Затем разместите или переместите жетон раны в эту систему.&lt;/ls&gt;&lt;/f&gt;</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Хранитель Вспышки Пустоты II [СЖК]&lt;/fs&gt;</t>
+    <t>&lt;fs=44&gt;Хранитель Вспышки Пустоты II&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;fs=64&gt;Анна Регия&lt;/fs&gt;</t>
@@ -8541,7 +8541,7 @@
     <t>&lt;fs=40&gt;эсминец Синдиката&lt;/fs&gt;</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Блокадопрорыватель II [КК]&lt;/fs&gt;</t>
+    <t>&lt;fs=64&gt;Блокадопрорыватель II&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;f=Myriad Pro Light;50;1;0;0;0&gt;&lt;ls=75&gt;Этот корабль может передвигаться через системы, в которых есть корабли других игроков.&lt;/ls&gt;&lt;/f&gt;</t>
@@ -8628,7 +8628,7 @@
     <t>&lt;f=Myriad Pro Light;50;1;0;0;0&gt;&lt;ls=75&gt;Этот отряд нельзя уничтожить картой действия «Прямое попадание».&lt;/ls&gt;&lt;/f&gt;</t>
   </si>
   <si>
-    <t>&lt;fs=64&gt;Штормовой Призыватель Авроры&lt;/fs&gt;</t>
+    <t>&lt;fs=44&gt;Штормовой Призыватель Авроры&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;fs=40&gt;Мех Велдир&lt;/fs&gt;</t>
@@ -25970,7 +25970,7 @@
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C1" sqref="C1:C169"/>
+      <selection pane="bottomLeft" activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -26002,7 +26002,7 @@
       <c r="C1" s="3" t="s">
         <v>433</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="3" t="s">
         <v>2266</v>
       </c>
       <c r="E1" s="2" t="s">
@@ -26091,7 +26091,7 @@
       <c r="C2" s="6" t="s">
         <v>2287</v>
       </c>
-      <c r="D2" s="5" t="s">
+      <c r="D2" s="6" t="s">
         <v>2288</v>
       </c>
       <c r="E2" s="5" t="s">
@@ -26154,7 +26154,7 @@
       <c r="C3" s="6" t="s">
         <v>2294</v>
       </c>
-      <c r="D3" s="5" t="s">
+      <c r="D3" s="6" t="s">
         <v>2288</v>
       </c>
       <c r="E3" s="5" t="s">
@@ -26221,7 +26221,7 @@
       <c r="C4" s="6" t="s">
         <v>2297</v>
       </c>
-      <c r="D4" s="5" t="s">
+      <c r="D4" s="6" t="s">
         <v>2298</v>
       </c>
       <c r="E4" s="5" t="s">
@@ -26284,7 +26284,7 @@
       <c r="C5" s="6" t="s">
         <v>2304</v>
       </c>
-      <c r="D5" s="5" t="s">
+      <c r="D5" s="6" t="s">
         <v>2298</v>
       </c>
       <c r="E5" s="5" t="s">
@@ -26349,7 +26349,7 @@
       <c r="C6" s="6" t="s">
         <v>2307</v>
       </c>
-      <c r="D6" s="5" t="s">
+      <c r="D6" s="6" t="s">
         <v>2308</v>
       </c>
       <c r="E6" s="5" t="s">
@@ -26414,7 +26414,7 @@
       <c r="C7" s="6" t="s">
         <v>2314</v>
       </c>
-      <c r="D7" s="5" t="s">
+      <c r="D7" s="6" t="s">
         <v>2315</v>
       </c>
       <c r="E7" s="5" t="s">
@@ -26479,7 +26479,7 @@
       <c r="C8" s="6" t="s">
         <v>2322</v>
       </c>
-      <c r="D8" s="5" t="s">
+      <c r="D8" s="6" t="s">
         <v>2323</v>
       </c>
       <c r="E8" s="5" t="s">
@@ -26542,7 +26542,7 @@
       <c r="C9" s="6" t="s">
         <v>2330</v>
       </c>
-      <c r="D9" s="5" t="s">
+      <c r="D9" s="6" t="s">
         <v>2331</v>
       </c>
       <c r="E9" s="5" t="s">
@@ -26607,7 +26607,7 @@
       <c r="C10" s="6" t="s">
         <v>2337</v>
       </c>
-      <c r="D10" s="5" t="s">
+      <c r="D10" s="6" t="s">
         <v>2338</v>
       </c>
       <c r="E10" s="5" t="s">
@@ -26674,7 +26674,7 @@
       <c r="C11" s="6" t="s">
         <v>2343</v>
       </c>
-      <c r="D11" s="5" t="s">
+      <c r="D11" s="6" t="s">
         <v>2338</v>
       </c>
       <c r="E11" s="5" t="s">
@@ -26739,7 +26739,7 @@
       <c r="C12" s="6" t="s">
         <v>2346</v>
       </c>
-      <c r="D12" s="5" t="s">
+      <c r="D12" s="6" t="s">
         <v>2347</v>
       </c>
       <c r="E12" s="5" t="s">
@@ -26804,7 +26804,7 @@
       <c r="C13" s="6" t="s">
         <v>2353</v>
       </c>
-      <c r="D13" s="5" t="s">
+      <c r="D13" s="6" t="s">
         <v>2354</v>
       </c>
       <c r="E13" s="5" t="s">
@@ -26867,7 +26867,7 @@
       <c r="C14" s="6" t="s">
         <v>2359</v>
       </c>
-      <c r="D14" s="5" t="s">
+      <c r="D14" s="6" t="s">
         <v>2354</v>
       </c>
       <c r="E14" s="5" t="s">
@@ -26932,7 +26932,7 @@
       <c r="C15" s="6" t="s">
         <v>2362</v>
       </c>
-      <c r="D15" s="5" t="s">
+      <c r="D15" s="6" t="s">
         <v>2363</v>
       </c>
       <c r="E15" s="5" t="s">
@@ -26999,7 +26999,7 @@
       <c r="C16" s="6" t="s">
         <v>2370</v>
       </c>
-      <c r="D16" s="5" t="s">
+      <c r="D16" s="6" t="s">
         <v>2371</v>
       </c>
       <c r="E16" s="5" t="s">
@@ -27062,7 +27062,7 @@
       <c r="C17" s="6" t="s">
         <v>2374</v>
       </c>
-      <c r="D17" s="5" t="s">
+      <c r="D17" s="6" t="s">
         <v>2371</v>
       </c>
       <c r="E17" s="5" t="s">
@@ -27125,7 +27125,7 @@
       <c r="C18" s="6" t="s">
         <v>2377</v>
       </c>
-      <c r="D18" s="5" t="s">
+      <c r="D18" s="6" t="s">
         <v>2378</v>
       </c>
       <c r="E18" s="5" t="s">
@@ -27192,7 +27192,7 @@
       <c r="C19" s="6" t="s">
         <v>2383</v>
       </c>
-      <c r="D19" s="5" t="s">
+      <c r="D19" s="6" t="s">
         <v>2384</v>
       </c>
       <c r="E19" s="5" t="s">
@@ -27259,7 +27259,7 @@
       <c r="C20" s="6" t="s">
         <v>2389</v>
       </c>
-      <c r="D20" s="5" t="s">
+      <c r="D20" s="6" t="s">
         <v>2384</v>
       </c>
       <c r="E20" s="5" t="s">
@@ -27324,7 +27324,7 @@
       <c r="C21" s="6" t="s">
         <v>2392</v>
       </c>
-      <c r="D21" s="5" t="s">
+      <c r="D21" s="6" t="s">
         <v>2393</v>
       </c>
       <c r="E21" s="5" t="s">
@@ -27387,7 +27387,7 @@
       <c r="C22" s="6" t="s">
         <v>2397</v>
       </c>
-      <c r="D22" s="5" t="s">
+      <c r="D22" s="6" t="s">
         <v>2398</v>
       </c>
       <c r="E22" s="5" t="s">
@@ -27452,7 +27452,7 @@
       <c r="C23" s="6" t="s">
         <v>2404</v>
       </c>
-      <c r="D23" s="5" t="s">
+      <c r="D23" s="6" t="s">
         <v>2398</v>
       </c>
       <c r="E23" s="5" t="s">
@@ -27515,7 +27515,7 @@
       <c r="C24" s="6" t="s">
         <v>2407</v>
       </c>
-      <c r="D24" s="5" t="s">
+      <c r="D24" s="6" t="s">
         <v>2408</v>
       </c>
       <c r="E24" s="5" t="s">
@@ -27580,7 +27580,7 @@
       <c r="C25" s="6" t="s">
         <v>2413</v>
       </c>
-      <c r="D25" s="5" t="s">
+      <c r="D25" s="6" t="s">
         <v>2408</v>
       </c>
       <c r="E25" s="5" t="s">
@@ -27647,7 +27647,7 @@
       <c r="C26" s="6" t="s">
         <v>2416</v>
       </c>
-      <c r="D26" s="5" t="s">
+      <c r="D26" s="6" t="s">
         <v>2417</v>
       </c>
       <c r="E26" s="5" t="s">
@@ -27712,7 +27712,7 @@
       <c r="C27" s="6" t="s">
         <v>2422</v>
       </c>
-      <c r="D27" s="5" t="s">
+      <c r="D27" s="6" t="s">
         <v>2417</v>
       </c>
       <c r="E27" s="5" t="s">
@@ -27777,7 +27777,7 @@
       <c r="C28" s="6" t="s">
         <v>2425</v>
       </c>
-      <c r="D28" s="5" t="s">
+      <c r="D28" s="6" t="s">
         <v>2426</v>
       </c>
       <c r="E28" s="5" t="s">
@@ -27842,7 +27842,7 @@
       <c r="C29" s="6" t="s">
         <v>2432</v>
       </c>
-      <c r="D29" s="5" t="s">
+      <c r="D29" s="6" t="s">
         <v>2426</v>
       </c>
       <c r="E29" s="5" t="s">
@@ -27905,7 +27905,7 @@
       <c r="C30" s="6" t="s">
         <v>2435</v>
       </c>
-      <c r="D30" s="5" t="s">
+      <c r="D30" s="6" t="s">
         <v>2436</v>
       </c>
       <c r="E30" s="5" t="s">
@@ -27970,7 +27970,7 @@
       <c r="C31" s="6" t="s">
         <v>2441</v>
       </c>
-      <c r="D31" s="5" t="s">
+      <c r="D31" s="6" t="s">
         <v>2436</v>
       </c>
       <c r="E31" s="5" t="s">
@@ -28035,7 +28035,7 @@
       <c r="C32" s="6" t="s">
         <v>2444</v>
       </c>
-      <c r="D32" s="5" t="s">
+      <c r="D32" s="6" t="s">
         <v>2445</v>
       </c>
       <c r="E32" s="5" t="s">
@@ -28100,7 +28100,7 @@
       <c r="C33" s="6" t="s">
         <v>2451</v>
       </c>
-      <c r="D33" s="5" t="s">
+      <c r="D33" s="6" t="s">
         <v>2452</v>
       </c>
       <c r="E33" s="5" t="s">
@@ -28165,7 +28165,7 @@
       <c r="C34" s="6" t="s">
         <v>2458</v>
       </c>
-      <c r="D34" s="5" t="s">
+      <c r="D34" s="6" t="s">
         <v>2459</v>
       </c>
       <c r="E34" s="5" t="s">
@@ -28230,7 +28230,7 @@
       <c r="C35" s="6" t="s">
         <v>2463</v>
       </c>
-      <c r="D35" s="5" t="s">
+      <c r="D35" s="6" t="s">
         <v>2464</v>
       </c>
       <c r="E35" s="5" t="s">
@@ -28295,7 +28295,7 @@
       <c r="C36" s="6" t="s">
         <v>2470</v>
       </c>
-      <c r="D36" s="5" t="s">
+      <c r="D36" s="6" t="s">
         <v>2464</v>
       </c>
       <c r="E36" s="5" t="s">
@@ -28360,7 +28360,7 @@
       <c r="C37" s="6" t="s">
         <v>2473</v>
       </c>
-      <c r="D37" s="5" t="s">
+      <c r="D37" s="6" t="s">
         <v>2474</v>
       </c>
       <c r="E37" s="5" t="s">
@@ -28425,7 +28425,7 @@
       <c r="C38" s="6" t="s">
         <v>2481</v>
       </c>
-      <c r="D38" s="5" t="s">
+      <c r="D38" s="6" t="s">
         <v>2482</v>
       </c>
       <c r="E38" s="5" t="s">
@@ -28488,7 +28488,7 @@
       <c r="C39" s="6" t="s">
         <v>2488</v>
       </c>
-      <c r="D39" s="5" t="s">
+      <c r="D39" s="6" t="s">
         <v>2489</v>
       </c>
       <c r="E39" s="5" t="s">
@@ -28553,7 +28553,7 @@
       <c r="C40" s="6" t="s">
         <v>2494</v>
       </c>
-      <c r="D40" s="5" t="s">
+      <c r="D40" s="6" t="s">
         <v>2495</v>
       </c>
       <c r="E40" s="5" t="s">
@@ -28616,7 +28616,7 @@
       <c r="C41" s="6" t="s">
         <v>2499</v>
       </c>
-      <c r="D41" s="5" t="s">
+      <c r="D41" s="6" t="s">
         <v>2495</v>
       </c>
       <c r="E41" s="5" t="s">
@@ -28679,7 +28679,7 @@
       <c r="C42" s="6" t="s">
         <v>2502</v>
       </c>
-      <c r="D42" s="5" t="s">
+      <c r="D42" s="6" t="s">
         <v>2503</v>
       </c>
       <c r="E42" s="5" t="s">
@@ -28746,7 +28746,7 @@
       <c r="C43" s="6" t="s">
         <v>2508</v>
       </c>
-      <c r="D43" s="5" t="s">
+      <c r="D43" s="6" t="s">
         <v>2503</v>
       </c>
       <c r="E43" s="5" t="s">
@@ -28811,7 +28811,7 @@
       <c r="C44" s="6" t="s">
         <v>2511</v>
       </c>
-      <c r="D44" s="5" t="s">
+      <c r="D44" s="6" t="s">
         <v>2512</v>
       </c>
       <c r="E44" s="5" t="s">
@@ -28876,7 +28876,7 @@
       <c r="C45" s="6" t="s">
         <v>2517</v>
       </c>
-      <c r="D45" s="5" t="s">
+      <c r="D45" s="6" t="s">
         <v>2518</v>
       </c>
       <c r="E45" s="5" t="s">
@@ -28939,7 +28939,7 @@
       <c r="C46" s="6" t="s">
         <v>2524</v>
       </c>
-      <c r="D46" s="5" t="s">
+      <c r="D46" s="6" t="s">
         <v>2525</v>
       </c>
       <c r="E46" s="5" t="s">
@@ -29002,7 +29002,7 @@
       <c r="C47" s="6" t="s">
         <v>2530</v>
       </c>
-      <c r="D47" s="5" t="s">
+      <c r="D47" s="6" t="s">
         <v>2525</v>
       </c>
       <c r="E47" s="5" t="s">
@@ -29067,7 +29067,7 @@
       <c r="C48" s="6" t="s">
         <v>2533</v>
       </c>
-      <c r="D48" s="5" t="s">
+      <c r="D48" s="6" t="s">
         <v>2534</v>
       </c>
       <c r="E48" s="5" t="s">
@@ -29130,7 +29130,7 @@
       <c r="C49" s="6" t="s">
         <v>2539</v>
       </c>
-      <c r="D49" s="5" t="s">
+      <c r="D49" s="6" t="s">
         <v>2540</v>
       </c>
       <c r="E49" s="5" t="s">
@@ -29195,7 +29195,7 @@
       <c r="C50" s="6" t="s">
         <v>2547</v>
       </c>
-      <c r="D50" s="5" t="s">
+      <c r="D50" s="6" t="s">
         <v>2548</v>
       </c>
       <c r="E50" s="5" t="s">
@@ -29258,7 +29258,7 @@
       <c r="C51" s="6" t="s">
         <v>2554</v>
       </c>
-      <c r="D51" s="5" t="s">
+      <c r="D51" s="6" t="s">
         <v>2555</v>
       </c>
       <c r="E51" s="5" t="s">
@@ -29331,7 +29331,7 @@
       <c r="C52" s="6" t="s">
         <v>2557</v>
       </c>
-      <c r="D52" s="5" t="s">
+      <c r="D52" s="6" t="s">
         <v>2558</v>
       </c>
       <c r="E52" s="5" t="s">
@@ -29400,7 +29400,7 @@
       <c r="C53" s="6" t="s">
         <v>2560</v>
       </c>
-      <c r="D53" s="5" t="s">
+      <c r="D53" s="6" t="s">
         <v>2561</v>
       </c>
       <c r="E53" s="5" t="s">
@@ -29473,7 +29473,7 @@
       <c r="C54" s="6" t="s">
         <v>2563</v>
       </c>
-      <c r="D54" s="5" t="s">
+      <c r="D54" s="6" t="s">
         <v>2564</v>
       </c>
       <c r="E54" s="5" t="s">
@@ -29542,7 +29542,7 @@
       <c r="C55" s="6" t="s">
         <v>2566</v>
       </c>
-      <c r="D55" s="5" t="s">
+      <c r="D55" s="6" t="s">
         <v>2567</v>
       </c>
       <c r="E55" s="5" t="s">
@@ -29615,7 +29615,7 @@
       <c r="C56" s="6" t="s">
         <v>2569</v>
       </c>
-      <c r="D56" s="5" t="s">
+      <c r="D56" s="6" t="s">
         <v>2570</v>
       </c>
       <c r="E56" s="5" t="s">
@@ -29676,7 +29676,7 @@
       <c r="C57" s="6" t="s">
         <v>2573</v>
       </c>
-      <c r="D57" s="5" t="s">
+      <c r="D57" s="6" t="s">
         <v>2570</v>
       </c>
       <c r="E57" s="5" t="s">
@@ -29741,7 +29741,7 @@
       <c r="C58" s="6" t="s">
         <v>2575</v>
       </c>
-      <c r="D58" s="5" t="s">
+      <c r="D58" s="6" t="s">
         <v>2576</v>
       </c>
       <c r="E58" s="5" t="s">
@@ -29810,7 +29810,7 @@
       <c r="C59" s="6" t="s">
         <v>2578</v>
       </c>
-      <c r="D59" s="5" t="s">
+      <c r="D59" s="6" t="s">
         <v>2579</v>
       </c>
       <c r="E59" s="5" t="s">
@@ -29883,7 +29883,7 @@
       <c r="C60" s="6" t="s">
         <v>2581</v>
       </c>
-      <c r="D60" s="5" t="s">
+      <c r="D60" s="6" t="s">
         <v>2582</v>
       </c>
       <c r="E60" s="5" t="s">
@@ -29956,7 +29956,7 @@
       <c r="C61" s="6" t="s">
         <v>2584</v>
       </c>
-      <c r="D61" s="5" t="s">
+      <c r="D61" s="6" t="s">
         <v>2582</v>
       </c>
       <c r="E61" s="5" t="s">
@@ -30035,7 +30035,7 @@
       <c r="C62" s="6" t="s">
         <v>2586</v>
       </c>
-      <c r="D62" s="5" t="s">
+      <c r="D62" s="6" t="s">
         <v>2587</v>
       </c>
       <c r="E62" s="5" t="s">
@@ -30104,7 +30104,7 @@
       <c r="C63" s="6" t="s">
         <v>2589</v>
       </c>
-      <c r="D63" s="5" t="s">
+      <c r="D63" s="6" t="s">
         <v>2590</v>
       </c>
       <c r="E63" s="5" t="s">
@@ -30177,7 +30177,7 @@
       <c r="C64" s="6" t="s">
         <v>2586</v>
       </c>
-      <c r="D64" s="5" t="s">
+      <c r="D64" s="6" t="s">
         <v>2587</v>
       </c>
       <c r="E64" s="5" t="s">
@@ -30246,7 +30246,7 @@
       <c r="C65" s="6" t="s">
         <v>2592</v>
       </c>
-      <c r="D65" s="5" t="s">
+      <c r="D65" s="6" t="s">
         <v>2593</v>
       </c>
       <c r="E65" s="5"/>
@@ -30313,7 +30313,7 @@
       <c r="C66" s="6" t="s">
         <v>2594</v>
       </c>
-      <c r="D66" s="5" t="s">
+      <c r="D66" s="6" t="s">
         <v>2593</v>
       </c>
       <c r="E66" s="5" t="s">
@@ -30386,7 +30386,7 @@
       <c r="C67" s="6" t="s">
         <v>2596</v>
       </c>
-      <c r="D67" s="5" t="s">
+      <c r="D67" s="6" t="s">
         <v>2597</v>
       </c>
       <c r="E67" s="5" t="s">
@@ -30459,7 +30459,7 @@
       <c r="C68" s="6" t="s">
         <v>2599</v>
       </c>
-      <c r="D68" s="5" t="s">
+      <c r="D68" s="6" t="s">
         <v>2600</v>
       </c>
       <c r="E68" s="5" t="s">
@@ -30532,7 +30532,7 @@
       <c r="C69" s="6" t="s">
         <v>2602</v>
       </c>
-      <c r="D69" s="5" t="s">
+      <c r="D69" s="6" t="s">
         <v>2600</v>
       </c>
       <c r="E69" s="5" t="s">
@@ -30611,7 +30611,7 @@
       <c r="C70" s="6" t="s">
         <v>2603</v>
       </c>
-      <c r="D70" s="5" t="s">
+      <c r="D70" s="6" t="s">
         <v>2604</v>
       </c>
       <c r="E70" s="5" t="s">
@@ -30680,7 +30680,7 @@
       <c r="C71" s="6" t="s">
         <v>2606</v>
       </c>
-      <c r="D71" s="5" t="s">
+      <c r="D71" s="6" t="s">
         <v>2607</v>
       </c>
       <c r="E71" s="5" t="s">
@@ -30753,7 +30753,7 @@
       <c r="C72" s="6" t="s">
         <v>2609</v>
       </c>
-      <c r="D72" s="5" t="s">
+      <c r="D72" s="6" t="s">
         <v>2610</v>
       </c>
       <c r="E72" s="5" t="s">
@@ -30822,7 +30822,7 @@
       <c r="C73" s="6" t="s">
         <v>2612</v>
       </c>
-      <c r="D73" s="5" t="s">
+      <c r="D73" s="6" t="s">
         <v>2613</v>
       </c>
       <c r="E73" s="5" t="s">
@@ -30895,7 +30895,7 @@
       <c r="C74" s="6" t="s">
         <v>2615</v>
       </c>
-      <c r="D74" s="5" t="s">
+      <c r="D74" s="6" t="s">
         <v>2616</v>
       </c>
       <c r="E74" s="5" t="s">
@@ -30966,7 +30966,7 @@
       <c r="C75" s="6" t="s">
         <v>2618</v>
       </c>
-      <c r="D75" s="5" t="s">
+      <c r="D75" s="6" t="s">
         <v>2616</v>
       </c>
       <c r="E75" s="5" t="s">
@@ -31041,7 +31041,7 @@
       <c r="C76" s="6" t="s">
         <v>2619</v>
       </c>
-      <c r="D76" s="5" t="s">
+      <c r="D76" s="6" t="s">
         <v>2620</v>
       </c>
       <c r="E76" s="5" t="s">
@@ -31110,7 +31110,7 @@
       <c r="C77" s="6" t="s">
         <v>2622</v>
       </c>
-      <c r="D77" s="5" t="s">
+      <c r="D77" s="6" t="s">
         <v>2623</v>
       </c>
       <c r="E77" s="5" t="s">
@@ -31183,7 +31183,7 @@
       <c r="C78" s="6" t="s">
         <v>2625</v>
       </c>
-      <c r="D78" s="5" t="s">
+      <c r="D78" s="6" t="s">
         <v>2626</v>
       </c>
       <c r="E78" s="5" t="s">
@@ -31252,7 +31252,7 @@
       <c r="C79" s="6" t="s">
         <v>2628</v>
       </c>
-      <c r="D79" s="5" t="s">
+      <c r="D79" s="6" t="s">
         <v>2629</v>
       </c>
       <c r="E79" s="5" t="s">
@@ -31325,7 +31325,7 @@
       <c r="C80" s="6" t="s">
         <v>2631</v>
       </c>
-      <c r="D80" s="5" t="s">
+      <c r="D80" s="6" t="s">
         <v>2629</v>
       </c>
       <c r="E80" s="5" t="s">
@@ -31398,7 +31398,7 @@
       <c r="C81" s="6" t="s">
         <v>2633</v>
       </c>
-      <c r="D81" s="5" t="s">
+      <c r="D81" s="6" t="s">
         <v>2634</v>
       </c>
       <c r="E81" s="5"/>
@@ -31469,7 +31469,7 @@
       <c r="C82" s="6" t="s">
         <v>2635</v>
       </c>
-      <c r="D82" s="5" t="s">
+      <c r="D82" s="6" t="s">
         <v>2634</v>
       </c>
       <c r="E82" s="5" t="s">
@@ -31546,7 +31546,7 @@
       <c r="C83" s="6" t="s">
         <v>2637</v>
       </c>
-      <c r="D83" s="5" t="s">
+      <c r="D83" s="6" t="s">
         <v>2638</v>
       </c>
       <c r="E83" s="5" t="s">
@@ -31615,7 +31615,7 @@
       <c r="C84" s="6" t="s">
         <v>2640</v>
       </c>
-      <c r="D84" s="5" t="s">
+      <c r="D84" s="6" t="s">
         <v>2641</v>
       </c>
       <c r="E84" s="5" t="s">
@@ -31688,7 +31688,7 @@
       <c r="C85" s="6" t="s">
         <v>2643</v>
       </c>
-      <c r="D85" s="5" t="s">
+      <c r="D85" s="6" t="s">
         <v>2644</v>
       </c>
       <c r="E85" s="5" t="s">
@@ -31757,7 +31757,7 @@
       <c r="C86" s="6" t="s">
         <v>2646</v>
       </c>
-      <c r="D86" s="5" t="s">
+      <c r="D86" s="6" t="s">
         <v>2647</v>
       </c>
       <c r="E86" s="5" t="s">
@@ -31830,7 +31830,7 @@
       <c r="C87" s="6" t="s">
         <v>2649</v>
       </c>
-      <c r="D87" s="5" t="s">
+      <c r="D87" s="6" t="s">
         <v>2650</v>
       </c>
       <c r="E87" s="5" t="s">
@@ -31891,7 +31891,7 @@
       <c r="C88" s="6" t="s">
         <v>2652</v>
       </c>
-      <c r="D88" s="5" t="s">
+      <c r="D88" s="6" t="s">
         <v>2650</v>
       </c>
       <c r="E88" s="5" t="s">
@@ -31956,7 +31956,7 @@
       <c r="C89" s="6" t="s">
         <v>2654</v>
       </c>
-      <c r="D89" s="5" t="s">
+      <c r="D89" s="6" t="s">
         <v>2655</v>
       </c>
       <c r="E89" s="5" t="s">
@@ -32025,7 +32025,7 @@
       <c r="C90" s="6" t="s">
         <v>2657</v>
       </c>
-      <c r="D90" s="5" t="s">
+      <c r="D90" s="6" t="s">
         <v>2658</v>
       </c>
       <c r="E90" s="5" t="s">
@@ -32098,7 +32098,7 @@
       <c r="C91" s="6" t="s">
         <v>2660</v>
       </c>
-      <c r="D91" s="5" t="s">
+      <c r="D91" s="6" t="s">
         <v>2661</v>
       </c>
       <c r="E91" s="5" t="s">
@@ -32167,7 +32167,7 @@
       <c r="C92" s="6" t="s">
         <v>2663</v>
       </c>
-      <c r="D92" s="5" t="s">
+      <c r="D92" s="6" t="s">
         <v>2664</v>
       </c>
       <c r="E92" s="5" t="s">
@@ -32240,7 +32240,7 @@
       <c r="C93" s="6" t="s">
         <v>2666</v>
       </c>
-      <c r="D93" s="5" t="s">
+      <c r="D93" s="6" t="s">
         <v>2667</v>
       </c>
       <c r="E93" s="5" t="s">
@@ -32313,7 +32313,7 @@
       <c r="C94" s="6" t="s">
         <v>2669</v>
       </c>
-      <c r="D94" s="5" t="s">
+      <c r="D94" s="6" t="s">
         <v>2667</v>
       </c>
       <c r="E94" s="5" t="s">
@@ -32390,7 +32390,7 @@
       <c r="C95" s="6" t="s">
         <v>2671</v>
       </c>
-      <c r="D95" s="5" t="s">
+      <c r="D95" s="6" t="s">
         <v>2672</v>
       </c>
       <c r="E95" s="5" t="s">
@@ -32459,7 +32459,7 @@
       <c r="C96" s="6" t="s">
         <v>2674</v>
       </c>
-      <c r="D96" s="5" t="s">
+      <c r="D96" s="6" t="s">
         <v>2675</v>
       </c>
       <c r="E96" s="5" t="s">
@@ -32532,7 +32532,7 @@
       <c r="C97" s="6" t="s">
         <v>2677</v>
       </c>
-      <c r="D97" s="5" t="s">
+      <c r="D97" s="6" t="s">
         <v>2678</v>
       </c>
       <c r="E97" s="5" t="s">
@@ -32601,7 +32601,7 @@
       <c r="C98" s="6" t="s">
         <v>2680</v>
       </c>
-      <c r="D98" s="5" t="s">
+      <c r="D98" s="6" t="s">
         <v>2681</v>
       </c>
       <c r="E98" s="5" t="s">
@@ -32674,7 +32674,7 @@
       <c r="C99" s="6" t="s">
         <v>2683</v>
       </c>
-      <c r="D99" s="5" t="s">
+      <c r="D99" s="6" t="s">
         <v>2684</v>
       </c>
       <c r="E99" s="5" t="s">
@@ -32743,7 +32743,7 @@
       <c r="C100" s="6" t="s">
         <v>2686</v>
       </c>
-      <c r="D100" s="5" t="s">
+      <c r="D100" s="6" t="s">
         <v>2687</v>
       </c>
       <c r="E100" s="5" t="s">
@@ -32816,7 +32816,7 @@
       <c r="C101" s="6" t="s">
         <v>2689</v>
       </c>
-      <c r="D101" s="5" t="s">
+      <c r="D101" s="6" t="s">
         <v>2690</v>
       </c>
       <c r="E101" s="5" t="s">
@@ -32885,7 +32885,7 @@
       <c r="C102" s="6" t="s">
         <v>2692</v>
       </c>
-      <c r="D102" s="5" t="s">
+      <c r="D102" s="6" t="s">
         <v>2693</v>
       </c>
       <c r="E102" s="5" t="s">
@@ -32958,7 +32958,7 @@
       <c r="C103" s="6" t="s">
         <v>2695</v>
       </c>
-      <c r="D103" s="5" t="s">
+      <c r="D103" s="6" t="s">
         <v>2696</v>
       </c>
       <c r="E103" s="5" t="s">
@@ -33027,7 +33027,7 @@
       <c r="C104" s="6" t="s">
         <v>2698</v>
       </c>
-      <c r="D104" s="5" t="s">
+      <c r="D104" s="6" t="s">
         <v>2699</v>
       </c>
       <c r="E104" s="5" t="s">
@@ -33100,7 +33100,7 @@
       <c r="C105" s="6" t="s">
         <v>2701</v>
       </c>
-      <c r="D105" s="5" t="s">
+      <c r="D105" s="6" t="s">
         <v>2702</v>
       </c>
       <c r="E105" s="5" t="s">
@@ -33169,7 +33169,7 @@
       <c r="C106" s="6" t="s">
         <v>2704</v>
       </c>
-      <c r="D106" s="5" t="s">
+      <c r="D106" s="6" t="s">
         <v>2705</v>
       </c>
       <c r="E106" s="5" t="s">
@@ -33242,7 +33242,7 @@
       <c r="C107" s="6" t="s">
         <v>2707</v>
       </c>
-      <c r="D107" s="5" t="s">
+      <c r="D107" s="6" t="s">
         <v>2708</v>
       </c>
       <c r="E107" s="5"/>
@@ -33309,7 +33309,7 @@
       <c r="C108" s="6" t="s">
         <v>2709</v>
       </c>
-      <c r="D108" s="5" t="s">
+      <c r="D108" s="6" t="s">
         <v>2708</v>
       </c>
       <c r="E108" s="5" t="s">
@@ -33384,7 +33384,7 @@
       <c r="C109" s="6" t="s">
         <v>2710</v>
       </c>
-      <c r="D109" s="5" t="s">
+      <c r="D109" s="6" t="s">
         <v>2711</v>
       </c>
       <c r="E109" s="5" t="s">
@@ -33453,7 +33453,7 @@
       <c r="C110" s="6" t="s">
         <v>2713</v>
       </c>
-      <c r="D110" s="5" t="s">
+      <c r="D110" s="6" t="s">
         <v>2714</v>
       </c>
       <c r="E110" s="5" t="s">
@@ -33526,7 +33526,7 @@
       <c r="C111" s="6" t="s">
         <v>2716</v>
       </c>
-      <c r="D111" s="5" t="s">
+      <c r="D111" s="6" t="s">
         <v>2717</v>
       </c>
       <c r="E111" s="5"/>
@@ -33597,7 +33597,7 @@
       <c r="C112" s="6" t="s">
         <v>2718</v>
       </c>
-      <c r="D112" s="5" t="s">
+      <c r="D112" s="6" t="s">
         <v>2717</v>
       </c>
       <c r="E112" s="5"/>
@@ -33674,7 +33674,7 @@
       <c r="C113" s="6" t="s">
         <v>2719</v>
       </c>
-      <c r="D113" s="5" t="s">
+      <c r="D113" s="6" t="s">
         <v>2720</v>
       </c>
       <c r="E113" s="5" t="s">
@@ -33743,7 +33743,7 @@
       <c r="C114" s="6" t="s">
         <v>2722</v>
       </c>
-      <c r="D114" s="5" t="s">
+      <c r="D114" s="6" t="s">
         <v>2723</v>
       </c>
       <c r="E114" s="5" t="s">
@@ -33816,7 +33816,7 @@
       <c r="C115" s="6" t="s">
         <v>2725</v>
       </c>
-      <c r="D115" s="5" t="s">
+      <c r="D115" s="6" t="s">
         <v>2726</v>
       </c>
       <c r="E115" s="5" t="s">
@@ -33879,7 +33879,7 @@
       <c r="C116" s="6" t="s">
         <v>2728</v>
       </c>
-      <c r="D116" s="5" t="s">
+      <c r="D116" s="6" t="s">
         <v>2726</v>
       </c>
       <c r="E116" s="5" t="s">
@@ -33948,7 +33948,7 @@
       <c r="C117" s="6" t="s">
         <v>2729</v>
       </c>
-      <c r="D117" s="5" t="s">
+      <c r="D117" s="6" t="s">
         <v>2730</v>
       </c>
       <c r="E117" s="5" t="s">
@@ -34017,7 +34017,7 @@
       <c r="C118" s="6" t="s">
         <v>2732</v>
       </c>
-      <c r="D118" s="5" t="s">
+      <c r="D118" s="6" t="s">
         <v>2733</v>
       </c>
       <c r="E118" s="5" t="s">
@@ -34090,7 +34090,7 @@
       <c r="C119" s="6" t="s">
         <v>2735</v>
       </c>
-      <c r="D119" s="5" t="s">
+      <c r="D119" s="6" t="s">
         <v>2736</v>
       </c>
       <c r="E119" s="5" t="s">
@@ -34159,7 +34159,7 @@
       <c r="C120" s="6" t="s">
         <v>2738</v>
       </c>
-      <c r="D120" s="5" t="s">
+      <c r="D120" s="6" t="s">
         <v>2739</v>
       </c>
       <c r="E120" s="5" t="s">
@@ -34232,7 +34232,7 @@
       <c r="C121" s="6" t="s">
         <v>2741</v>
       </c>
-      <c r="D121" s="5" t="s">
+      <c r="D121" s="6" t="s">
         <v>2742</v>
       </c>
       <c r="E121" s="5" t="s">
@@ -34293,7 +34293,7 @@
       <c r="C122" s="6" t="s">
         <v>2744</v>
       </c>
-      <c r="D122" s="5" t="s">
+      <c r="D122" s="6" t="s">
         <v>2742</v>
       </c>
       <c r="E122" s="9" t="s">
@@ -34358,7 +34358,7 @@
       <c r="C123" s="6" t="s">
         <v>2746</v>
       </c>
-      <c r="D123" s="5" t="s">
+      <c r="D123" s="6" t="s">
         <v>2747</v>
       </c>
       <c r="E123" s="5" t="s">
@@ -34427,7 +34427,7 @@
       <c r="C124" s="6" t="s">
         <v>2749</v>
       </c>
-      <c r="D124" s="5" t="s">
+      <c r="D124" s="6" t="s">
         <v>2750</v>
       </c>
       <c r="E124" s="5" t="s">
@@ -34500,7 +34500,7 @@
       <c r="C125" s="6" t="s">
         <v>2752</v>
       </c>
-      <c r="D125" s="5" t="s">
+      <c r="D125" s="6" t="s">
         <v>2753</v>
       </c>
       <c r="E125" s="5" t="s">
@@ -34569,7 +34569,7 @@
       <c r="C126" s="6" t="s">
         <v>2755</v>
       </c>
-      <c r="D126" s="5" t="s">
+      <c r="D126" s="6" t="s">
         <v>2753</v>
       </c>
       <c r="E126" s="5" t="s">
@@ -34644,7 +34644,7 @@
       <c r="C127" s="6" t="s">
         <v>2756</v>
       </c>
-      <c r="D127" s="5" t="s">
+      <c r="D127" s="6" t="s">
         <v>2757</v>
       </c>
       <c r="E127" s="5" t="s">
@@ -34717,7 +34717,7 @@
       <c r="C128" s="6" t="s">
         <v>2759</v>
       </c>
-      <c r="D128" s="5" t="s">
+      <c r="D128" s="6" t="s">
         <v>2760</v>
       </c>
       <c r="E128" s="5" t="s">
@@ -34788,7 +34788,7 @@
       <c r="C129" s="6" t="s">
         <v>2762</v>
       </c>
-      <c r="D129" s="5" t="s">
+      <c r="D129" s="6" t="s">
         <v>2760</v>
       </c>
       <c r="E129" s="5" t="s">
@@ -34863,7 +34863,7 @@
       <c r="C130" s="6" t="s">
         <v>2764</v>
       </c>
-      <c r="D130" s="5" t="s">
+      <c r="D130" s="6" t="s">
         <v>2765</v>
       </c>
       <c r="E130" s="5" t="s">
@@ -34932,7 +34932,7 @@
       <c r="C131" s="6" t="s">
         <v>2767</v>
       </c>
-      <c r="D131" s="5" t="s">
+      <c r="D131" s="6" t="s">
         <v>2768</v>
       </c>
       <c r="E131" s="5" t="s">
@@ -35005,7 +35005,7 @@
       <c r="C132" s="6" t="s">
         <v>2770</v>
       </c>
-      <c r="D132" s="5" t="s">
+      <c r="D132" s="6" t="s">
         <v>2771</v>
       </c>
       <c r="E132" s="5" t="s">
@@ -35074,7 +35074,7 @@
       <c r="C133" s="6" t="s">
         <v>2773</v>
       </c>
-      <c r="D133" s="5" t="s">
+      <c r="D133" s="6" t="s">
         <v>2771</v>
       </c>
       <c r="E133" s="5" t="s">
@@ -35143,7 +35143,7 @@
       <c r="C134" s="6" t="s">
         <v>2775</v>
       </c>
-      <c r="D134" s="5" t="s">
+      <c r="D134" s="6" t="s">
         <v>2776</v>
       </c>
       <c r="E134" s="5" t="s">
@@ -35216,7 +35216,7 @@
       <c r="C135" s="6" t="s">
         <v>2778</v>
       </c>
-      <c r="D135" s="5" t="s">
+      <c r="D135" s="6" t="s">
         <v>2779</v>
       </c>
       <c r="E135" s="5" t="s">
@@ -35285,7 +35285,7 @@
       <c r="C136" s="6" t="s">
         <v>2781</v>
       </c>
-      <c r="D136" s="5" t="s">
+      <c r="D136" s="6" t="s">
         <v>2782</v>
       </c>
       <c r="E136" s="5" t="s">
@@ -35358,7 +35358,7 @@
       <c r="C137" s="6" t="s">
         <v>2784</v>
       </c>
-      <c r="D137" s="5" t="s">
+      <c r="D137" s="6" t="s">
         <v>2785</v>
       </c>
       <c r="E137" s="5" t="s">
@@ -35427,7 +35427,7 @@
       <c r="C138" s="6" t="s">
         <v>2788</v>
       </c>
-      <c r="D138" s="5" t="s">
+      <c r="D138" s="6" t="s">
         <v>2785</v>
       </c>
       <c r="E138" s="5" t="s">
@@ -35508,7 +35508,7 @@
       <c r="C139" s="6" t="s">
         <v>2790</v>
       </c>
-      <c r="D139" s="5" t="s">
+      <c r="D139" s="6" t="s">
         <v>2791</v>
       </c>
       <c r="E139" s="5" t="s">
@@ -35577,7 +35577,7 @@
       <c r="C140" s="6" t="s">
         <v>2793</v>
       </c>
-      <c r="D140" s="5" t="s">
+      <c r="D140" s="6" t="s">
         <v>2794</v>
       </c>
       <c r="E140" s="5" t="s">
@@ -35650,7 +35650,7 @@
       <c r="C141" s="6" t="s">
         <v>2796</v>
       </c>
-      <c r="D141" s="5" t="s">
+      <c r="D141" s="6" t="s">
         <v>2797</v>
       </c>
       <c r="E141" s="5"/>
@@ -35719,7 +35719,7 @@
       <c r="C142" s="6" t="s">
         <v>2798</v>
       </c>
-      <c r="D142" s="5" t="s">
+      <c r="D142" s="6" t="s">
         <v>2797</v>
       </c>
       <c r="E142" s="5" t="s">
@@ -35794,7 +35794,7 @@
       <c r="C143" s="6" t="s">
         <v>2800</v>
       </c>
-      <c r="D143" s="5" t="s">
+      <c r="D143" s="6" t="s">
         <v>2801</v>
       </c>
       <c r="E143" s="5" t="s">
@@ -35863,7 +35863,7 @@
       <c r="C144" s="6" t="s">
         <v>2803</v>
       </c>
-      <c r="D144" s="5" t="s">
+      <c r="D144" s="6" t="s">
         <v>2804</v>
       </c>
       <c r="E144" s="5" t="s">
@@ -35936,7 +35936,7 @@
       <c r="C145" s="6" t="s">
         <v>2806</v>
       </c>
-      <c r="D145" s="5" t="s">
+      <c r="D145" s="6" t="s">
         <v>2807</v>
       </c>
       <c r="E145" s="5" t="s">
@@ -36005,7 +36005,7 @@
       <c r="C146" s="6" t="s">
         <v>2809</v>
       </c>
-      <c r="D146" s="5" t="s">
+      <c r="D146" s="6" t="s">
         <v>2810</v>
       </c>
       <c r="E146" s="5" t="s">
@@ -36078,7 +36078,7 @@
       <c r="C147" s="6" t="s">
         <v>2812</v>
       </c>
-      <c r="D147" s="5" t="s">
+      <c r="D147" s="6" t="s">
         <v>2813</v>
       </c>
       <c r="E147" s="5" t="s">
@@ -36151,7 +36151,7 @@
       <c r="C148" s="6" t="s">
         <v>2815</v>
       </c>
-      <c r="D148" s="5" t="s">
+      <c r="D148" s="6" t="s">
         <v>2813</v>
       </c>
       <c r="E148" s="5" t="s">
@@ -36230,7 +36230,7 @@
       <c r="C149" s="6" t="s">
         <v>2817</v>
       </c>
-      <c r="D149" s="5" t="s">
+      <c r="D149" s="6" t="s">
         <v>2818</v>
       </c>
       <c r="E149" s="5" t="s">
@@ -36299,7 +36299,7 @@
       <c r="C150" s="6" t="s">
         <v>2820</v>
       </c>
-      <c r="D150" s="5" t="s">
+      <c r="D150" s="6" t="s">
         <v>2821</v>
       </c>
       <c r="E150" s="5" t="s">
@@ -36372,7 +36372,7 @@
       <c r="C151" s="6" t="s">
         <v>2823</v>
       </c>
-      <c r="D151" s="5" t="s">
+      <c r="D151" s="6" t="s">
         <v>2824</v>
       </c>
       <c r="E151" s="5"/>
@@ -36443,7 +36443,7 @@
       <c r="C152" s="6" t="s">
         <v>2825</v>
       </c>
-      <c r="D152" s="5" t="s">
+      <c r="D152" s="6" t="s">
         <v>2824</v>
       </c>
       <c r="E152" s="5" t="s">
@@ -36522,7 +36522,7 @@
       <c r="C153" s="6" t="s">
         <v>2827</v>
       </c>
-      <c r="D153" s="5" t="s">
+      <c r="D153" s="6" t="s">
         <v>2828</v>
       </c>
       <c r="E153" s="5" t="s">
@@ -36591,7 +36591,7 @@
       <c r="C154" s="6" t="s">
         <v>2830</v>
       </c>
-      <c r="D154" s="5" t="s">
+      <c r="D154" s="6" t="s">
         <v>2831</v>
       </c>
       <c r="E154" s="5" t="s">
@@ -36664,7 +36664,7 @@
       <c r="C155" s="6" t="s">
         <v>2833</v>
       </c>
-      <c r="D155" s="5" t="s">
+      <c r="D155" s="6" t="s">
         <v>2834</v>
       </c>
       <c r="E155" s="5" t="s">
@@ -36733,7 +36733,7 @@
       <c r="C156" s="6" t="s">
         <v>2836</v>
       </c>
-      <c r="D156" s="5" t="s">
+      <c r="D156" s="6" t="s">
         <v>2834</v>
       </c>
       <c r="E156" s="5" t="s">
@@ -36806,7 +36806,7 @@
       <c r="C157" s="6" t="s">
         <v>2838</v>
       </c>
-      <c r="D157" s="5" t="s">
+      <c r="D157" s="6" t="s">
         <v>2839</v>
       </c>
       <c r="E157" s="5" t="s">
@@ -36875,7 +36875,7 @@
       <c r="C158" s="6" t="s">
         <v>2842</v>
       </c>
-      <c r="D158" s="5" t="s">
+      <c r="D158" s="6" t="s">
         <v>2843</v>
       </c>
       <c r="E158" s="5" t="s">
@@ -36942,7 +36942,7 @@
       <c r="C159" s="6" t="s">
         <v>2847</v>
       </c>
-      <c r="D159" s="5" t="s">
+      <c r="D159" s="6" t="s">
         <v>2848</v>
       </c>
       <c r="E159" s="5" t="s">
@@ -37003,7 +37003,7 @@
       <c r="A160" s="5"/>
       <c r="B160" s="5"/>
       <c r="C160" s="6"/>
-      <c r="D160" s="5"/>
+      <c r="D160" s="6"/>
       <c r="E160" s="5"/>
       <c r="F160" s="5"/>
       <c r="G160" s="10"/>
@@ -37034,7 +37034,7 @@
       <c r="A161" s="5"/>
       <c r="B161" s="5"/>
       <c r="C161" s="6"/>
-      <c r="D161" s="5"/>
+      <c r="D161" s="6"/>
       <c r="E161" s="5"/>
       <c r="F161" s="5"/>
       <c r="G161" s="5"/>
@@ -37065,7 +37065,7 @@
       <c r="A162" s="5"/>
       <c r="B162" s="5"/>
       <c r="C162" s="6"/>
-      <c r="D162" s="5"/>
+      <c r="D162" s="6"/>
       <c r="E162" s="5"/>
       <c r="F162" s="5"/>
       <c r="G162" s="5"/>
@@ -37096,7 +37096,7 @@
       <c r="A163" s="5"/>
       <c r="B163" s="5"/>
       <c r="C163" s="6"/>
-      <c r="D163" s="5"/>
+      <c r="D163" s="6"/>
       <c r="E163" s="5"/>
       <c r="F163" s="5"/>
       <c r="G163" s="5"/>
@@ -37127,7 +37127,7 @@
       <c r="A164" s="5"/>
       <c r="B164" s="5"/>
       <c r="C164" s="6"/>
-      <c r="D164" s="5"/>
+      <c r="D164" s="6"/>
       <c r="E164" s="5"/>
       <c r="F164" s="5"/>
       <c r="G164" s="5"/>
@@ -37158,7 +37158,7 @@
       <c r="A165" s="5"/>
       <c r="B165" s="5"/>
       <c r="C165" s="6"/>
-      <c r="D165" s="5"/>
+      <c r="D165" s="6"/>
       <c r="E165" s="5"/>
       <c r="F165" s="5"/>
       <c r="G165" s="5"/>
@@ -37189,7 +37189,7 @@
       <c r="A166" s="5"/>
       <c r="B166" s="5"/>
       <c r="C166" s="6"/>
-      <c r="D166" s="5"/>
+      <c r="D166" s="6"/>
       <c r="E166" s="5"/>
       <c r="F166" s="5"/>
       <c r="G166" s="5"/>
@@ -37220,7 +37220,7 @@
       <c r="A167" s="5"/>
       <c r="B167" s="5"/>
       <c r="C167" s="6"/>
-      <c r="D167" s="5"/>
+      <c r="D167" s="6"/>
       <c r="E167" s="5"/>
       <c r="F167" s="5"/>
       <c r="G167" s="5"/>
@@ -37251,7 +37251,7 @@
       <c r="A168" s="5"/>
       <c r="B168" s="5"/>
       <c r="C168" s="6"/>
-      <c r="D168" s="5"/>
+      <c r="D168" s="6"/>
       <c r="E168" s="5"/>
       <c r="F168" s="5"/>
       <c r="G168" s="5"/>
@@ -37282,7 +37282,7 @@
       <c r="A169" s="5"/>
       <c r="B169" s="5"/>
       <c r="C169" s="6"/>
-      <c r="D169" s="5"/>
+      <c r="D169" s="6"/>
       <c r="E169" s="5"/>
       <c r="F169" s="5"/>
       <c r="G169" s="5"/>

</xml_diff>

<commit_message>
fixed some cards from feedback
</commit_message>
<xml_diff>
--- a/Template_Data.xlsx
+++ b/Template_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12885" tabRatio="796" activeTab="2"/>
+    <workbookView windowWidth="28800" windowHeight="12885" tabRatio="796" firstSheet="7" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Actions" sheetId="14" r:id="rId1"/>
@@ -3065,7 +3065,7 @@
     <t>&lt;fc=13DFF1&gt;&lt;fs=40&gt;Полемарх&lt;/fs&gt;&lt;/fc&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=75&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt;&lt;f=Myriad Pro;50;1;0;0;0&gt;ДЕЙСТВИЕ: &lt;/f&gt;разместите отряды из вашего снабжения в количестве, равном вашим начальным отрядам, в любой комбинации в космосе любых систем, в которых есть хотя бы 1 ваше сооружение и нет кораблей других игроков, или на подконтрольных вам планетах.&lt;/ls&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;&lt;ls=75&gt;Затем изгоните эту карту.&lt;/f&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=66&gt;&lt;f=Myriad Pro Light;44;1;0;0;0&gt;&lt;f=Myriad Pro;44;1;0;0;0&gt;ДЕЙСТВИЕ: &lt;/f&gt;разместите отряды из вашего снабжения в количестве, равном вашим начальным отрядам, в любой комбинации на любых подконтрольных вам планетах и/или в космосе любых систем, в которых есть хотя бы 1 ваше сооружение и нет кораблей других игроков.&lt;/ls&gt;&lt;ls=53&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;&lt;ls=66&gt;Затем изгоните эту карту.&lt;/f&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>&lt;f=Myriad Pro Light;40;1;0;1;0&gt;&lt;ls=62&gt;«Срок истёк, требования не выполнены. Теперь действовать будем мы». Эмиссар начал отве-&lt;br&gt;чать, но его прервали — по связи Полемарх услышал сигналы тре-&lt;br&gt;воги и панический голос, произно-&lt;br&gt;сящий: «Они — они повсюду!»&lt;/ls&gt;&lt;/f&gt;</t>
@@ -3368,7 +3368,7 @@
     <t>&lt;fc=1ABCB6&gt;&lt;fs=40&gt;Дружелюбный Дипломат&lt;/fs&gt;&lt;/fc&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=66&gt;&lt;f=Myriad Pro Light;44;1;0;0;0&gt;Эта карта обладает способ-&lt;br&gt;ностью карт способностей подконтрольных легендарных планет, даже если эти карты перевёрнуты.&lt;/ls&gt;&lt;ls=53&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;&lt;ls=66&gt;Вы можете позволить другому игроку использовать способность этой карты.&lt;/f&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=66&gt;&lt;f=Myriad Pro Light;44;1;0;0;0&gt;Эта карта обладает текстовой способностью каждой карты способностей подконтрольных легендарных планет, даже если эти карты перевёрнуты.&lt;/ls&gt;&lt;ls=53&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;&lt;ls=66&gt;Вы можете позволить другому игроку использовать способность этой карты.&lt;/f&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>&lt;f=Myriad Pro Light;44;1;0;1;0&gt;&lt;ls=68&gt;Известный в совете, Кордо имел репутацию переговорщика по совместным проектам по всей галактике.&lt;/ls&gt;&lt;/f&gt;</t>
@@ -6491,7 +6491,7 @@
     <t>&lt;fs=64&gt;ФРАКТАЛЬНЫЕ ВРАТА&lt;/fs&gt;</t>
   </si>
   <si>
-    <t>&lt;fs=42&gt;&lt;ls=67&gt;Вы можете перевернуть эту карту в конце вашего хода, чтобы убрать 1 из ваших кораблей с игрового поля и разместить этот отряд в смежной системе, в которой нет кораблей другого игрока.&lt;/ls&gt;&lt;/fs&gt;</t>
+    <t>&lt;fs=50&gt;&lt;ls=80&gt;Вы можете перевернуть эту карту в конце вашего хода, чтобы переместить 1 из ваших кораблей в смежную систему, в которой нет кораблей других игроков.&lt;/ls&gt;&lt;/fs&gt;</t>
   </si>
   <si>
     <t>&lt;fs=42&gt;&lt;ls=68&gt;Пропавшие рядом с этой плане-&lt;br&gt;той корабли обнаруживались по всей галактике. Этому феномену не было логичного объяснения.&lt;/ls&gt;&lt;/fs&gt;</t>
@@ -9606,7 +9606,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="32">
+  <cellXfs count="33">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -9636,15 +9636,18 @@
     <xf numFmtId="0" fontId="1" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -9996,55 +9999,55 @@
   <cols>
     <col min="1" max="1" width="9" style="1" customWidth="1"/>
     <col min="2" max="2" width="18" style="1" customWidth="1"/>
-    <col min="3" max="3" width="18" style="26" customWidth="1"/>
-    <col min="4" max="4" width="17.8571428571429" style="27" customWidth="1"/>
-    <col min="5" max="5" width="44.7142857142857" style="27" customWidth="1"/>
-    <col min="6" max="6" width="19.5714285714286" style="27" customWidth="1"/>
+    <col min="3" max="3" width="18" style="27" customWidth="1"/>
+    <col min="4" max="4" width="17.8571428571429" style="28" customWidth="1"/>
+    <col min="5" max="5" width="44.7142857142857" style="28" customWidth="1"/>
+    <col min="6" max="6" width="19.5714285714286" style="28" customWidth="1"/>
     <col min="7" max="10" width="9" style="1"/>
-    <col min="11" max="12" width="9" style="26"/>
+    <col min="11" max="12" width="9" style="27"/>
     <col min="13" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="28" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="28" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="29" t="s">
+      <c r="B1" s="29" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="29" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="28" t="s">
+      <c r="E1" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="30" t="s">
+      <c r="F1" s="31" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="28">
+      <c r="A2" s="29">
         <v>0</v>
       </c>
-      <c r="B2" s="28"/>
-      <c r="C2" s="28" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="28"/>
-      <c r="E2" s="28"/>
-      <c r="F2" s="30"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="31"/>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="28">
+      <c r="A3" s="29">
         <v>1</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="28" t="s">
+      <c r="C3" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D3" s="4" t="s">
@@ -10053,18 +10056,18 @@
       <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="31" t="s">
+      <c r="F3" s="32" t="s">
         <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="28">
+      <c r="A4" s="29">
         <v>1</v>
       </c>
       <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="28" t="s">
+      <c r="C4" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="4" t="s">
@@ -10073,18 +10076,18 @@
       <c r="E4" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="F4" s="31" t="s">
+      <c r="F4" s="32" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="28">
+      <c r="A5" s="29">
         <v>1</v>
       </c>
       <c r="B5" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="28" t="s">
+      <c r="C5" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D5" s="4" t="s">
@@ -10093,18 +10096,18 @@
       <c r="E5" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="F5" s="31" t="s">
+      <c r="F5" s="32" t="s">
         <v>17</v>
       </c>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="28">
+      <c r="A6" s="29">
         <v>1</v>
       </c>
       <c r="B6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D6" s="4" t="s">
@@ -10113,18 +10116,18 @@
       <c r="E6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="F6" s="31" t="s">
+      <c r="F6" s="32" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="28">
+      <c r="A7" s="29">
         <v>1</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="28" t="s">
+      <c r="C7" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="4" t="s">
@@ -10133,18 +10136,18 @@
       <c r="E7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="F7" s="31" t="s">
+      <c r="F7" s="32" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="28">
+      <c r="A8" s="29">
         <v>1</v>
       </c>
       <c r="B8" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D8" s="4" t="s">
@@ -10153,18 +10156,18 @@
       <c r="E8" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="F8" s="31" t="s">
+      <c r="F8" s="32" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="28">
+      <c r="A9" s="29">
         <v>1</v>
       </c>
       <c r="B9" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="28" t="s">
+      <c r="C9" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D9" s="4" t="s">
@@ -10173,18 +10176,18 @@
       <c r="E9" s="4" t="s">
         <v>28</v>
       </c>
-      <c r="F9" s="31" t="s">
+      <c r="F9" s="32" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:6">
-      <c r="A10" s="28">
+      <c r="A10" s="29">
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C10" s="28" t="s">
+      <c r="C10" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D10" s="4" t="s">
@@ -10193,18 +10196,18 @@
       <c r="E10" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="31" t="s">
+      <c r="F10" s="32" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="11" spans="1:6">
-      <c r="A11" s="28">
+      <c r="A11" s="29">
         <v>1</v>
       </c>
       <c r="B11" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C11" s="28" t="s">
+      <c r="C11" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D11" s="4" t="s">
@@ -10213,18 +10216,18 @@
       <c r="E11" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="F11" s="31" t="s">
+      <c r="F11" s="32" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="28">
+      <c r="A12" s="29">
         <v>1</v>
       </c>
       <c r="B12" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C12" s="28" t="s">
+      <c r="C12" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D12" s="4" t="s">
@@ -10233,18 +10236,18 @@
       <c r="E12" s="4" t="s">
         <v>37</v>
       </c>
-      <c r="F12" s="31" t="s">
+      <c r="F12" s="32" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="28">
+      <c r="A13" s="29">
         <v>1</v>
       </c>
       <c r="B13" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="28" t="s">
+      <c r="C13" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D13" s="4" t="s">
@@ -10253,18 +10256,18 @@
       <c r="E13" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="F13" s="31" t="s">
+      <c r="F13" s="32" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:6">
-      <c r="A14" s="28">
+      <c r="A14" s="29">
         <v>1</v>
       </c>
       <c r="B14" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="28" t="s">
+      <c r="C14" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D14" s="4" t="s">
@@ -10273,18 +10276,18 @@
       <c r="E14" s="4" t="s">
         <v>43</v>
       </c>
-      <c r="F14" s="31" t="s">
+      <c r="F14" s="32" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="28">
+      <c r="A15" s="29">
         <v>1</v>
       </c>
       <c r="B15" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C15" s="28" t="s">
+      <c r="C15" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D15" s="4" t="s">
@@ -10293,18 +10296,18 @@
       <c r="E15" s="4" t="s">
         <v>46</v>
       </c>
-      <c r="F15" s="31" t="s">
+      <c r="F15" s="32" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="16" spans="1:6">
-      <c r="A16" s="28">
+      <c r="A16" s="29">
         <v>1</v>
       </c>
       <c r="B16" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C16" s="28" t="s">
+      <c r="C16" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D16" s="4" t="s">
@@ -10313,18 +10316,18 @@
       <c r="E16" s="4" t="s">
         <v>49</v>
       </c>
-      <c r="F16" s="31" t="s">
+      <c r="F16" s="32" t="s">
         <v>50</v>
       </c>
     </row>
     <row r="17" spans="1:6">
-      <c r="A17" s="28">
+      <c r="A17" s="29">
         <v>1</v>
       </c>
       <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="28" t="s">
+      <c r="C17" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D17" s="4" t="s">
@@ -10333,18 +10336,18 @@
       <c r="E17" s="4" t="s">
         <v>52</v>
       </c>
-      <c r="F17" s="31" t="s">
+      <c r="F17" s="32" t="s">
         <v>53</v>
       </c>
     </row>
     <row r="18" spans="1:6">
-      <c r="A18" s="28">
+      <c r="A18" s="29">
         <v>1</v>
       </c>
       <c r="B18" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C18" s="28" t="s">
+      <c r="C18" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D18" s="4" t="s">
@@ -10353,18 +10356,18 @@
       <c r="E18" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="F18" s="31" t="s">
+      <c r="F18" s="32" t="s">
         <v>56</v>
       </c>
     </row>
     <row r="19" spans="1:6">
-      <c r="A19" s="28">
+      <c r="A19" s="29">
         <v>1</v>
       </c>
       <c r="B19" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C19" s="28" t="s">
+      <c r="C19" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D19" s="4" t="s">
@@ -10373,18 +10376,18 @@
       <c r="E19" s="4" t="s">
         <v>58</v>
       </c>
-      <c r="F19" s="31" t="s">
+      <c r="F19" s="32" t="s">
         <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="28">
+      <c r="A20" s="29">
         <v>1</v>
       </c>
       <c r="B20" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C20" s="28" t="s">
+      <c r="C20" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D20" s="4" t="s">
@@ -10393,18 +10396,18 @@
       <c r="E20" s="4" t="s">
         <v>61</v>
       </c>
-      <c r="F20" s="31" t="s">
+      <c r="F20" s="32" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="21" spans="1:6">
-      <c r="A21" s="28">
+      <c r="A21" s="29">
         <v>1</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C21" s="28" t="s">
+      <c r="C21" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D21" s="4" t="s">
@@ -10413,18 +10416,18 @@
       <c r="E21" s="4" t="s">
         <v>64</v>
       </c>
-      <c r="F21" s="31" t="s">
+      <c r="F21" s="32" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="22" spans="1:6">
-      <c r="A22" s="28">
+      <c r="A22" s="29">
         <v>1</v>
       </c>
       <c r="B22" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C22" s="28" t="s">
+      <c r="C22" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D22" s="4" t="s">
@@ -10433,18 +10436,18 @@
       <c r="E22" s="4" t="s">
         <v>67</v>
       </c>
-      <c r="F22" s="31" t="s">
+      <c r="F22" s="32" t="s">
         <v>68</v>
       </c>
     </row>
     <row r="23" spans="1:6">
-      <c r="A23" s="28">
+      <c r="A23" s="29">
         <v>1</v>
       </c>
       <c r="B23" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C23" s="28" t="s">
+      <c r="C23" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D23" s="4" t="s">
@@ -10453,18 +10456,18 @@
       <c r="E23" s="4" t="s">
         <v>70</v>
       </c>
-      <c r="F23" s="31" t="s">
+      <c r="F23" s="32" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="24" spans="1:6">
-      <c r="A24" s="28">
+      <c r="A24" s="29">
         <v>1</v>
       </c>
       <c r="B24" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C24" s="28" t="s">
+      <c r="C24" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D24" s="4" t="s">
@@ -10473,18 +10476,18 @@
       <c r="E24" s="4" t="s">
         <v>73</v>
       </c>
-      <c r="F24" s="31" t="s">
+      <c r="F24" s="32" t="s">
         <v>74</v>
       </c>
     </row>
     <row r="25" spans="1:6">
-      <c r="A25" s="28">
+      <c r="A25" s="29">
         <v>1</v>
       </c>
       <c r="B25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C25" s="28" t="s">
+      <c r="C25" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D25" s="4" t="s">
@@ -10493,18 +10496,18 @@
       <c r="E25" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="F25" s="31" t="s">
+      <c r="F25" s="32" t="s">
         <v>77</v>
       </c>
     </row>
     <row r="26" spans="1:6">
-      <c r="A26" s="28">
+      <c r="A26" s="29">
         <v>1</v>
       </c>
       <c r="B26" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D26" s="4" t="s">
@@ -10513,18 +10516,18 @@
       <c r="E26" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="F26" s="31" t="s">
+      <c r="F26" s="32" t="s">
         <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="28">
+      <c r="A27" s="29">
         <v>1</v>
       </c>
       <c r="B27" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="28" t="s">
+      <c r="C27" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D27" s="4" t="s">
@@ -10533,18 +10536,18 @@
       <c r="E27" s="4" t="s">
         <v>82</v>
       </c>
-      <c r="F27" s="31" t="s">
+      <c r="F27" s="32" t="s">
         <v>83</v>
       </c>
     </row>
     <row r="28" spans="1:6">
-      <c r="A28" s="28">
+      <c r="A28" s="29">
         <v>1</v>
       </c>
       <c r="B28" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D28" s="4" t="s">
@@ -10553,18 +10556,18 @@
       <c r="E28" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F28" s="31" t="s">
+      <c r="F28" s="32" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="28">
+      <c r="A29" s="29">
         <v>1</v>
       </c>
       <c r="B29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C29" s="28" t="s">
+      <c r="C29" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D29" s="4" t="s">
@@ -10573,18 +10576,18 @@
       <c r="E29" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="F29" s="31" t="s">
+      <c r="F29" s="32" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="30" spans="1:6">
-      <c r="A30" s="28">
+      <c r="A30" s="29">
         <v>1</v>
       </c>
       <c r="B30" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C30" s="28" t="s">
+      <c r="C30" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D30" s="4" t="s">
@@ -10593,18 +10596,18 @@
       <c r="E30" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="F30" s="31" t="s">
+      <c r="F30" s="32" t="s">
         <v>92</v>
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="28">
+      <c r="A31" s="29">
         <v>1</v>
       </c>
       <c r="B31" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C31" s="28" t="s">
+      <c r="C31" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D31" s="4" t="s">
@@ -10613,18 +10616,18 @@
       <c r="E31" s="4" t="s">
         <v>94</v>
       </c>
-      <c r="F31" s="31" t="s">
+      <c r="F31" s="32" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="32" spans="1:6">
-      <c r="A32" s="28">
+      <c r="A32" s="29">
         <v>1</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C32" s="28" t="s">
+      <c r="C32" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D32" s="4" t="s">
@@ -10633,18 +10636,18 @@
       <c r="E32" s="4" t="s">
         <v>97</v>
       </c>
-      <c r="F32" s="31" t="s">
+      <c r="F32" s="32" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="33" spans="1:6">
-      <c r="A33" s="28">
+      <c r="A33" s="29">
         <v>1</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C33" s="28" t="s">
+      <c r="C33" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D33" s="4" t="s">
@@ -10653,18 +10656,18 @@
       <c r="E33" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="F33" s="31" t="s">
+      <c r="F33" s="32" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="34" spans="1:6">
-      <c r="A34" s="28">
+      <c r="A34" s="29">
         <v>1</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C34" s="28" t="s">
+      <c r="C34" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D34" s="4" t="s">
@@ -10673,18 +10676,18 @@
       <c r="E34" s="4" t="s">
         <v>103</v>
       </c>
-      <c r="F34" s="31" t="s">
+      <c r="F34" s="32" t="s">
         <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:6">
-      <c r="A35" s="28">
+      <c r="A35" s="29">
         <v>1</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="28" t="s">
+      <c r="C35" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D35" s="4" t="s">
@@ -10693,18 +10696,18 @@
       <c r="E35" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="F35" s="31" t="s">
+      <c r="F35" s="32" t="s">
         <v>107</v>
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="28">
+      <c r="A36" s="29">
         <v>1</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C36" s="28" t="s">
+      <c r="C36" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D36" s="4" t="s">
@@ -10713,18 +10716,18 @@
       <c r="E36" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="F36" s="31" t="s">
+      <c r="F36" s="32" t="s">
         <v>110</v>
       </c>
     </row>
     <row r="37" spans="1:6">
-      <c r="A37" s="28">
+      <c r="A37" s="29">
         <v>1</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C37" s="28" t="s">
+      <c r="C37" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D37" s="4" t="s">
@@ -10733,18 +10736,18 @@
       <c r="E37" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="F37" s="31" t="s">
+      <c r="F37" s="32" t="s">
         <v>113</v>
       </c>
     </row>
     <row r="38" spans="1:6">
-      <c r="A38" s="28">
+      <c r="A38" s="29">
         <v>1</v>
       </c>
       <c r="B38" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C38" s="28" t="s">
+      <c r="C38" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D38" s="4" t="s">
@@ -10753,18 +10756,18 @@
       <c r="E38" s="4" t="s">
         <v>115</v>
       </c>
-      <c r="F38" s="31" t="s">
+      <c r="F38" s="32" t="s">
         <v>116</v>
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="28">
+      <c r="A39" s="29">
         <v>1</v>
       </c>
       <c r="B39" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C39" s="28" t="s">
+      <c r="C39" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D39" s="4" t="s">
@@ -10773,18 +10776,18 @@
       <c r="E39" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="F39" s="31" t="s">
+      <c r="F39" s="32" t="s">
         <v>119</v>
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="28">
+      <c r="A40" s="29">
         <v>1</v>
       </c>
       <c r="B40" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C40" s="28" t="s">
+      <c r="C40" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D40" s="4" t="s">
@@ -10793,18 +10796,18 @@
       <c r="E40" s="4" t="s">
         <v>121</v>
       </c>
-      <c r="F40" s="31" t="s">
+      <c r="F40" s="32" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="41" spans="1:6">
-      <c r="A41" s="28">
+      <c r="A41" s="29">
         <v>1</v>
       </c>
       <c r="B41" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C41" s="28" t="s">
+      <c r="C41" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D41" s="4" t="s">
@@ -10813,18 +10816,18 @@
       <c r="E41" s="4" t="s">
         <v>124</v>
       </c>
-      <c r="F41" s="31" t="s">
+      <c r="F41" s="32" t="s">
         <v>125</v>
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="28">
+      <c r="A42" s="29">
         <v>1</v>
       </c>
       <c r="B42" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C42" s="28" t="s">
+      <c r="C42" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D42" s="4" t="s">
@@ -10833,18 +10836,18 @@
       <c r="E42" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="F42" s="31" t="s">
+      <c r="F42" s="32" t="s">
         <v>128</v>
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="28">
+      <c r="A43" s="29">
         <v>1</v>
       </c>
       <c r="B43" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C43" s="28" t="s">
+      <c r="C43" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D43" s="4" t="s">
@@ -10853,18 +10856,18 @@
       <c r="E43" s="4" t="s">
         <v>131</v>
       </c>
-      <c r="F43" s="31" t="s">
+      <c r="F43" s="32" t="s">
         <v>132</v>
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="28">
+      <c r="A44" s="29">
         <v>1</v>
       </c>
       <c r="B44" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C44" s="28" t="s">
+      <c r="C44" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D44" s="4" t="s">
@@ -10873,18 +10876,18 @@
       <c r="E44" s="4" t="s">
         <v>134</v>
       </c>
-      <c r="F44" s="31" t="s">
+      <c r="F44" s="32" t="s">
         <v>135</v>
       </c>
     </row>
     <row r="45" spans="1:6">
-      <c r="A45" s="28">
+      <c r="A45" s="29">
         <v>1</v>
       </c>
       <c r="B45" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C45" s="28" t="s">
+      <c r="C45" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D45" s="4" t="s">
@@ -10893,18 +10896,18 @@
       <c r="E45" s="4" t="s">
         <v>137</v>
       </c>
-      <c r="F45" s="31" t="s">
+      <c r="F45" s="32" t="s">
         <v>138</v>
       </c>
     </row>
     <row r="46" spans="1:6">
-      <c r="A46" s="28">
+      <c r="A46" s="29">
         <v>1</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C46" s="28" t="s">
+      <c r="C46" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D46" s="4" t="s">
@@ -10913,18 +10916,18 @@
       <c r="E46" s="4" t="s">
         <v>140</v>
       </c>
-      <c r="F46" s="31" t="s">
+      <c r="F46" s="32" t="s">
         <v>141</v>
       </c>
     </row>
     <row r="47" spans="1:6">
-      <c r="A47" s="28">
+      <c r="A47" s="29">
         <v>1</v>
       </c>
       <c r="B47" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C47" s="28" t="s">
+      <c r="C47" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D47" s="4" t="s">
@@ -10933,18 +10936,18 @@
       <c r="E47" s="4" t="s">
         <v>143</v>
       </c>
-      <c r="F47" s="31" t="s">
+      <c r="F47" s="32" t="s">
         <v>144</v>
       </c>
     </row>
     <row r="48" spans="1:6">
-      <c r="A48" s="28">
+      <c r="A48" s="29">
         <v>1</v>
       </c>
       <c r="B48" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C48" s="28" t="s">
+      <c r="C48" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D48" s="4" t="s">
@@ -10953,18 +10956,18 @@
       <c r="E48" s="4" t="s">
         <v>146</v>
       </c>
-      <c r="F48" s="31" t="s">
+      <c r="F48" s="32" t="s">
         <v>147</v>
       </c>
     </row>
     <row r="49" spans="1:6">
-      <c r="A49" s="28">
+      <c r="A49" s="29">
         <v>1</v>
       </c>
       <c r="B49" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C49" s="28" t="s">
+      <c r="C49" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D49" s="4" t="s">
@@ -10973,18 +10976,18 @@
       <c r="E49" s="4" t="s">
         <v>149</v>
       </c>
-      <c r="F49" s="31" t="s">
+      <c r="F49" s="32" t="s">
         <v>150</v>
       </c>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="28">
+      <c r="A50" s="29">
         <v>1</v>
       </c>
       <c r="B50" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C50" s="28" t="s">
+      <c r="C50" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D50" s="4" t="s">
@@ -10993,18 +10996,18 @@
       <c r="E50" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="F50" s="31" t="s">
+      <c r="F50" s="32" t="s">
         <v>153</v>
       </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="28">
+      <c r="A51" s="29">
         <v>1</v>
       </c>
       <c r="B51" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C51" s="28" t="s">
+      <c r="C51" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D51" s="4" t="s">
@@ -11013,18 +11016,18 @@
       <c r="E51" s="4" t="s">
         <v>155</v>
       </c>
-      <c r="F51" s="31" t="s">
+      <c r="F51" s="32" t="s">
         <v>156</v>
       </c>
     </row>
     <row r="52" spans="1:6">
-      <c r="A52" s="28">
+      <c r="A52" s="29">
         <v>1</v>
       </c>
       <c r="B52" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C52" s="28" t="s">
+      <c r="C52" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D52" s="4" t="s">
@@ -11033,18 +11036,18 @@
       <c r="E52" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="F52" s="31" t="s">
+      <c r="F52" s="32" t="s">
         <v>159</v>
       </c>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="28">
+      <c r="A53" s="29">
         <v>1</v>
       </c>
       <c r="B53" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C53" s="28" t="s">
+      <c r="C53" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D53" s="4" t="s">
@@ -11053,18 +11056,18 @@
       <c r="E53" s="4" t="s">
         <v>161</v>
       </c>
-      <c r="F53" s="31" t="s">
+      <c r="F53" s="32" t="s">
         <v>162</v>
       </c>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="28">
+      <c r="A54" s="29">
         <v>1</v>
       </c>
       <c r="B54" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C54" s="28" t="s">
+      <c r="C54" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D54" s="4" t="s">
@@ -11073,18 +11076,18 @@
       <c r="E54" s="4" t="s">
         <v>164</v>
       </c>
-      <c r="F54" s="31" t="s">
+      <c r="F54" s="32" t="s">
         <v>165</v>
       </c>
     </row>
     <row r="55" spans="1:6">
-      <c r="A55" s="28">
+      <c r="A55" s="29">
         <v>1</v>
       </c>
       <c r="B55" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C55" s="28" t="s">
+      <c r="C55" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D55" s="4" t="s">
@@ -11093,18 +11096,18 @@
       <c r="E55" s="4" t="s">
         <v>167</v>
       </c>
-      <c r="F55" s="31" t="s">
+      <c r="F55" s="32" t="s">
         <v>168</v>
       </c>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="28">
+      <c r="A56" s="29">
         <v>1</v>
       </c>
       <c r="B56" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C56" s="28" t="s">
+      <c r="C56" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D56" s="4" t="s">
@@ -11113,18 +11116,18 @@
       <c r="E56" s="4" t="s">
         <v>170</v>
       </c>
-      <c r="F56" s="31" t="s">
+      <c r="F56" s="32" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="28">
+      <c r="A57" s="29">
         <v>1</v>
       </c>
       <c r="B57" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C57" s="28" t="s">
+      <c r="C57" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D57" s="4" t="s">
@@ -11133,18 +11136,18 @@
       <c r="E57" s="4" t="s">
         <v>173</v>
       </c>
-      <c r="F57" s="31" t="s">
+      <c r="F57" s="32" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="28">
+      <c r="A58" s="29">
         <v>1</v>
       </c>
       <c r="B58" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C58" s="28" t="s">
+      <c r="C58" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D58" s="4" t="s">
@@ -11153,18 +11156,18 @@
       <c r="E58" s="4" t="s">
         <v>176</v>
       </c>
-      <c r="F58" s="31" t="s">
+      <c r="F58" s="32" t="s">
         <v>177</v>
       </c>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="28">
+      <c r="A59" s="29">
         <v>1</v>
       </c>
       <c r="B59" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C59" s="28" t="s">
+      <c r="C59" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D59" s="4" t="s">
@@ -11173,18 +11176,18 @@
       <c r="E59" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="F59" s="31" t="s">
+      <c r="F59" s="32" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="60" spans="1:6">
-      <c r="A60" s="28">
+      <c r="A60" s="29">
         <v>1</v>
       </c>
       <c r="B60" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C60" s="28" t="s">
+      <c r="C60" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D60" s="4" t="s">
@@ -11193,18 +11196,18 @@
       <c r="E60" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="F60" s="31" t="s">
+      <c r="F60" s="32" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="61" spans="1:6">
-      <c r="A61" s="28">
+      <c r="A61" s="29">
         <v>1</v>
       </c>
       <c r="B61" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C61" s="28" t="s">
+      <c r="C61" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D61" s="4" t="s">
@@ -11213,18 +11216,18 @@
       <c r="E61" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="F61" s="31" t="s">
+      <c r="F61" s="32" t="s">
         <v>181</v>
       </c>
     </row>
     <row r="62" spans="1:6">
-      <c r="A62" s="28">
+      <c r="A62" s="29">
         <v>1</v>
       </c>
       <c r="B62" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="C62" s="28" t="s">
+      <c r="C62" s="29" t="s">
         <v>8</v>
       </c>
       <c r="D62" s="4" t="s">
@@ -11233,7 +11236,7 @@
       <c r="E62" s="4" t="s">
         <v>178</v>
       </c>
-      <c r="F62" s="31" t="s">
+      <c r="F62" s="32" t="s">
         <v>182</v>
       </c>
     </row>
@@ -11248,20 +11251,20 @@
   <sheetPr/>
   <dimension ref="A1:P116"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="C1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A46" activePane="bottomLeft" state="frozen"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" topLeftCell="D1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A20" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="I34" sqref="I34"/>
+      <selection pane="bottomLeft" activeCell="O26" sqref="O26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="9" style="17"/>
-    <col min="2" max="2" width="27.8857142857143" style="17" customWidth="1"/>
-    <col min="3" max="3" width="12.1714285714286" style="17" customWidth="1"/>
-    <col min="4" max="16" width="9" style="17"/>
-    <col min="17" max="17" width="14.4380952380952" style="17" customWidth="1"/>
-    <col min="18" max="16384" width="9" style="17"/>
+    <col min="1" max="1" width="9" style="18"/>
+    <col min="2" max="2" width="27.8857142857143" style="18" customWidth="1"/>
+    <col min="3" max="3" width="12.1714285714286" style="18" customWidth="1"/>
+    <col min="4" max="16" width="9" style="18"/>
+    <col min="17" max="17" width="14.4380952380952" style="18" customWidth="1"/>
+    <col min="18" max="16384" width="9" style="18"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16">
@@ -11899,7 +11902,7 @@
       <c r="N13" s="4" t="s">
         <v>926</v>
       </c>
-      <c r="O13" s="4" t="s">
+      <c r="O13" s="19" t="s">
         <v>973</v>
       </c>
       <c r="P13" s="4" t="s">
@@ -18027,13 +18030,13 @@
       <c r="E2" t="s">
         <v>1821</v>
       </c>
-      <c r="F2" s="15" t="s">
+      <c r="F2" s="16" t="s">
         <v>1822</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="17" t="s">
         <v>475</v>
       </c>
-      <c r="H2" s="16" t="s">
+      <c r="H2" s="17" t="s">
         <v>623</v>
       </c>
       <c r="I2" t="s">
@@ -18045,7 +18048,7 @@
       <c r="L2">
         <v>6</v>
       </c>
-      <c r="M2" s="32" t="s">
+      <c r="M2" s="33" t="s">
         <v>1823</v>
       </c>
     </row>
@@ -18065,13 +18068,13 @@
       <c r="E3" t="s">
         <v>1825</v>
       </c>
-      <c r="F3" s="15" t="s">
+      <c r="F3" s="16" t="s">
         <v>1826</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="H3" s="16" t="s">
+      <c r="H3" s="17" t="s">
         <v>639</v>
       </c>
       <c r="K3">
@@ -18080,7 +18083,7 @@
       <c r="L3">
         <v>6</v>
       </c>
-      <c r="M3" s="32" t="s">
+      <c r="M3" s="33" t="s">
         <v>1823</v>
       </c>
     </row>
@@ -18100,13 +18103,13 @@
       <c r="E4" t="s">
         <v>1828</v>
       </c>
-      <c r="F4" s="15" t="s">
+      <c r="F4" s="16" t="s">
         <v>1829</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="17" t="s">
         <v>504</v>
       </c>
-      <c r="H4" s="16">
+      <c r="H4" s="17">
         <v>565656</v>
       </c>
       <c r="K4">
@@ -18115,10 +18118,10 @@
       <c r="L4">
         <v>6</v>
       </c>
-      <c r="M4" s="32" t="s">
+      <c r="M4" s="33" t="s">
         <v>1823</v>
       </c>
-      <c r="O4" s="32" t="s">
+      <c r="O4" s="33" t="s">
         <v>1830</v>
       </c>
     </row>
@@ -18138,10 +18141,10 @@
       <c r="E5" t="s">
         <v>1832</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="17" t="s">
         <v>507</v>
       </c>
-      <c r="H5" s="16" t="s">
+      <c r="H5" s="17" t="s">
         <v>666</v>
       </c>
       <c r="K5">
@@ -18150,7 +18153,7 @@
       <c r="L5">
         <v>6</v>
       </c>
-      <c r="M5" s="32" t="s">
+      <c r="M5" s="33" t="s">
         <v>1823</v>
       </c>
     </row>
@@ -18170,13 +18173,13 @@
       <c r="E6" t="s">
         <v>1834</v>
       </c>
-      <c r="F6" s="15" t="s">
+      <c r="F6" s="16" t="s">
         <v>1835</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="17" t="s">
         <v>512</v>
       </c>
-      <c r="H6" s="16" t="s">
+      <c r="H6" s="17" t="s">
         <v>682</v>
       </c>
       <c r="K6">
@@ -18185,7 +18188,7 @@
       <c r="L6">
         <v>6</v>
       </c>
-      <c r="M6" s="32" t="s">
+      <c r="M6" s="33" t="s">
         <v>1823</v>
       </c>
     </row>
@@ -18205,13 +18208,13 @@
       <c r="E7" t="s">
         <v>1837</v>
       </c>
-      <c r="F7" s="15" t="s">
+      <c r="F7" s="16" t="s">
         <v>1838</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="17" t="s">
         <v>525</v>
       </c>
-      <c r="H7" s="16">
+      <c r="H7" s="17">
         <v>790200</v>
       </c>
       <c r="K7">
@@ -18220,7 +18223,7 @@
       <c r="L7" t="s">
         <v>1839</v>
       </c>
-      <c r="M7" s="32" t="s">
+      <c r="M7" s="33" t="s">
         <v>1823</v>
       </c>
     </row>
@@ -22335,8 +22338,8 @@
   <sheetPr/>
   <dimension ref="A1:AI98"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="U7" sqref="U7"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="U2" sqref="U2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -22521,7 +22524,7 @@
       <c r="T2" s="14" t="s">
         <v>2114</v>
       </c>
-      <c r="U2" s="14" t="s">
+      <c r="U2" s="15" t="s">
         <v>2115</v>
       </c>
       <c r="V2" s="14" t="s">
@@ -37641,13 +37644,13 @@
       <c r="F2" t="s">
         <v>2866</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="33" t="s">
         <v>2867</v>
       </c>
-      <c r="H2" s="32" t="s">
+      <c r="H2" s="33" t="s">
         <v>2868</v>
       </c>
-      <c r="I2" s="32" t="s">
+      <c r="I2" s="33" t="s">
         <v>2869</v>
       </c>
       <c r="J2" t="s">
@@ -37691,13 +37694,13 @@
       <c r="F3" t="s">
         <v>2878</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="33" t="s">
         <v>2867</v>
       </c>
-      <c r="H3" s="32" t="s">
+      <c r="H3" s="33" t="s">
         <v>2879</v>
       </c>
-      <c r="I3" s="32" t="s">
+      <c r="I3" s="33" t="s">
         <v>2869</v>
       </c>
       <c r="J3" t="s">
@@ -37741,13 +37744,13 @@
       <c r="F4" t="s">
         <v>2884</v>
       </c>
-      <c r="G4" s="32" t="s">
+      <c r="G4" s="33" t="s">
         <v>2867</v>
       </c>
-      <c r="H4" s="32" t="s">
+      <c r="H4" s="33" t="s">
         <v>2885</v>
       </c>
-      <c r="I4" s="32" t="s">
+      <c r="I4" s="33" t="s">
         <v>2869</v>
       </c>
       <c r="J4" t="s">
@@ -37812,7 +37815,7 @@
       <c r="A3" t="s">
         <v>2890</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="33" t="s">
         <v>2891</v>
       </c>
     </row>
@@ -37820,7 +37823,7 @@
       <c r="A4" t="s">
         <v>2892</v>
       </c>
-      <c r="B4" s="32" t="s">
+      <c r="B4" s="33" t="s">
         <v>2893</v>
       </c>
     </row>
@@ -37828,7 +37831,7 @@
       <c r="A5" t="s">
         <v>569</v>
       </c>
-      <c r="B5" s="32" t="s">
+      <c r="B5" s="33" t="s">
         <v>2894</v>
       </c>
     </row>
@@ -37892,7 +37895,7 @@
       <c r="A13" t="s">
         <v>2909</v>
       </c>
-      <c r="B13" s="32" t="s">
+      <c r="B13" s="33" t="s">
         <v>2910</v>
       </c>
     </row>
@@ -37900,7 +37903,7 @@
       <c r="A14" t="s">
         <v>737</v>
       </c>
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="33" t="s">
         <v>2911</v>
       </c>
     </row>
@@ -37908,7 +37911,7 @@
       <c r="A15" t="s">
         <v>467</v>
       </c>
-      <c r="B15" s="32" t="s">
+      <c r="B15" s="33" t="s">
         <v>2912</v>
       </c>
     </row>
@@ -37916,7 +37919,7 @@
       <c r="A16" t="s">
         <v>747</v>
       </c>
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="33" t="s">
         <v>2913</v>
       </c>
     </row>
@@ -37924,7 +37927,7 @@
       <c r="A17" t="s">
         <v>742</v>
       </c>
-      <c r="B17" s="32" t="s">
+      <c r="B17" s="33" t="s">
         <v>2914</v>
       </c>
     </row>
@@ -37932,7 +37935,7 @@
       <c r="A18" t="s">
         <v>752</v>
       </c>
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="33" t="s">
         <v>2915</v>
       </c>
     </row>
@@ -37940,7 +37943,7 @@
       <c r="A19" t="s">
         <v>760</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="33" t="s">
         <v>2916</v>
       </c>
     </row>
@@ -37948,7 +37951,7 @@
       <c r="A20" t="s">
         <v>763</v>
       </c>
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="33" t="s">
         <v>2917</v>
       </c>
     </row>
@@ -37956,7 +37959,7 @@
       <c r="A21" t="s">
         <v>766</v>
       </c>
-      <c r="B21" s="32" t="s">
+      <c r="B21" s="33" t="s">
         <v>2918</v>
       </c>
     </row>
@@ -37964,7 +37967,7 @@
       <c r="A22" t="s">
         <v>468</v>
       </c>
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="33" t="s">
         <v>2919</v>
       </c>
     </row>
@@ -37972,7 +37975,7 @@
       <c r="A23" t="s">
         <v>756</v>
       </c>
-      <c r="B23" s="32" t="s">
+      <c r="B23" s="33" t="s">
         <v>2920</v>
       </c>
     </row>
@@ -38108,7 +38111,7 @@
       </c>
     </row>
     <row r="7" spans="1:6">
-      <c r="A7" s="22">
+      <c r="A7" s="23">
         <v>1</v>
       </c>
       <c r="B7" s="9" t="s">
@@ -38128,7 +38131,7 @@
       </c>
     </row>
     <row r="8" spans="1:6">
-      <c r="A8" s="23">
+      <c r="A8" s="24">
         <v>1</v>
       </c>
       <c r="B8" s="9" t="s">
@@ -38148,7 +38151,7 @@
       </c>
     </row>
     <row r="9" spans="1:6">
-      <c r="A9" s="23">
+      <c r="A9" s="24">
         <v>1</v>
       </c>
       <c r="B9" s="9" t="s">
@@ -38208,7 +38211,7 @@
       </c>
     </row>
     <row r="12" spans="1:6">
-      <c r="A12" s="23">
+      <c r="A12" s="24">
         <v>1</v>
       </c>
       <c r="B12" s="9" t="s">
@@ -38228,7 +38231,7 @@
       </c>
     </row>
     <row r="13" spans="1:6">
-      <c r="A13" s="24">
+      <c r="A13" s="25">
         <v>1</v>
       </c>
       <c r="B13" s="9" t="s">
@@ -38268,7 +38271,7 @@
       </c>
     </row>
     <row r="15" spans="1:6">
-      <c r="A15" s="24">
+      <c r="A15" s="25">
         <v>1</v>
       </c>
       <c r="B15" s="9" t="s">
@@ -38368,7 +38371,7 @@
       </c>
     </row>
     <row r="20" spans="1:6">
-      <c r="A20" s="23">
+      <c r="A20" s="24">
         <v>1</v>
       </c>
       <c r="B20" s="9" t="s">
@@ -38508,7 +38511,7 @@
       </c>
     </row>
     <row r="27" spans="1:6">
-      <c r="A27" s="22">
+      <c r="A27" s="23">
         <v>1</v>
       </c>
       <c r="B27" s="9" t="s">
@@ -38548,7 +38551,7 @@
       </c>
     </row>
     <row r="29" spans="1:6">
-      <c r="A29" s="23">
+      <c r="A29" s="24">
         <v>1</v>
       </c>
       <c r="B29" s="9" t="s">
@@ -38588,7 +38591,7 @@
       </c>
     </row>
     <row r="31" spans="1:6">
-      <c r="A31" s="24">
+      <c r="A31" s="25">
         <v>1</v>
       </c>
       <c r="B31" s="9" t="s">
@@ -38688,7 +38691,7 @@
       </c>
     </row>
     <row r="36" spans="1:6">
-      <c r="A36" s="25">
+      <c r="A36" s="26">
         <v>1</v>
       </c>
       <c r="B36" s="9" t="s">
@@ -38748,7 +38751,7 @@
       </c>
     </row>
     <row r="39" spans="1:6">
-      <c r="A39" s="23">
+      <c r="A39" s="24">
         <v>1</v>
       </c>
       <c r="B39" s="9" t="s">
@@ -38768,7 +38771,7 @@
       </c>
     </row>
     <row r="40" spans="1:6">
-      <c r="A40" s="24">
+      <c r="A40" s="25">
         <v>1</v>
       </c>
       <c r="B40" s="9" t="s">
@@ -38808,7 +38811,7 @@
       </c>
     </row>
     <row r="42" spans="1:6">
-      <c r="A42" s="23">
+      <c r="A42" s="24">
         <v>1</v>
       </c>
       <c r="B42" s="9" t="s">
@@ -38828,7 +38831,7 @@
       </c>
     </row>
     <row r="43" spans="1:6">
-      <c r="A43" s="22">
+      <c r="A43" s="23">
         <v>1</v>
       </c>
       <c r="B43" s="9" t="s">
@@ -38848,7 +38851,7 @@
       </c>
     </row>
     <row r="44" spans="1:6">
-      <c r="A44" s="24">
+      <c r="A44" s="25">
         <v>1</v>
       </c>
       <c r="B44" s="9" t="s">
@@ -38968,7 +38971,7 @@
       </c>
     </row>
     <row r="50" spans="1:6">
-      <c r="A50" s="23">
+      <c r="A50" s="24">
         <v>1</v>
       </c>
       <c r="B50" s="9" t="s">
@@ -38988,7 +38991,7 @@
       </c>
     </row>
     <row r="51" spans="1:6">
-      <c r="A51" s="23">
+      <c r="A51" s="24">
         <v>1</v>
       </c>
       <c r="B51" s="9" t="s">
@@ -39028,7 +39031,7 @@
       </c>
     </row>
     <row r="53" spans="1:6">
-      <c r="A53" s="23">
+      <c r="A53" s="24">
         <v>1</v>
       </c>
       <c r="B53" s="9" t="s">
@@ -39048,7 +39051,7 @@
       </c>
     </row>
     <row r="54" spans="1:6">
-      <c r="A54" s="23">
+      <c r="A54" s="24">
         <v>1</v>
       </c>
       <c r="B54" s="9" t="s">
@@ -39088,7 +39091,7 @@
       </c>
     </row>
     <row r="56" spans="1:6">
-      <c r="A56" s="23">
+      <c r="A56" s="24">
         <v>1</v>
       </c>
       <c r="B56" s="9" t="s">
@@ -39108,7 +39111,7 @@
       </c>
     </row>
     <row r="57" spans="1:6">
-      <c r="A57" s="23">
+      <c r="A57" s="24">
         <v>1</v>
       </c>
       <c r="B57" s="9" t="s">
@@ -39128,7 +39131,7 @@
       </c>
     </row>
     <row r="58" spans="1:6">
-      <c r="A58" s="23">
+      <c r="A58" s="24">
         <v>1</v>
       </c>
       <c r="B58" s="9" t="s">
@@ -39148,7 +39151,7 @@
       </c>
     </row>
     <row r="59" spans="1:6">
-      <c r="A59" s="23">
+      <c r="A59" s="24">
         <v>1</v>
       </c>
       <c r="B59" s="9" t="s">
@@ -39198,14 +39201,14 @@
   <sheetPr/>
   <dimension ref="A1:L62"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="2" max="2" width="17.4380952380952" customWidth="1"/>
-    <col min="6" max="9" width="9" style="20"/>
+    <col min="6" max="9" width="9" style="22"/>
     <col min="10" max="10" width="19.7809523809524" customWidth="1"/>
     <col min="11" max="11" width="13.1047619047619" customWidth="1"/>
     <col min="12" max="12" width="10.9142857142857" customWidth="1"/>
@@ -39416,7 +39419,7 @@
       <c r="J7" s="9" t="s">
         <v>337</v>
       </c>
-      <c r="K7" s="21" t="s">
+      <c r="K7" s="9" t="s">
         <v>338</v>
       </c>
       <c r="L7" s="9" t="s">
@@ -40700,7 +40703,7 @@
       <c r="F2" t="s">
         <v>439</v>
       </c>
-      <c r="G2" s="32" t="s">
+      <c r="G2" s="33" t="s">
         <v>440</v>
       </c>
       <c r="H2" t="s">
@@ -40726,7 +40729,7 @@
       <c r="F3" t="s">
         <v>439</v>
       </c>
-      <c r="G3" s="32" t="s">
+      <c r="G3" s="33" t="s">
         <v>443</v>
       </c>
       <c r="H3" t="s">
@@ -40898,7 +40901,7 @@
       <c r="G2" t="s">
         <v>474</v>
       </c>
-      <c r="I2" s="16" t="s">
+      <c r="I2" s="17" t="s">
         <v>475</v>
       </c>
       <c r="J2">
@@ -40913,13 +40916,13 @@
       <c r="M2" t="s">
         <v>478</v>
       </c>
-      <c r="N2" s="32" t="s">
+      <c r="N2" s="33" t="s">
         <v>479</v>
       </c>
-      <c r="O2" s="32" t="s">
+      <c r="O2" s="33" t="s">
         <v>480</v>
       </c>
-      <c r="P2" s="32" t="s">
+      <c r="P2" s="33" t="s">
         <v>481</v>
       </c>
       <c r="Q2" t="s">
@@ -40936,7 +40939,7 @@
       </c>
     </row>
     <row r="3" spans="1:20">
-      <c r="A3" s="19">
+      <c r="A3" s="21">
         <v>1</v>
       </c>
       <c r="B3" t="s">
@@ -40957,13 +40960,13 @@
       <c r="H3" t="s">
         <v>488</v>
       </c>
-      <c r="I3" s="16" t="s">
+      <c r="I3" s="17" t="s">
         <v>489</v>
       </c>
       <c r="J3">
         <v>3</v>
       </c>
-      <c r="K3" s="32" t="s">
+      <c r="K3" s="33" t="s">
         <v>490</v>
       </c>
       <c r="L3" t="s">
@@ -40972,13 +40975,13 @@
       <c r="M3" t="s">
         <v>492</v>
       </c>
-      <c r="N3" s="32" t="s">
+      <c r="N3" s="33" t="s">
         <v>493</v>
       </c>
-      <c r="O3" s="32" t="s">
+      <c r="O3" s="33" t="s">
         <v>494</v>
       </c>
-      <c r="P3" s="32" t="s">
+      <c r="P3" s="33" t="s">
         <v>495</v>
       </c>
       <c r="Q3" t="s">
@@ -40995,7 +40998,7 @@
       </c>
     </row>
     <row r="4" spans="1:10">
-      <c r="A4" s="19">
+      <c r="A4" s="21">
         <v>1</v>
       </c>
       <c r="B4" t="s">
@@ -41016,7 +41019,7 @@
       <c r="H4" t="s">
         <v>503</v>
       </c>
-      <c r="I4" s="16" t="s">
+      <c r="I4" s="17" t="s">
         <v>504</v>
       </c>
       <c r="J4">
@@ -41024,7 +41027,7 @@
       </c>
     </row>
     <row r="5" spans="1:10">
-      <c r="A5" s="19">
+      <c r="A5" s="21">
         <v>1</v>
       </c>
       <c r="B5" t="s">
@@ -41042,7 +41045,7 @@
       <c r="G5" t="s">
         <v>506</v>
       </c>
-      <c r="I5" s="16" t="s">
+      <c r="I5" s="17" t="s">
         <v>507</v>
       </c>
       <c r="J5">
@@ -41050,7 +41053,7 @@
       </c>
     </row>
     <row r="6" spans="1:20">
-      <c r="A6" s="19">
+      <c r="A6" s="21">
         <v>1</v>
       </c>
       <c r="B6" t="s">
@@ -41071,13 +41074,13 @@
       <c r="H6" t="s">
         <v>511</v>
       </c>
-      <c r="I6" s="16" t="s">
+      <c r="I6" s="17" t="s">
         <v>512</v>
       </c>
       <c r="J6">
         <v>4</v>
       </c>
-      <c r="K6" s="32" t="s">
+      <c r="K6" s="33" t="s">
         <v>513</v>
       </c>
       <c r="L6" t="s">
@@ -41086,13 +41089,13 @@
       <c r="M6" t="s">
         <v>492</v>
       </c>
-      <c r="N6" s="32" t="s">
+      <c r="N6" s="33" t="s">
         <v>515</v>
       </c>
-      <c r="O6" s="32" t="s">
+      <c r="O6" s="33" t="s">
         <v>516</v>
       </c>
-      <c r="P6" s="32" t="s">
+      <c r="P6" s="33" t="s">
         <v>517</v>
       </c>
       <c r="Q6" t="s">
@@ -41109,7 +41112,7 @@
       </c>
     </row>
     <row r="7" spans="1:13">
-      <c r="A7" s="19">
+      <c r="A7" s="21">
         <v>1</v>
       </c>
       <c r="B7" t="s">
@@ -41130,13 +41133,13 @@
       <c r="H7" t="s">
         <v>524</v>
       </c>
-      <c r="I7" s="16" t="s">
+      <c r="I7" s="17" t="s">
         <v>525</v>
       </c>
       <c r="J7">
         <v>3</v>
       </c>
-      <c r="K7" s="32" t="s">
+      <c r="K7" s="33" t="s">
         <v>526</v>
       </c>
       <c r="L7" t="s">
@@ -41164,9 +41167,9 @@
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
   <cols>
     <col min="3" max="3" width="29.552380952381" customWidth="1"/>
-    <col min="4" max="4" width="16.6666666666667" style="16" customWidth="1"/>
-    <col min="5" max="5" width="18.6666666666667" style="16" customWidth="1"/>
-    <col min="6" max="7" width="15.7809523809524" style="16" customWidth="1"/>
+    <col min="4" max="4" width="16.6666666666667" style="17" customWidth="1"/>
+    <col min="5" max="5" width="18.6666666666667" style="17" customWidth="1"/>
+    <col min="6" max="7" width="15.7809523809524" style="17" customWidth="1"/>
     <col min="8" max="8" width="9.43809523809524" customWidth="1"/>
     <col min="11" max="11" width="13.3333333333333" customWidth="1"/>
     <col min="12" max="12" width="29.4380952380952" customWidth="1"/>
@@ -41194,16 +41197,16 @@
       <c r="C1" t="s">
         <v>183</v>
       </c>
-      <c r="D1" s="16" t="s">
+      <c r="D1" s="17" t="s">
         <v>530</v>
       </c>
-      <c r="E1" s="16" t="s">
+      <c r="E1" s="17" t="s">
         <v>531</v>
       </c>
-      <c r="F1" s="16" t="s">
+      <c r="F1" s="17" t="s">
         <v>532</v>
       </c>
-      <c r="G1" s="16" t="s">
+      <c r="G1" s="17" t="s">
         <v>533</v>
       </c>
       <c r="H1" t="s">
@@ -41334,16 +41337,16 @@
       <c r="C2" t="s">
         <v>570</v>
       </c>
-      <c r="D2" s="16" t="s">
+      <c r="D2" s="17" t="s">
         <v>571</v>
       </c>
-      <c r="E2" s="16" t="s">
+      <c r="E2" s="17" t="s">
         <v>572</v>
       </c>
-      <c r="F2" s="16" t="s">
+      <c r="F2" s="17" t="s">
         <v>573</v>
       </c>
-      <c r="G2" s="16" t="s">
+      <c r="G2" s="17" t="s">
         <v>572</v>
       </c>
       <c r="H2" t="s">
@@ -41367,10 +41370,10 @@
       <c r="N2" t="s">
         <v>579</v>
       </c>
-      <c r="P2" s="32" t="s">
+      <c r="P2" s="33" t="s">
         <v>580</v>
       </c>
-      <c r="AK2" s="32" t="s">
+      <c r="AK2" s="33" t="s">
         <v>581</v>
       </c>
     </row>
@@ -41384,16 +41387,16 @@
       <c r="C3" t="s">
         <v>570</v>
       </c>
-      <c r="D3" s="16" t="s">
+      <c r="D3" s="17" t="s">
         <v>582</v>
       </c>
-      <c r="E3" s="16" t="s">
+      <c r="E3" s="17" t="s">
         <v>571</v>
       </c>
-      <c r="F3" s="16" t="s">
+      <c r="F3" s="17" t="s">
         <v>572</v>
       </c>
-      <c r="G3" s="16" t="s">
+      <c r="G3" s="17" t="s">
         <v>571</v>
       </c>
       <c r="H3" t="s">
@@ -41417,10 +41420,10 @@
       <c r="N3" t="s">
         <v>583</v>
       </c>
-      <c r="P3" s="32" t="s">
+      <c r="P3" s="33" t="s">
         <v>580</v>
       </c>
-      <c r="AK3" s="32" t="s">
+      <c r="AK3" s="33" t="s">
         <v>581</v>
       </c>
     </row>
@@ -41434,16 +41437,16 @@
       <c r="C4" t="s">
         <v>570</v>
       </c>
-      <c r="D4" s="16" t="s">
+      <c r="D4" s="17" t="s">
         <v>573</v>
       </c>
-      <c r="E4" s="16" t="s">
+      <c r="E4" s="17" t="s">
         <v>582</v>
       </c>
-      <c r="F4" s="16" t="s">
+      <c r="F4" s="17" t="s">
         <v>571</v>
       </c>
-      <c r="G4" s="16" t="s">
+      <c r="G4" s="17" t="s">
         <v>582</v>
       </c>
       <c r="H4" t="s">
@@ -41467,10 +41470,10 @@
       <c r="N4" t="s">
         <v>579</v>
       </c>
-      <c r="P4" s="32" t="s">
+      <c r="P4" s="33" t="s">
         <v>580</v>
       </c>
-      <c r="AK4" s="32" t="s">
+      <c r="AK4" s="33" t="s">
         <v>581</v>
       </c>
     </row>
@@ -41484,16 +41487,16 @@
       <c r="C5" t="s">
         <v>570</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="17" t="s">
         <v>572</v>
       </c>
-      <c r="E5" s="16" t="s">
+      <c r="E5" s="17" t="s">
         <v>573</v>
       </c>
-      <c r="F5" s="16" t="s">
+      <c r="F5" s="17" t="s">
         <v>582</v>
       </c>
-      <c r="G5" s="16" t="s">
+      <c r="G5" s="17" t="s">
         <v>573</v>
       </c>
       <c r="H5" t="s">
@@ -41517,10 +41520,10 @@
       <c r="N5" t="s">
         <v>583</v>
       </c>
-      <c r="P5" s="32" t="s">
+      <c r="P5" s="33" t="s">
         <v>580</v>
       </c>
-      <c r="AK5" s="32" t="s">
+      <c r="AK5" s="33" t="s">
         <v>581</v>
       </c>
     </row>
@@ -41531,16 +41534,16 @@
       <c r="B6" t="s">
         <v>569</v>
       </c>
-      <c r="D6" s="16" t="s">
+      <c r="D6" s="17" t="s">
         <v>585</v>
       </c>
-      <c r="E6" s="16" t="s">
+      <c r="E6" s="17" t="s">
         <v>586</v>
       </c>
-      <c r="F6" s="16" t="s">
+      <c r="F6" s="17" t="s">
         <v>587</v>
       </c>
-      <c r="G6" s="16" t="s">
+      <c r="G6" s="17" t="s">
         <v>586</v>
       </c>
       <c r="H6" t="s">
@@ -41567,64 +41570,64 @@
       <c r="P6" t="s">
         <v>591</v>
       </c>
-      <c r="R6" s="32" t="s">
+      <c r="R6" s="33" t="s">
         <v>592</v>
       </c>
-      <c r="S6" s="32" t="s">
+      <c r="S6" s="33" t="s">
         <v>593</v>
       </c>
-      <c r="T6" s="32" t="s">
+      <c r="T6" s="33" t="s">
         <v>594</v>
       </c>
-      <c r="U6" s="32" t="s">
+      <c r="U6" s="33" t="s">
         <v>595</v>
       </c>
-      <c r="V6" s="32" t="s">
+      <c r="V6" s="33" t="s">
         <v>596</v>
       </c>
-      <c r="W6" s="32" t="s">
+      <c r="W6" s="33" t="s">
         <v>597</v>
       </c>
-      <c r="X6" s="32" t="s">
+      <c r="X6" s="33" t="s">
         <v>598</v>
       </c>
-      <c r="Y6" s="32" t="s">
+      <c r="Y6" s="33" t="s">
         <v>599</v>
       </c>
-      <c r="Z6" s="32" t="s">
+      <c r="Z6" s="33" t="s">
         <v>600</v>
       </c>
-      <c r="AA6" s="32" t="s">
+      <c r="AA6" s="33" t="s">
         <v>601</v>
       </c>
-      <c r="AB6" s="32" t="s">
+      <c r="AB6" s="33" t="s">
         <v>602</v>
       </c>
-      <c r="AC6" s="32" t="s">
+      <c r="AC6" s="33" t="s">
         <v>603</v>
       </c>
-      <c r="AD6" s="32" t="s">
+      <c r="AD6" s="33" t="s">
         <v>604</v>
       </c>
-      <c r="AE6" s="32" t="s">
+      <c r="AE6" s="33" t="s">
         <v>605</v>
       </c>
-      <c r="AF6" s="32" t="s">
+      <c r="AF6" s="33" t="s">
         <v>606</v>
       </c>
-      <c r="AG6" s="32" t="s">
+      <c r="AG6" s="33" t="s">
         <v>607</v>
       </c>
-      <c r="AH6" s="32" t="s">
+      <c r="AH6" s="33" t="s">
         <v>607</v>
       </c>
-      <c r="AI6" s="32" t="s">
+      <c r="AI6" s="33" t="s">
         <v>608</v>
       </c>
-      <c r="AJ6" s="32" t="s">
+      <c r="AJ6" s="33" t="s">
         <v>609</v>
       </c>
-      <c r="AK6" s="32" t="s">
+      <c r="AK6" s="33" t="s">
         <v>581</v>
       </c>
       <c r="AP6" t="s">
@@ -41641,16 +41644,16 @@
       <c r="B7" t="s">
         <v>569</v>
       </c>
-      <c r="D7" s="16" t="s">
+      <c r="D7" s="17" t="s">
         <v>585</v>
       </c>
-      <c r="E7" s="16" t="s">
+      <c r="E7" s="17" t="s">
         <v>586</v>
       </c>
-      <c r="F7" s="16" t="s">
+      <c r="F7" s="17" t="s">
         <v>587</v>
       </c>
-      <c r="G7" s="16" t="s">
+      <c r="G7" s="17" t="s">
         <v>586</v>
       </c>
       <c r="H7" t="s">
@@ -41677,61 +41680,61 @@
       <c r="P7" t="s">
         <v>591</v>
       </c>
-      <c r="R7" s="32" t="s">
+      <c r="R7" s="33" t="s">
         <v>592</v>
       </c>
-      <c r="S7" s="32" t="s">
+      <c r="S7" s="33" t="s">
         <v>593</v>
       </c>
-      <c r="T7" s="32" t="s">
+      <c r="T7" s="33" t="s">
         <v>594</v>
       </c>
-      <c r="U7" s="32" t="s">
+      <c r="U7" s="33" t="s">
         <v>595</v>
       </c>
-      <c r="V7" s="32" t="s">
+      <c r="V7" s="33" t="s">
         <v>596</v>
       </c>
-      <c r="W7" s="32" t="s">
+      <c r="W7" s="33" t="s">
         <v>597</v>
       </c>
-      <c r="X7" s="32" t="s">
+      <c r="X7" s="33" t="s">
         <v>598</v>
       </c>
-      <c r="Y7" s="32" t="s">
+      <c r="Y7" s="33" t="s">
         <v>599</v>
       </c>
-      <c r="Z7" s="32" t="s">
+      <c r="Z7" s="33" t="s">
         <v>600</v>
       </c>
-      <c r="AA7" s="32" t="s">
+      <c r="AA7" s="33" t="s">
         <v>601</v>
       </c>
-      <c r="AB7" s="32" t="s">
+      <c r="AB7" s="33" t="s">
         <v>602</v>
       </c>
-      <c r="AC7" s="32" t="s">
+      <c r="AC7" s="33" t="s">
         <v>603</v>
       </c>
-      <c r="AD7" s="32" t="s">
+      <c r="AD7" s="33" t="s">
         <v>604</v>
       </c>
-      <c r="AE7" s="32" t="s">
+      <c r="AE7" s="33" t="s">
         <v>605</v>
       </c>
-      <c r="AF7" s="32" t="s">
+      <c r="AF7" s="33" t="s">
         <v>606</v>
       </c>
-      <c r="AG7" s="32" t="s">
+      <c r="AG7" s="33" t="s">
         <v>607</v>
       </c>
-      <c r="AH7" s="32" t="s">
+      <c r="AH7" s="33" t="s">
         <v>607</v>
       </c>
-      <c r="AI7" s="32" t="s">
+      <c r="AI7" s="33" t="s">
         <v>608</v>
       </c>
-      <c r="AJ7" s="32" t="s">
+      <c r="AJ7" s="33" t="s">
         <v>609</v>
       </c>
       <c r="AK7" t="s">
@@ -41775,16 +41778,16 @@
       <c r="C8" t="s">
         <v>622</v>
       </c>
-      <c r="D8" s="16" t="s">
+      <c r="D8" s="17" t="s">
         <v>475</v>
       </c>
-      <c r="E8" s="16" t="s">
+      <c r="E8" s="17" t="s">
         <v>623</v>
       </c>
-      <c r="F8" s="16" t="s">
+      <c r="F8" s="17" t="s">
         <v>624</v>
       </c>
-      <c r="G8" s="16" t="s">
+      <c r="G8" s="17" t="s">
         <v>623</v>
       </c>
       <c r="H8" t="s">
@@ -41805,61 +41808,61 @@
       <c r="O8" t="s">
         <v>590</v>
       </c>
-      <c r="P8" s="32" t="s">
+      <c r="P8" s="33" t="s">
         <v>627</v>
       </c>
-      <c r="Q8" s="32" t="s">
+      <c r="Q8" s="33" t="s">
         <v>628</v>
       </c>
-      <c r="R8" s="32" t="s">
+      <c r="R8" s="33" t="s">
         <v>629</v>
       </c>
-      <c r="S8" s="32" t="s">
+      <c r="S8" s="33" t="s">
         <v>630</v>
       </c>
-      <c r="T8" s="32" t="s">
+      <c r="T8" s="33" t="s">
         <v>631</v>
       </c>
-      <c r="U8" s="32" t="s">
+      <c r="U8" s="33" t="s">
         <v>632</v>
       </c>
-      <c r="V8" s="32" t="s">
+      <c r="V8" s="33" t="s">
         <v>633</v>
       </c>
-      <c r="W8" s="32" t="s">
+      <c r="W8" s="33" t="s">
         <v>634</v>
       </c>
-      <c r="X8" s="32" t="s">
+      <c r="X8" s="33" t="s">
         <v>600</v>
       </c>
-      <c r="AA8" s="32" t="s">
+      <c r="AA8" s="33" t="s">
         <v>601</v>
       </c>
-      <c r="AB8" s="32" t="s">
+      <c r="AB8" s="33" t="s">
         <v>602</v>
       </c>
-      <c r="AC8" s="32" t="s">
+      <c r="AC8" s="33" t="s">
         <v>603</v>
       </c>
-      <c r="AD8" s="32" t="s">
+      <c r="AD8" s="33" t="s">
         <v>604</v>
       </c>
-      <c r="AE8" s="32" t="s">
+      <c r="AE8" s="33" t="s">
         <v>605</v>
       </c>
-      <c r="AF8" s="32" t="s">
+      <c r="AF8" s="33" t="s">
         <v>606</v>
       </c>
-      <c r="AG8" s="32" t="s">
+      <c r="AG8" s="33" t="s">
         <v>607</v>
       </c>
-      <c r="AH8" s="32" t="s">
+      <c r="AH8" s="33" t="s">
         <v>635</v>
       </c>
-      <c r="AI8" s="32" t="s">
+      <c r="AI8" s="33" t="s">
         <v>636</v>
       </c>
-      <c r="AJ8" s="32" t="s">
+      <c r="AJ8" s="33" t="s">
         <v>637</v>
       </c>
       <c r="AK8" t="s">
@@ -41876,16 +41879,16 @@
       <c r="C9" t="s">
         <v>622</v>
       </c>
-      <c r="D9" s="16" t="s">
+      <c r="D9" s="17" t="s">
         <v>489</v>
       </c>
-      <c r="E9" s="16" t="s">
+      <c r="E9" s="17" t="s">
         <v>639</v>
       </c>
-      <c r="F9" s="16" t="s">
+      <c r="F9" s="17" t="s">
         <v>640</v>
       </c>
-      <c r="G9" s="16" t="s">
+      <c r="G9" s="17" t="s">
         <v>639</v>
       </c>
       <c r="H9" t="s">
@@ -41912,7 +41915,7 @@
       <c r="Q9" t="s">
         <v>645</v>
       </c>
-      <c r="R9" s="32" t="s">
+      <c r="R9" s="33" t="s">
         <v>646</v>
       </c>
       <c r="S9" t="s">
@@ -41933,22 +41936,22 @@
       <c r="X9" t="s">
         <v>650</v>
       </c>
-      <c r="AA9" s="32" t="s">
+      <c r="AA9" s="33" t="s">
         <v>601</v>
       </c>
-      <c r="AB9" s="32" t="s">
+      <c r="AB9" s="33" t="s">
         <v>602</v>
       </c>
-      <c r="AC9" s="32" t="s">
+      <c r="AC9" s="33" t="s">
         <v>603</v>
       </c>
-      <c r="AD9" s="32" t="s">
+      <c r="AD9" s="33" t="s">
         <v>604</v>
       </c>
-      <c r="AE9" s="32" t="s">
+      <c r="AE9" s="33" t="s">
         <v>605</v>
       </c>
-      <c r="AF9" s="32" t="s">
+      <c r="AF9" s="33" t="s">
         <v>606</v>
       </c>
       <c r="AG9" t="s">
@@ -41966,7 +41969,7 @@
       <c r="AK9" t="s">
         <v>655</v>
       </c>
-      <c r="AR9" s="32" t="s">
+      <c r="AR9" s="33" t="s">
         <v>656</v>
       </c>
     </row>
@@ -41980,16 +41983,16 @@
       <c r="C10" t="s">
         <v>622</v>
       </c>
-      <c r="D10" s="16" t="s">
+      <c r="D10" s="17" t="s">
         <v>504</v>
       </c>
-      <c r="E10" s="16">
+      <c r="E10" s="17">
         <v>565656</v>
       </c>
-      <c r="F10" s="16" t="s">
+      <c r="F10" s="17" t="s">
         <v>657</v>
       </c>
-      <c r="G10" s="16" t="s">
+      <c r="G10" s="17" t="s">
         <v>504</v>
       </c>
       <c r="H10" t="s">
@@ -42010,61 +42013,61 @@
       <c r="O10" t="s">
         <v>660</v>
       </c>
-      <c r="P10" s="32" t="s">
+      <c r="P10" s="33" t="s">
         <v>661</v>
       </c>
-      <c r="Q10" s="32" t="s">
+      <c r="Q10" s="33" t="s">
         <v>662</v>
       </c>
-      <c r="R10" s="32" t="s">
+      <c r="R10" s="33" t="s">
         <v>607</v>
       </c>
       <c r="S10" t="s">
         <v>630</v>
       </c>
-      <c r="T10" s="32" t="s">
+      <c r="T10" s="33" t="s">
         <v>631</v>
       </c>
-      <c r="U10" s="32" t="s">
+      <c r="U10" s="33" t="s">
         <v>633</v>
       </c>
-      <c r="V10" s="32" t="s">
+      <c r="V10" s="33" t="s">
         <v>663</v>
       </c>
-      <c r="W10" s="32" t="s">
+      <c r="W10" s="33" t="s">
         <v>600</v>
       </c>
-      <c r="X10" s="32" t="s">
+      <c r="X10" s="33" t="s">
         <v>650</v>
       </c>
-      <c r="AA10" s="32" t="s">
+      <c r="AA10" s="33" t="s">
         <v>601</v>
       </c>
-      <c r="AB10" s="32" t="s">
+      <c r="AB10" s="33" t="s">
         <v>602</v>
       </c>
-      <c r="AC10" s="32" t="s">
+      <c r="AC10" s="33" t="s">
         <v>603</v>
       </c>
-      <c r="AD10" s="32" t="s">
+      <c r="AD10" s="33" t="s">
         <v>604</v>
       </c>
-      <c r="AE10" s="32" t="s">
+      <c r="AE10" s="33" t="s">
         <v>605</v>
       </c>
-      <c r="AF10" s="32" t="s">
+      <c r="AF10" s="33" t="s">
         <v>607</v>
       </c>
-      <c r="AG10" s="32" t="s">
+      <c r="AG10" s="33" t="s">
         <v>607</v>
       </c>
-      <c r="AH10" s="32" t="s">
+      <c r="AH10" s="33" t="s">
         <v>607</v>
       </c>
-      <c r="AI10" s="32" t="s">
+      <c r="AI10" s="33" t="s">
         <v>607</v>
       </c>
-      <c r="AJ10" s="32" t="s">
+      <c r="AJ10" s="33" t="s">
         <v>607</v>
       </c>
       <c r="AK10" t="s">
@@ -42084,16 +42087,16 @@
       <c r="C11" t="s">
         <v>622</v>
       </c>
-      <c r="D11" s="16" t="s">
+      <c r="D11" s="17" t="s">
         <v>507</v>
       </c>
-      <c r="E11" s="16" t="s">
+      <c r="E11" s="17" t="s">
         <v>666</v>
       </c>
-      <c r="F11" s="16" t="s">
+      <c r="F11" s="17" t="s">
         <v>667</v>
       </c>
-      <c r="G11" s="16" t="s">
+      <c r="G11" s="17" t="s">
         <v>666</v>
       </c>
       <c r="H11" t="s">
@@ -42117,64 +42120,64 @@
       <c r="O11" t="s">
         <v>671</v>
       </c>
-      <c r="P11" s="32" t="s">
+      <c r="P11" s="33" t="s">
         <v>672</v>
       </c>
-      <c r="Q11" s="18" t="s">
+      <c r="Q11" s="20" t="s">
         <v>673</v>
       </c>
-      <c r="R11" s="33" t="s">
+      <c r="R11" s="34" t="s">
         <v>674</v>
       </c>
-      <c r="S11" s="32" t="s">
+      <c r="S11" s="33" t="s">
         <v>647</v>
       </c>
-      <c r="T11" s="32" t="s">
+      <c r="T11" s="33" t="s">
         <v>675</v>
       </c>
-      <c r="U11" s="32" t="s">
+      <c r="U11" s="33" t="s">
         <v>633</v>
       </c>
-      <c r="V11" s="32" t="s">
+      <c r="V11" s="33" t="s">
         <v>634</v>
       </c>
-      <c r="W11" s="32" t="s">
+      <c r="W11" s="33" t="s">
         <v>676</v>
       </c>
-      <c r="X11" s="32" t="s">
+      <c r="X11" s="33" t="s">
         <v>600</v>
       </c>
-      <c r="Y11" s="32" t="s">
+      <c r="Y11" s="33" t="s">
         <v>650</v>
       </c>
-      <c r="AA11" s="32" t="s">
+      <c r="AA11" s="33" t="s">
         <v>601</v>
       </c>
-      <c r="AB11" s="32" t="s">
+      <c r="AB11" s="33" t="s">
         <v>602</v>
       </c>
-      <c r="AC11" s="32" t="s">
+      <c r="AC11" s="33" t="s">
         <v>603</v>
       </c>
-      <c r="AD11" s="32" t="s">
+      <c r="AD11" s="33" t="s">
         <v>604</v>
       </c>
-      <c r="AE11" s="32" t="s">
+      <c r="AE11" s="33" t="s">
         <v>605</v>
       </c>
-      <c r="AF11" s="32" t="s">
+      <c r="AF11" s="33" t="s">
         <v>677</v>
       </c>
-      <c r="AG11" s="32" t="s">
+      <c r="AG11" s="33" t="s">
         <v>678</v>
       </c>
-      <c r="AH11" s="32" t="s">
+      <c r="AH11" s="33" t="s">
         <v>679</v>
       </c>
-      <c r="AI11" s="32" t="s">
+      <c r="AI11" s="33" t="s">
         <v>680</v>
       </c>
-      <c r="AJ11" s="32" t="s">
+      <c r="AJ11" s="33" t="s">
         <v>654</v>
       </c>
       <c r="AK11" t="s">
@@ -42191,16 +42194,16 @@
       <c r="C12" t="s">
         <v>622</v>
       </c>
-      <c r="D12" s="16" t="s">
+      <c r="D12" s="17" t="s">
         <v>512</v>
       </c>
-      <c r="E12" s="16" t="s">
+      <c r="E12" s="17" t="s">
         <v>682</v>
       </c>
-      <c r="F12" s="16" t="s">
+      <c r="F12" s="17" t="s">
         <v>683</v>
       </c>
-      <c r="G12" s="16" t="s">
+      <c r="G12" s="17" t="s">
         <v>682</v>
       </c>
       <c r="H12" t="s">
@@ -42221,61 +42224,61 @@
       <c r="O12" t="s">
         <v>686</v>
       </c>
-      <c r="P12" s="32" t="s">
+      <c r="P12" s="33" t="s">
         <v>687</v>
       </c>
-      <c r="Q12" s="18" t="s">
+      <c r="Q12" s="20" t="s">
         <v>688</v>
       </c>
-      <c r="R12" s="33" t="s">
+      <c r="R12" s="34" t="s">
         <v>689</v>
       </c>
-      <c r="S12" s="32" t="s">
+      <c r="S12" s="33" t="s">
         <v>631</v>
       </c>
-      <c r="T12" s="32" t="s">
+      <c r="T12" s="33" t="s">
         <v>690</v>
       </c>
-      <c r="U12" s="32" t="s">
+      <c r="U12" s="33" t="s">
         <v>648</v>
       </c>
-      <c r="V12" s="32" t="s">
+      <c r="V12" s="33" t="s">
         <v>649</v>
       </c>
-      <c r="W12" s="32" t="s">
+      <c r="W12" s="33" t="s">
         <v>600</v>
       </c>
-      <c r="X12" s="32" t="s">
+      <c r="X12" s="33" t="s">
         <v>650</v>
       </c>
-      <c r="AA12" s="32" t="s">
+      <c r="AA12" s="33" t="s">
         <v>601</v>
       </c>
-      <c r="AB12" s="32" t="s">
+      <c r="AB12" s="33" t="s">
         <v>602</v>
       </c>
-      <c r="AC12" s="32" t="s">
+      <c r="AC12" s="33" t="s">
         <v>603</v>
       </c>
-      <c r="AD12" s="32" t="s">
+      <c r="AD12" s="33" t="s">
         <v>604</v>
       </c>
-      <c r="AE12" s="32" t="s">
+      <c r="AE12" s="33" t="s">
         <v>605</v>
       </c>
-      <c r="AF12" s="32" t="s">
+      <c r="AF12" s="33" t="s">
         <v>606</v>
       </c>
-      <c r="AG12" s="32" t="s">
+      <c r="AG12" s="33" t="s">
         <v>691</v>
       </c>
-      <c r="AH12" s="32" t="s">
+      <c r="AH12" s="33" t="s">
         <v>692</v>
       </c>
-      <c r="AI12" s="32" t="s">
+      <c r="AI12" s="33" t="s">
         <v>693</v>
       </c>
-      <c r="AJ12" s="32" t="s">
+      <c r="AJ12" s="33" t="s">
         <v>694</v>
       </c>
       <c r="AK12" t="s">
@@ -42295,16 +42298,16 @@
       <c r="C13" t="s">
         <v>622</v>
       </c>
-      <c r="D13" s="16" t="s">
+      <c r="D13" s="17" t="s">
         <v>525</v>
       </c>
-      <c r="E13" s="16">
+      <c r="E13" s="17">
         <v>790200</v>
       </c>
-      <c r="F13" s="16" t="s">
+      <c r="F13" s="17" t="s">
         <v>697</v>
       </c>
-      <c r="G13" s="16">
+      <c r="G13" s="17">
         <v>790200</v>
       </c>
       <c r="H13" t="s">
@@ -42325,58 +42328,58 @@
       <c r="O13" t="s">
         <v>700</v>
       </c>
-      <c r="P13" s="32" t="s">
+      <c r="P13" s="33" t="s">
         <v>701</v>
       </c>
-      <c r="Q13" s="18" t="s">
+      <c r="Q13" s="20" t="s">
         <v>187</v>
       </c>
-      <c r="R13" s="32" t="s">
+      <c r="R13" s="33" t="s">
         <v>702</v>
       </c>
-      <c r="S13" s="32" t="s">
+      <c r="S13" s="33" t="s">
         <v>703</v>
       </c>
-      <c r="T13" s="32" t="s">
+      <c r="T13" s="33" t="s">
         <v>675</v>
       </c>
-      <c r="U13" s="32" t="s">
+      <c r="U13" s="33" t="s">
         <v>633</v>
       </c>
-      <c r="V13" s="32" t="s">
+      <c r="V13" s="33" t="s">
         <v>704</v>
       </c>
-      <c r="W13" s="32" t="s">
+      <c r="W13" s="33" t="s">
         <v>600</v>
       </c>
-      <c r="AA13" s="32" t="s">
+      <c r="AA13" s="33" t="s">
         <v>601</v>
       </c>
-      <c r="AB13" s="32" t="s">
+      <c r="AB13" s="33" t="s">
         <v>602</v>
       </c>
-      <c r="AC13" s="32" t="s">
+      <c r="AC13" s="33" t="s">
         <v>603</v>
       </c>
-      <c r="AD13" s="32" t="s">
+      <c r="AD13" s="33" t="s">
         <v>604</v>
       </c>
-      <c r="AE13" s="32" t="s">
+      <c r="AE13" s="33" t="s">
         <v>605</v>
       </c>
-      <c r="AF13" s="32" t="s">
+      <c r="AF13" s="33" t="s">
         <v>606</v>
       </c>
-      <c r="AG13" s="32" t="s">
+      <c r="AG13" s="33" t="s">
         <v>705</v>
       </c>
-      <c r="AH13" s="32" t="s">
+      <c r="AH13" s="33" t="s">
         <v>706</v>
       </c>
-      <c r="AI13" s="32" t="s">
+      <c r="AI13" s="33" t="s">
         <v>707</v>
       </c>
-      <c r="AJ13" s="32" t="s">
+      <c r="AJ13" s="33" t="s">
         <v>694</v>
       </c>
       <c r="AK13" t="s">
@@ -42596,19 +42599,19 @@
       <c r="K2" t="s">
         <v>734</v>
       </c>
-      <c r="M2" s="32" t="s">
+      <c r="M2" s="33" t="s">
         <v>735</v>
       </c>
-      <c r="N2" s="32" t="s">
+      <c r="N2" s="33" t="s">
         <v>735</v>
       </c>
-      <c r="O2" s="32" t="s">
+      <c r="O2" s="33" t="s">
         <v>735</v>
       </c>
-      <c r="P2" s="32" t="s">
+      <c r="P2" s="33" t="s">
         <v>735</v>
       </c>
-      <c r="Q2" s="32" t="s">
+      <c r="Q2" s="33" t="s">
         <v>736</v>
       </c>
     </row>
@@ -42640,16 +42643,16 @@
       <c r="J3" t="s">
         <v>738</v>
       </c>
-      <c r="M3" s="32" t="s">
+      <c r="M3" s="33" t="s">
         <v>739</v>
       </c>
-      <c r="N3" s="32" t="s">
+      <c r="N3" s="33" t="s">
         <v>739</v>
       </c>
-      <c r="O3" s="32" t="s">
+      <c r="O3" s="33" t="s">
         <v>739</v>
       </c>
-      <c r="P3" s="32" t="s">
+      <c r="P3" s="33" t="s">
         <v>739</v>
       </c>
       <c r="T3" t="s">
@@ -42702,7 +42705,7 @@
       <c r="O4" t="s">
         <v>745</v>
       </c>
-      <c r="P4" s="32" t="s">
+      <c r="P4" s="33" t="s">
         <v>739</v>
       </c>
       <c r="T4" t="s">
@@ -42758,10 +42761,10 @@
       <c r="P5">
         <v>1</v>
       </c>
-      <c r="Q5" s="32" t="s">
+      <c r="Q5" s="33" t="s">
         <v>736</v>
       </c>
-      <c r="R5" s="32" t="s">
+      <c r="R5" s="33" t="s">
         <v>750</v>
       </c>
       <c r="T5" t="s">
@@ -42817,7 +42820,7 @@
       <c r="O6">
         <v>2</v>
       </c>
-      <c r="Q6" s="32" t="s">
+      <c r="Q6" s="33" t="s">
         <v>755</v>
       </c>
       <c r="T6" t="s">
@@ -42858,10 +42861,10 @@
       <c r="J7" t="s">
         <v>757</v>
       </c>
-      <c r="Q7" s="32" t="s">
+      <c r="Q7" s="33" t="s">
         <v>758</v>
       </c>
-      <c r="R7" s="32" t="s">
+      <c r="R7" s="33" t="s">
         <v>759</v>
       </c>
       <c r="T7" t="s">
@@ -42964,7 +42967,7 @@
       <c r="N9" t="s">
         <v>754</v>
       </c>
-      <c r="O9" s="32" t="s">
+      <c r="O9" s="33" t="s">
         <v>739</v>
       </c>
       <c r="T9" t="s">
@@ -43055,7 +43058,7 @@
       <c r="L11" t="s">
         <v>772</v>
       </c>
-      <c r="Q11" s="32" t="s">
+      <c r="Q11" s="33" t="s">
         <v>773</v>
       </c>
       <c r="T11" t="s">
@@ -43111,7 +43114,7 @@
       <c r="M12">
         <v>8</v>
       </c>
-      <c r="N12" s="32" t="s">
+      <c r="N12" s="33" t="s">
         <v>777</v>
       </c>
       <c r="O12">
@@ -43120,10 +43123,10 @@
       <c r="P12">
         <v>3</v>
       </c>
-      <c r="Q12" s="32" t="s">
+      <c r="Q12" s="33" t="s">
         <v>736</v>
       </c>
-      <c r="R12" s="32" t="s">
+      <c r="R12" s="33" t="s">
         <v>778</v>
       </c>
     </row>
@@ -43167,7 +43170,7 @@
       <c r="M13">
         <v>8</v>
       </c>
-      <c r="N13" s="32" t="s">
+      <c r="N13" s="33" t="s">
         <v>782</v>
       </c>
       <c r="O13">
@@ -43176,7 +43179,7 @@
       <c r="P13">
         <v>4</v>
       </c>
-      <c r="Q13" s="32" t="s">
+      <c r="Q13" s="33" t="s">
         <v>736</v>
       </c>
     </row>
@@ -43220,7 +43223,7 @@
       <c r="N14" t="s">
         <v>744</v>
       </c>
-      <c r="O14" s="32" t="s">
+      <c r="O14" s="33" t="s">
         <v>739</v>
       </c>
       <c r="T14" t="s">
@@ -43273,7 +43276,7 @@
       <c r="M15">
         <v>8</v>
       </c>
-      <c r="N15" s="32" t="s">
+      <c r="N15" s="33" t="s">
         <v>777</v>
       </c>
       <c r="O15">
@@ -43282,7 +43285,7 @@
       <c r="P15">
         <v>3</v>
       </c>
-      <c r="Q15" s="32" t="s">
+      <c r="Q15" s="33" t="s">
         <v>736</v>
       </c>
     </row>
@@ -43323,7 +43326,7 @@
       <c r="L16" t="s">
         <v>790</v>
       </c>
-      <c r="Q16" s="32" t="s">
+      <c r="Q16" s="33" t="s">
         <v>791</v>
       </c>
       <c r="T16" t="s">
@@ -43379,7 +43382,7 @@
       <c r="M17">
         <v>8</v>
       </c>
-      <c r="N17" s="32" t="s">
+      <c r="N17" s="33" t="s">
         <v>782</v>
       </c>
       <c r="O17">
@@ -43388,10 +43391,10 @@
       <c r="P17">
         <v>4</v>
       </c>
-      <c r="Q17" s="32" t="s">
+      <c r="Q17" s="33" t="s">
         <v>736</v>
       </c>
-      <c r="R17" s="32" t="s">
+      <c r="R17" s="33" t="s">
         <v>795</v>
       </c>
     </row>
@@ -43435,7 +43438,7 @@
       <c r="M18">
         <v>1</v>
       </c>
-      <c r="N18" s="32" t="s">
+      <c r="N18" s="33" t="s">
         <v>799</v>
       </c>
       <c r="O18">
@@ -43444,7 +43447,7 @@
       <c r="P18">
         <v>8</v>
       </c>
-      <c r="Q18" s="32" t="s">
+      <c r="Q18" s="33" t="s">
         <v>736</v>
       </c>
     </row>
@@ -43494,7 +43497,7 @@
       <c r="P19">
         <v>1</v>
       </c>
-      <c r="Q19" s="32" t="s">
+      <c r="Q19" s="33" t="s">
         <v>755</v>
       </c>
       <c r="T19" t="s">
@@ -43550,7 +43553,7 @@
       <c r="M20">
         <v>8</v>
       </c>
-      <c r="N20" s="32" t="s">
+      <c r="N20" s="33" t="s">
         <v>777</v>
       </c>
       <c r="O20">
@@ -43559,7 +43562,7 @@
       <c r="P20">
         <v>3</v>
       </c>
-      <c r="Q20" s="32" t="s">
+      <c r="Q20" s="33" t="s">
         <v>736</v>
       </c>
     </row>
@@ -43612,10 +43615,10 @@
       <c r="P21">
         <v>1</v>
       </c>
-      <c r="Q21" s="32" t="s">
+      <c r="Q21" s="33" t="s">
         <v>736</v>
       </c>
-      <c r="R21" s="32" t="s">
+      <c r="R21" s="33" t="s">
         <v>750</v>
       </c>
       <c r="T21" t="s">
@@ -43671,7 +43674,7 @@
       <c r="L22" t="s">
         <v>810</v>
       </c>
-      <c r="Q22" s="32" t="s">
+      <c r="Q22" s="33" t="s">
         <v>791</v>
       </c>
       <c r="T22" t="s">
@@ -43721,28 +43724,28 @@
       <c r="K29" t="s">
         <v>734</v>
       </c>
-      <c r="M29" s="32" t="s">
+      <c r="M29" s="33" t="s">
         <v>735</v>
       </c>
-      <c r="N29" s="32" t="s">
+      <c r="N29" s="33" t="s">
         <v>735</v>
       </c>
-      <c r="O29" s="32" t="s">
+      <c r="O29" s="33" t="s">
         <v>735</v>
       </c>
-      <c r="P29" s="32" t="s">
+      <c r="P29" s="33" t="s">
         <v>735</v>
       </c>
-      <c r="Q29" s="32" t="s">
+      <c r="Q29" s="33" t="s">
         <v>736</v>
       </c>
-      <c r="X29" s="32" t="s">
+      <c r="X29" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="Y29" s="32" t="s">
+      <c r="Y29" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="Z29" s="32" t="s">
+      <c r="Z29" s="33" t="s">
         <v>584</v>
       </c>
       <c r="AA29" t="s">
@@ -43757,13 +43760,13 @@
       <c r="AD29" t="s">
         <v>584</v>
       </c>
-      <c r="AE29" s="32" t="s">
+      <c r="AE29" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="AF29" s="32" t="s">
+      <c r="AF29" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="AG29" s="32" t="s">
+      <c r="AG29" s="33" t="s">
         <v>584</v>
       </c>
     </row>
@@ -43804,16 +43807,16 @@
       <c r="L30" t="s">
         <v>813</v>
       </c>
-      <c r="M30" s="32" t="s">
+      <c r="M30" s="33" t="s">
         <v>739</v>
       </c>
-      <c r="N30" s="32" t="s">
+      <c r="N30" s="33" t="s">
         <v>739</v>
       </c>
-      <c r="O30" s="32" t="s">
+      <c r="O30" s="33" t="s">
         <v>739</v>
       </c>
-      <c r="P30" s="32" t="s">
+      <c r="P30" s="33" t="s">
         <v>739</v>
       </c>
       <c r="T30" t="s">
@@ -43828,13 +43831,13 @@
       <c r="W30" t="s">
         <v>741</v>
       </c>
-      <c r="X30" s="32" t="s">
+      <c r="X30" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="Y30" s="32" t="s">
+      <c r="Y30" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="Z30" s="32" t="s">
+      <c r="Z30" s="33" t="s">
         <v>584</v>
       </c>
       <c r="AA30" t="s">
@@ -43846,16 +43849,16 @@
       <c r="AC30" t="s">
         <v>584</v>
       </c>
-      <c r="AD30" s="32" t="s">
+      <c r="AD30" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="AE30" s="32" t="s">
+      <c r="AE30" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="AF30" s="32" t="s">
+      <c r="AF30" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="AG30" s="32" t="s">
+      <c r="AG30" s="33" t="s">
         <v>584</v>
       </c>
     </row>
@@ -43905,7 +43908,7 @@
       <c r="O31" t="s">
         <v>745</v>
       </c>
-      <c r="P31" s="32" t="s">
+      <c r="P31" s="33" t="s">
         <v>739</v>
       </c>
       <c r="T31" t="s">
@@ -43917,13 +43920,13 @@
       <c r="V31" t="s">
         <v>746</v>
       </c>
-      <c r="X31" s="32" t="s">
+      <c r="X31" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="Y31" s="32" t="s">
+      <c r="Y31" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="Z31" s="32" t="s">
+      <c r="Z31" s="33" t="s">
         <v>584</v>
       </c>
       <c r="AA31" t="s">
@@ -43935,16 +43938,16 @@
       <c r="AC31" t="s">
         <v>584</v>
       </c>
-      <c r="AD31" s="32" t="s">
+      <c r="AD31" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="AE31" s="32" t="s">
+      <c r="AE31" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="AF31" s="32" t="s">
+      <c r="AF31" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="AG31" s="32" t="s">
+      <c r="AG31" s="33" t="s">
         <v>584</v>
       </c>
       <c r="AH31">
@@ -44000,10 +44003,10 @@
       <c r="P32">
         <v>1</v>
       </c>
-      <c r="Q32" s="32" t="s">
+      <c r="Q32" s="33" t="s">
         <v>736</v>
       </c>
-      <c r="R32" s="32" t="s">
+      <c r="R32" s="33" t="s">
         <v>750</v>
       </c>
       <c r="T32" t="s">
@@ -44015,13 +44018,13 @@
       <c r="V32" t="s">
         <v>751</v>
       </c>
-      <c r="X32" s="32" t="s">
+      <c r="X32" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="Y32" s="32" t="s">
+      <c r="Y32" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="Z32" s="32" t="s">
+      <c r="Z32" s="33" t="s">
         <v>584</v>
       </c>
       <c r="AA32" t="s">
@@ -44033,16 +44036,16 @@
       <c r="AC32" t="s">
         <v>584</v>
       </c>
-      <c r="AD32" s="32" t="s">
+      <c r="AD32" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="AE32" s="32" t="s">
+      <c r="AE32" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="AF32" s="32" t="s">
+      <c r="AF32" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="AG32" s="32" t="s">
+      <c r="AG32" s="33" t="s">
         <v>584</v>
       </c>
       <c r="AH32">
@@ -44098,7 +44101,7 @@
       <c r="O33">
         <v>2</v>
       </c>
-      <c r="Q33" s="32" t="s">
+      <c r="Q33" s="33" t="s">
         <v>755</v>
       </c>
       <c r="T33" t="s">
@@ -44107,7 +44110,7 @@
       <c r="U33" t="s">
         <v>740</v>
       </c>
-      <c r="X33" s="32" t="s">
+      <c r="X33" s="33" t="s">
         <v>584</v>
       </c>
       <c r="Y33" t="s">
@@ -44128,13 +44131,13 @@
       <c r="AD33" t="s">
         <v>584</v>
       </c>
-      <c r="AE33" s="32" t="s">
+      <c r="AE33" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="AF33" s="32" t="s">
+      <c r="AF33" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="AG33" s="32" t="s">
+      <c r="AG33" s="33" t="s">
         <v>584</v>
       </c>
       <c r="AI33">
@@ -44178,10 +44181,10 @@
       <c r="L34" t="s">
         <v>813</v>
       </c>
-      <c r="Q34" s="32" t="s">
+      <c r="Q34" s="33" t="s">
         <v>758</v>
       </c>
-      <c r="R34" s="32" t="s">
+      <c r="R34" s="33" t="s">
         <v>759</v>
       </c>
       <c r="T34" t="s">
@@ -44211,10 +44214,10 @@
       <c r="AD34" t="s">
         <v>584</v>
       </c>
-      <c r="AE34" s="32" t="s">
+      <c r="AE34" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="AF34" s="32" t="s">
+      <c r="AF34" s="33" t="s">
         <v>584</v>
       </c>
       <c r="AG34" t="s">
@@ -44273,10 +44276,10 @@
       <c r="P35">
         <v>12</v>
       </c>
-      <c r="Q35" s="32" t="s">
+      <c r="Q35" s="33" t="s">
         <v>758</v>
       </c>
-      <c r="R35" s="32" t="s">
+      <c r="R35" s="33" t="s">
         <v>759</v>
       </c>
       <c r="T35" t="s">
@@ -44306,10 +44309,10 @@
       <c r="AD35" t="s">
         <v>584</v>
       </c>
-      <c r="AE35" s="32" t="s">
+      <c r="AE35" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="AF35" s="32" t="s">
+      <c r="AF35" s="33" t="s">
         <v>584</v>
       </c>
       <c r="AG35" t="s">
@@ -44398,7 +44401,7 @@
       <c r="AD36" t="s">
         <v>584</v>
       </c>
-      <c r="AE36" s="32" t="s">
+      <c r="AE36" s="33" t="s">
         <v>584</v>
       </c>
       <c r="AF36" t="s">
@@ -44457,7 +44460,7 @@
       <c r="N37" t="s">
         <v>754</v>
       </c>
-      <c r="O37" s="32" t="s">
+      <c r="O37" s="33" t="s">
         <v>739</v>
       </c>
       <c r="T37" t="s">
@@ -44487,7 +44490,7 @@
       <c r="AD37" t="s">
         <v>584</v>
       </c>
-      <c r="AE37" s="32" t="s">
+      <c r="AE37" s="33" t="s">
         <v>584</v>
       </c>
       <c r="AF37" t="s">
@@ -44570,10 +44573,10 @@
       <c r="AD38" t="s">
         <v>584</v>
       </c>
-      <c r="AE38" s="32" t="s">
+      <c r="AE38" s="33" t="s">
         <v>584</v>
       </c>
-      <c r="AF38" s="32" t="s">
+      <c r="AF38" s="33" t="s">
         <v>584</v>
       </c>
       <c r="AG38" t="s">
@@ -44623,7 +44626,7 @@
       <c r="L39" t="s">
         <v>813</v>
       </c>
-      <c r="Q39" s="32" t="s">
+      <c r="Q39" s="33" t="s">
         <v>773</v>
       </c>
       <c r="T39" t="s">
@@ -44653,7 +44656,7 @@
       <c r="AD39" t="s">
         <v>584</v>
       </c>
-      <c r="AE39" s="32" t="s">
+      <c r="AE39" s="33" t="s">
         <v>584</v>
       </c>
       <c r="AF39" t="s">
@@ -44739,7 +44742,7 @@
       <c r="AD40" t="s">
         <v>584</v>
       </c>
-      <c r="AE40" s="32" t="s">
+      <c r="AE40" s="33" t="s">
         <v>584</v>
       </c>
       <c r="AF40" t="s">

</xml_diff>

<commit_message>
add Promissory note req img
</commit_message>
<xml_diff>
--- a/Template_Data.xlsx
+++ b/Template_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12165" tabRatio="796" firstSheet="6" activeTab="14"/>
+    <workbookView windowWidth="14400" windowHeight="12975" tabRatio="796" activeTab="14"/>
   </bookViews>
   <sheets>
     <sheet name="Actions" sheetId="14" r:id="rId1"/>
@@ -6650,7 +6650,7 @@
     <t>&lt;fs=60&gt;    Ключи    &lt;br&gt;Шифрования&lt;/fs&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=75&gt;&lt;fs=50&gt;&lt;f=Myriad Pro&gt;ДЕЙСТВИЕ: &lt;/f&gt;прикрепите эту карту к подконтрольной вам неродной планете.&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Эта планета имеет технологическую специализацию любого цвета.&lt;/fs&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=75&gt;&lt;fs=50&gt;&lt;f=Myriad Pro&gt;ДЕЙСТВИЕ: &lt;/f&gt;прикрепите эту карту к подконтрольной вам неродной планете.&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Эта планета имеет техно-&lt;br&gt;логическую специализа-&lt;br&gt;цию любого цвета.&lt;/fs&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>1.8745;0;0;0;0;0;1.8196;0;0;0;0;0;0.3843;0;0;0;0;0;1;0;-0.8745;-0.8196;0.6157;0;1</t>
@@ -6665,7 +6665,7 @@
     <t>&lt;fs=60&gt;Торговый альянс&lt;/fs&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=56&gt;&lt;fs=37&gt;Когда вы получаете эту карту, если вы не играете за Келдарскую Торговую Конфедерацию, положите её перед собой лицевой стороной вверх.&lt;ls=44&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Пока эта карта лежит перед вами, вы можете использовать способность командира Келдарской Торговой Конфедерации, если она разблокирована.&lt;ls=44&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Если вы активировали систему, в которой есть хотя бы 1 отряд игрока Келдарской Торговой Конфедерации, верните эту карту обещания игроку, играющего за Келдарскую Торговую Конфедерацию.&lt;/fs&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=56&gt;&lt;fs=37&gt;Когда вы получаете эту карту, если вы не играете за Келдарскую Торго-&lt;br&gt;вую Конфедерацию, положите её пе-&lt;br&gt;ред собой лицевой стороной вверх.&lt;ls=44&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Пока эта карта лежит перед вами, вы можете использовать способность командира Келдарской Торговой Конфедерации, если она разблоки-&lt;br&gt;рована.&lt;ls=44&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Если вы активировали систему, в которой есть хотя бы 1 отряд игрока Келдарской Торговой Конфедера-&lt;br&gt;ции, верните эту карту обещания игроку, играющему за Келдарскую Торговую Конфедерацию.&lt;/fs&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>1.8667;0;0;0;0;0;1.098;0;0;0;0;0;0.4235;0;0;0;0;0;1;0;-0.8667;-0.098;0.5765;0;1</t>
@@ -6695,7 +6695,7 @@
     <t>&lt;fs=56&gt;Алгоритмическая Репликация&lt;/fs&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=75&gt;&lt;fs=50&gt;&lt;f=Myriad Pro&gt;ДЕЙСТВИЕ: &lt;/f&gt;выберите 1 карту действий из стопки сброса карт действий и добавьте её в свою руку.&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Затем изгоните эту карту.&lt;/fs&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=75&gt;&lt;fs=50&gt;&lt;f=Myriad Pro&gt;ДЕЙСТВИЕ: &lt;/f&gt;выберите 1 карту действий из стопки сброса карт действий и возьмите её себе в руку.&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Затем изгоните эту карту.&lt;/fs&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>1.1608;0;0;0;0;0;1.1608;0;0;0;0;0;1.1608;0;0;0;0;0;1;0;-0.1608;-0.1608;-0.1608;0;1</t>
@@ -6725,7 +6725,7 @@
     <t>&lt;fs=60&gt;Поправка Эдин&lt;/fs&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=69&gt;&lt;fs=46&gt;&lt;f=Myriad Pro&gt;После раскрытия карты политики:&lt;/f&gt;&lt;ls=55&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Вы не можете голосовать по этой карте политики. Предскажите вслух результат голосования по этой карте. Если ваше предсказание верно, разместите 1 жетон приказа из снабжения другого игрока в системе, в которой есть ваши отряды.&lt;ls=55&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Затем верните эту карту игроку, играющему&lt;br&gt;за Мандат Эдин.&lt;/fs&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=63&gt;&lt;fs=42&gt;&lt;f=Myriad Pro&gt;После раскрытия карты политики:&lt;/f&gt;&lt;ls=50&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Вы не можете голосовать по этой карте политики. Предскажите вслух результат голосования по этой карте. Если ваше предсказание верно, разместите 1 жетон приказа из снабжения другого игрока в системе, в которой есть ваши отряды.&lt;ls=50&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Затем верните эту карту&lt;br&gt;игроку, играющему за&lt;br&gt;Мандат Эдин.&lt;/fs&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>0.7373;0;0;0;0;0;0.9255;0;0;0;0;0;1.6;0;0;0;0;0;1;0;0.2627;0.0745;-0.6;0;1</t>
@@ -6797,7 +6797,7 @@
     <t>&lt;fs=60&gt;Действующая база «ПРГ»&lt;/fs&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=75&gt;&lt;fs=50&gt;&lt;f=Myriad Pro&gt;ДЕЙСТВИЕ: &lt;/f&gt;прикрепите эту карту к подконтрольной вам неродной планете.&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Значение ресурсов этой планеты увеличивается на 2.&lt;/fs&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=75&gt;&lt;fs=50&gt;&lt;f=Myriad Pro&gt;ДЕЙСТВИЕ: &lt;/f&gt;прикрепите эту карту к подконтрольной вам неродной планете.&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Значение ресурсов этой планеты увеличивается&lt;br&gt;на 2.&lt;/fs&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>0.298;0;0;0;0;0;0.8941;0;0;0;0;0;1.6941;0;0;0;0;0;1;0;0.702;0.1059;-0.6941;0;1</t>
@@ -6812,7 +6812,7 @@
     <t>&lt;fs=60&gt;Прорицание&lt;/fs&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=63&gt;&lt;fs=42&gt;&lt;f=Myriad Pro&gt;ДЕЙСТВИЕ: &lt;/f&gt;положите эту карту перед собой лицевой стороной вверх.&lt;ls=50&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Пока эта карта лежит перед вами, вы можете смотреть карту общей цели на планшете фракции игрока, играющего за Авгуров Иликсума.&lt;ls=50&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Если вы активируете систему, в которой есть хотя бы 1 отряд игрока, играющего за авгуров Иликсума, верните ему&lt;br&gt;эту карту.&lt;/fs&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=63&gt;&lt;fs=42&gt;&lt;f=Myriad Pro&gt;ДЕЙСТВИЕ: &lt;/f&gt;положите эту карту перед собой лицевой стороной вверх.&lt;ls=50&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Пока эта карта лежит перед вами, вы можете смотреть карту общей цели на планшете фракции игрока, играющего&lt;br&gt;за Авгуров Иликсума.&lt;ls=50&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Если вы активируете систему, в которой есть хотя бы 1 отряд игрока, играющего за авгуров Иликсума, верните ему&lt;br&gt;эту карту.&lt;/fs&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>0.5098;0;0;0;0;0;1.1451;0;0;0;0;0;0.4784;0;0;0;0;0;1;0;0.4902;-0.1451;0.5216;0;1</t>
@@ -6824,7 +6824,7 @@
     <t>&lt;fs=60&gt;Вассалитет&lt;/fs&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=69&gt;&lt;fs=46&gt;&lt;f=Myriad Pro&gt;В начале боя:&lt;/f&gt;&lt;ls=55&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Добавляйте +1 к результатам боевых проверок каждого вашего истребителя во время этого боя. Игрок, играющий за Берсерков Кьяленгарда, захватывает каждый ваш истребитель, уничтоженный во время этого боя.&lt;ls=55&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Затем верните эту карту игроку, играющему за Берсерков Кьяленгарда.&lt;/fs&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=69&gt;&lt;fs=46&gt;&lt;f=Myriad Pro&gt;В начале боя:&lt;/f&gt;&lt;ls=55&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Добавляйте +1 к результатам боевых проверок каждого вашего истребителя во время этого боя. Игрок, играющий за Берсерков Кьяленгарда, захватывает каждый ваш истребитель, уничтоженный во время этого боя.&lt;ls=55&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Затем верните эту карту игроку, играющему&lt;br&gt;за Берсерков&lt;br&gt;Кьяленгарда.&lt;/fs&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>1.5373;0;0;0;0;0;1.9294;0;0;0;0;0;0.1569;0;0;0;0;0;1;0;-0.5373;-0.9294;0.8431;0;1</t>
@@ -6878,7 +6878,7 @@
     <t>&lt;fs=60&gt;Поправка Кайро&lt;/fs&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=69&gt;&lt;fs=46&gt;&lt;f=Myriad Pro&gt;После раскрытия карты политики:&lt;/f&gt;&lt;ls=55&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Вы не можете голосовать по этой карте. Предскажите вслух результат голосования по ней. Если предсказание окажется верным, разместите 3 отряда пехоты из вашего снабжения на подконтрольной вам планете.&lt;ls=55&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Затем верните эту карту игроку, играющему&lt;br&gt;за Общину Кайро.&lt;/fs&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=69&gt;&lt;fs=46&gt;&lt;f=Myriad Pro&gt;После раскрытия карты политики:&lt;/f&gt;&lt;ls=55&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Вы не можете голосовать по этой карте. Предскажите вслух результат голосования по ней. Если предсказание окажется верным, размести-&lt;br&gt;те 3 отряда пехоты из вашего снабжения на подконтроль-&lt;br&gt;ной вам планете.&lt;ls=55&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Затем верните эту карту игроку, играющему&lt;br&gt;за Общину Кайро.&lt;/fs&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>1.7804;0;0;0;0;0;0.5725;0;0;0;0;0;1.0039;0;0;0;0;0;1;0;-0.7804;0.4275;-0.0039;0;1</t>
@@ -6893,7 +6893,7 @@
     <t>&lt;fs=60&gt;Трофеи войны&lt;/fs&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=75&gt;&lt;fs=50&gt;&lt;f=Myriad Pro&gt;После того как вы выиграли бой:&lt;/f&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Положите её перед собой лицевой стороной вверх, чтобы разведать 1 подконтрольную вам планету.&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;В начале хода игрока, играющего за Осколки Ланефир, верните ему&lt;br&gt;эту карту.&lt;/fs&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=75&gt;&lt;fs=50&gt;&lt;f=Myriad Pro&gt;После того как вы выиграли бой:&lt;/f&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Положите её перед собой лицевой стороной вверх, чтобы разведать 1 подкон-&lt;br&gt;трольную вам планету.&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;В начале хода игрока, играющего за Осколки Ланефир, верните ему&lt;br&gt;эту карту.&lt;/fs&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>1.6941;0;0;0;0;0;0.5255;0;0;0;0;0;1.4196;0;0;0;0;0;1;0;-0.6941;0.4745;-0.4196;0;1</t>
@@ -6923,7 +6923,7 @@
     <t>&lt;fs=60&gt;Глас камней&lt;/fs&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=63&gt;&lt;fs=42&gt;&lt;f=Myriad Pro&gt;Во время тактического действия, когда вы используете способность &lt;/f&gt;&lt;push=0;14&gt;&lt;f=Russo One;34;0;0;0;0&gt;«БОМБАРДИРОВКА»&lt;/f&gt;&lt;push=0;-14&gt;&lt;f=Myriad Pro&gt; и наносите хотя бы 1 попадание:&lt;/f&gt;&lt;ls=50&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;За каждое нанесённое вами попадание вы можете вместо этого разместить 1 отряд пехоты из вашего снабжения на планете, против которой была использована способность.&lt;ls=50&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Затем верните эту карту игроку, играющему за Л’токк Кхраск.&lt;/fs&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=63&gt;&lt;fs=42&gt;&lt;f=Myriad Pro&gt;Во время тактического дей-&lt;br&gt;ствия, когда вы используете способность &lt;/f&gt;&lt;push=0;14&gt;&lt;f=Russo One;34;0;0;0;0&gt;«БОМБАРДИРОВКА»&lt;/f&gt;&lt;push=0;-14&gt;&lt;f=Myriad Pro&gt; и наносите хотя бы 1 попадание:&lt;/f&gt;&lt;ls=50&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;За каждое нанесённое вами попадание вы можете вместо этого разместить 1 отряд пехоты из вашего снабжения на планете, против которой была использована способность.&lt;ls=50&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Затем верните эту карту&lt;br&gt;игроку, играющему за&lt;br&gt;Л’токк Кхраск.&lt;/fs&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>0.6275;0;0;0;0;0;1.0353;0;0;0;0;0;1.7961;0;0;0;0;0;1;0;0.3725;-0.0353;-0.7961;0;1</t>
@@ -6980,7 +6980,7 @@
     <t>&lt;fs=60&gt;Наставление&lt;br&gt;    Нивин    &lt;/fs&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=75&gt;&lt;fs=50&gt;&lt;f=Myriad Pro&gt;После того как вы активировали систему:&lt;/f&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Во время шага «Передвижение» этого тактического действия игнорируйте эффекты аномалий.&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Затем верните эту карту игроку, играющему за Звёздных Королей Нивин.&lt;/fs&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=75&gt;&lt;fs=50&gt;&lt;f=Myriad Pro&gt;После того как вы активировали систему:&lt;/f&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Во время шага «Передви-&lt;br&gt;жение» этого тактического действия игнорируйте эффекты аномалий.&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Затем верните эту карту игроку, играющему за Звёздных Королей Нивин.&lt;/fs&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>0.8863;0;0;0;0;0;0.8941;0;0;0;0;0;0.8784;0;0;0;0;0;1;0;0.1137;0.1059;0.1216;0;1</t>
@@ -7025,7 +7025,7 @@
     <t>&lt;fs=56&gt;Благосклонность&lt;br&gt;    Родуна    &lt;/fs&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=75&gt;&lt;fs=50&gt;&lt;f=Myriad Pro&gt;Когда вы исследуете технологию и игнорируете требование:&lt;/f&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Вы можете проигнорировать 1 дополнительное требование того же цвета.&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Затем верните эту карту игроку, играющему за Фанатиков Родуна.&lt;/fs&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=75&gt;&lt;fs=50&gt;&lt;f=Myriad Pro&gt;Когда вы исследуете тех-&lt;br&gt;нологию и игнорируете требование:&lt;/f&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Вы можете проигнори-&lt;br&gt;ровать 1 дополнительное требование того же цвета.&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Затем верните эту карту игроку, играющему за Фанатиков Родуна.&lt;/fs&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>1.8745;0;0;0;0;0;0.3608;0;0;0;0;0;0.4314;0;0;0;0;0;1;0;-0.8745;0.6392;0.5686;0;1</t>
@@ -7040,7 +7040,7 @@
     <t>&lt;fs=60&gt;Автоматоны&lt;/fs&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=75&gt;&lt;fs=50&gt;&lt;f=Myriad Pro&gt;В конце вашего хода:&lt;/f&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Можете прикрепить эту карту к неродной подконтрольной вам планете (кроме Мекатол-Рекса). Эта планета имеет способность &lt;/f&gt;&lt;push=0;17&gt;&lt;f=Russo One;40;0;0;0;0&gt;«ПРОИЗВОДСТВО 3»&lt;/f&gt;&lt;push=0;-17&gt;, как если бы это был отряд.&lt;/fs&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=75&gt;&lt;fs=50&gt;&lt;f=Myriad Pro&gt;В конце вашего хода:&lt;/f&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Можете прикрепить эту карту к неродной подкон-&lt;br&gt;трольной вам планете (кроме Мекатол-Рекса).&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Эта планета имеет способ-&lt;br&gt;ность &lt;/f&gt;&lt;push=0;17&gt;&lt;f=Russo One;40;0;0;0;0&gt;«ПРОИЗВОДСТВО 3»&lt;/f&gt;&lt;push=0;-17&gt;, как если бы это был отряд.&lt;/fs&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>1.4667;0;0;0;0;0;1.6941;0;0;0;0;0;0.4627;0;0;0;0;0;1;0;-0.4667;-0.6941;0.5373;0;1</t>
@@ -7097,7 +7097,7 @@
     <t>&lt;fs=51&gt;    Филиал    &lt;br&gt;Налоговая Гавань&lt;/fs&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=75&gt;&lt;fs=50&gt;Когда вы получаете эту карту, вы должны прикрепить её к неродной подконтрольной вам планете (кроме Мекатол-Рекса), на которой нет филиала.&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Значение влияния этой планеты увеличивается&lt;br&gt;на 1.&lt;/fs&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=69&gt;&lt;fs=46&gt;Когда вы получаете эту карту, вы должны прикрепить её к неродной подконтрольной вам планете (кроме Мекатол-Рекса), на которой нет филиала.&lt;ls=55&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Значение влияния этой планеты увеличивается на 1.&lt;/fs&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>1.8431;0;0;0;0;0;0.5569;0;0;0;0;0;0.3922;0;0;0;0;0;1;0;-0.8431;0.4431;0.6078;0;1</t>
@@ -7115,7 +7115,7 @@
     <t>&lt;fs=51&gt;    Филиал    &lt;br&gt;Резервный Банк&lt;/fs&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=75&gt;&lt;fs=50&gt;Когда вы получаете эту карту, вы должны прикрепить её к неродной подконтрольной вам планете (кроме Мекатол-Рекса), на которой нет филиала.&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Значение ресурсов этой планеты увеличивается&lt;br&gt;на 1.&lt;/fs&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=69&gt;&lt;fs=46&gt;Когда вы получаете эту карту, вы должны прикрепить её к неродной подконтрольной вам планете (кроме Мекатол-Рекса), на которой нет филиала.&lt;ls=55&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Значение ресурсов этой планеты увеличивается на 1.&lt;/fs&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>&lt;fs=51&gt;    Филиал    &lt;br&gt;Орбитальная Верфь&lt;/fs&gt;</t>
@@ -7124,7 +7124,7 @@
     <t>&lt;fs=51&gt;Гиперкинетический Боеприпас&lt;/fs&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=75&gt;&lt;fs=50&gt;&lt;f=Myriad Pro&gt;Перед тем как вы бросите кубики для проверки способности &lt;/f&gt;&lt;push=0;17&gt;&lt;f=Russo One;40;0;0;0;0&gt;«БОМБАРДИРОВКА»&lt;/f&gt;&lt;push=0;-17&gt;:&lt;/f&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Если вы наносите хотя бы 1 попадание во время этой проверки, нанесите 1 дополнительное попадание.&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Затем верните эту карту игроку, играющему&lt;br&gt;за Зелиана.&lt;/fs&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=75&gt;&lt;fs=50&gt;&lt;f=Myriad Pro&gt;Перед тем как вы бросите кубики для проверки способности &lt;/f&gt;&lt;push=0;17&gt;&lt;f=Russo One;40;0;0;0;0&gt;«БОМБАРДИ-&lt;br&gt;РОВКА»&lt;/f&gt;&lt;push=-4;-17&gt;:&lt;/f&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Если вы наносите хотя бы 1 попадание во время этой проверки, нанесите 1 дополнительное попадание.&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;Затем верните эту карту игроку, играющему&lt;br&gt;за Зелиана.&lt;/fs&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>0.4392;0;0;0;0;0;1.9373;0;0;0;0;0;1.9137;0;0;0;0;0;1;0;0.5608;-0.9373;-0.9137;0;1</t>
@@ -24977,7 +24977,7 @@
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="F3" sqref="F3:J39"/>
+      <selection pane="bottomLeft" activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>
@@ -25236,7 +25236,7 @@
       <c r="D9" s="9" t="s">
         <v>2192</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="10" t="s">
         <v>2193</v>
       </c>
       <c r="F9" s="10" t="s">
@@ -25940,7 +25940,7 @@
       <c r="D31" s="9" t="s">
         <v>2297</v>
       </c>
-      <c r="E31" s="9" t="s">
+      <c r="E31" s="10" t="s">
         <v>2298</v>
       </c>
       <c r="F31" s="10" t="s">
@@ -26068,7 +26068,7 @@
       <c r="D35" s="9" t="s">
         <v>2316</v>
       </c>
-      <c r="E35" s="9" t="s">
+      <c r="E35" s="10" t="s">
         <v>2317</v>
       </c>
       <c r="F35" s="10" t="s">
@@ -26100,7 +26100,7 @@
       <c r="D36" s="9" t="s">
         <v>2321</v>
       </c>
-      <c r="E36" s="9" t="s">
+      <c r="E36" s="10" t="s">
         <v>2317</v>
       </c>
       <c r="F36" s="10" t="s">
@@ -26132,7 +26132,7 @@
       <c r="D37" s="9" t="s">
         <v>2322</v>
       </c>
-      <c r="E37" s="9" t="s">
+      <c r="E37" s="10" t="s">
         <v>2323</v>
       </c>
       <c r="F37" s="10" t="s">
@@ -26164,7 +26164,7 @@
       <c r="D38" s="9" t="s">
         <v>2324</v>
       </c>
-      <c r="E38" s="9" t="s">
+      <c r="E38" s="10" t="s">
         <v>2323</v>
       </c>
       <c r="F38" s="10" t="s">

</xml_diff>

<commit_message>
expansion icons & leaders inactive
</commit_message>
<xml_diff>
--- a/Template_Data.xlsx
+++ b/Template_Data.xlsx
@@ -2894,13 +2894,13 @@
     <t>&lt;fc=CF14EE&gt;&lt;fs=36&gt;Дальновидный Исследователь&lt;/fs&gt;&lt;/fc&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=63&gt;&lt;f=Myriad Pro;42;1;0;0;0&gt;РАЗБЛОКИРОВКА:&lt;/f&gt;&lt;f=Myriad Pro Light;42;1;0;0;0&gt;&lt;br&gt;у вас должно быть 3 выполненные цели.&lt;/f&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=63&gt;&lt;f=Myriad Pro;42;1;0;0;0&gt;РАЗБЛОКИРОВКА:&lt;/f&gt;&lt;f=Myriad Pro Light;42;1;0;0;0&gt;&lt;br&gt;у вас должно быть 3&lt;br&gt;выполненные цели.&lt;/f&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>&lt;ls=75&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt;&lt;f=Myriad Pro;50;1;0;0;0&gt;ДЕЙСТВИЕ: &lt;/f&gt;изгоните эту карту, чтобы разведать каждую подконтрольную вам планету, в любом порядке.&lt;/f&gt;&lt;/ls&gt;</t>
   </si>
   <si>
-    <t>&lt;f=Myriad Pro Light;40;1;0;1;0&gt;&lt;ls=62&gt;«Удвойте свои усилия, мы должны выполнить квартальный план». Конгломерат ещё никогда не сры-&lt;br&gt;вал сроков, и новый гендиректор готов был разорвать на части целые миры, чтобы так продолжалось и дальше.&lt;/ls&gt;&lt;/f&gt;</t>
+    <t>&lt;f=Myriad Pro Light;40;1;0;1;0&gt;&lt;ls=62&gt;«Удвойте свои усилия, мы должны выполнить квартальный план». Конгломерат ещё никогда не сры-&lt;br&gt;вал сроков, и новый гендиректор готов был разорвать на части целые миры, чтобы так продолжалось&lt;br&gt;и дальше.&lt;/ls&gt;&lt;/f&gt;</t>
   </si>
   <si>
     <t>Celdauri</t>
@@ -3311,7 +3311,7 @@
     <t>&lt;ls=75&gt;&lt;f=Myriad Pro;50;1;0;0;0&gt;Во время тактического действия, после того, как&lt;br&gt;вы получаете контроль&lt;br&gt;над неродной планетой&lt;br&gt;в активной системе,&lt;br&gt;в которой есть хотя&lt;br&gt;бы 1 ваш корабль:&lt;/f&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt;Можете произвести 1&lt;br&gt;корабль в этой системе.&lt;/f&gt;&lt;/ls&gt;</t>
   </si>
   <si>
-    <t>&lt;f=Myriad Pro Light;44;1;0;1;0&gt;&lt;ls=68&gt;Первый президент Содружества была избрана за то, что была миротворцем и дипломатом. Это было&lt;br&gt;мирное время.&lt;/ls&gt;&lt;/f&gt;</t>
+    <t>&lt;f=Myriad Pro Light;44;1;0;1;0&gt;&lt;ls=68&gt;Первый президент Содружества была избрана за то, что была миротворцем и дипломатом. Это было мирное время.&lt;/ls&gt;&lt;/f&gt;</t>
   </si>
   <si>
     <t>&lt;fs=64&gt;Сердце Восстания&lt;/fs&gt;</t>
@@ -3374,7 +3374,7 @@
     <t>&lt;ls=75&gt;&lt;f=Myriad Pro;50;1;0;0;0&gt;После того как вы выиграли бой в системе, в которой нет планет, или на планете, на которой есть сооружение:&lt;/f&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt;Можете получить 1 товар.&lt;/f&gt;&lt;/ls&gt;</t>
   </si>
   <si>
-    <t>&lt;f=Myriad Pro Light;44;1;0;1;0&gt;&lt;ls=68&gt;Ярлы выбираются из своих местных кланов, чтобы возглавить военные отряды Гемины; из них только самые свирепые поднимаются до почётного звания лидеров двойных рейдов.&lt;/ls&gt;&lt;/f&gt;</t>
+    <t>&lt;f=Myriad Pro Light;44;1;0;1;0&gt;&lt;ls=68&gt;Ярлы выбираются из своих мест-&lt;br&gt;ных кланов, чтобы возглавить военные отряды Гемины; из них только самые свирепые поднимаются до почётного звания лидеров двойных рейдов.&lt;/ls&gt;&lt;/f&gt;</t>
   </si>
   <si>
     <t>10_1</t>
@@ -3686,7 +3686,7 @@
     <t>&lt;ls=66&gt;&lt;f=Myriad Pro Light;44;1;0;0;0&gt;Эта карта удовлетворяет синему требованию технологии.&lt;/ls&gt;&lt;ls=53&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;&lt;ls=66&gt;Когда вы отступаете, если в активной системе нет вашего жетона приказа, вы не размещаете жетон приказа&lt;br&gt;в систему, в которую&lt;br&gt;отступили ваши отряды.&lt;/f&gt;&lt;/ls&gt;</t>
   </si>
   <si>
-    <t>&lt;f=Myriad Pro Light;42;1;0;1;0&gt;&lt;ls=65&gt;Известный уклонением от захвата, бесследным исчезновением и безрассудными прыжковыми маневрами, Кадо «Дым» С’мах-Кар — известный пилот и контрабандист.&lt;/ls&gt;&lt;/f&gt;</t>
+    <t>&lt;f=Myriad Pro Light;42;1;0;1;0&gt;&lt;ls=65&gt;Известный уклонением от&lt;br&gt;захвата, бесследным исчезновением и безрассудными прыжковыми маневрами, Кадо «Дым» С’мах-Кар — известный пилот и контрабандист.&lt;/ls&gt;&lt;/f&gt;</t>
   </si>
   <si>
     <t>B</t>
@@ -3806,7 +3806,7 @@
     <t>&lt;ls=75&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt;Во время первого раунда&lt;br&gt;боя, вы можете отменить&lt;br&gt;1 попадание.&lt;/f&gt;&lt;/ls&gt;</t>
   </si>
   <si>
-    <t>&lt;f=Myriad Pro Light;44;1;0;1;0&gt;&lt;ls=68&gt;Корталии верят, что только самые стойкие из их воинов будут удостоены высшей чести перерождения&lt;br&gt;в Рыцарей Королев.&lt;/ls&gt;&lt;/f&gt;</t>
+    <t>&lt;f=Myriad Pro Light;44;1;0;1;0&gt;&lt;ls=68&gt;Корталии верят, что только самые стойкие из их воинов будут удостоены высшей чести перерождения в Рыцарей&lt;br&gt;Королев.&lt;/ls&gt;&lt;/f&gt;</t>
   </si>
   <si>
     <t>&lt;fs=64&gt;Зов Королев&lt;/fs&gt;</t>
@@ -3821,7 +3821,7 @@
     <t>&lt;fc=FFFFFF&gt;&lt;fs=40&gt;Жизнь и Смерть&lt;/fs&gt;&lt;/fc&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=66&gt;&lt;f=Myriad Pro;44;1;0;0;0&gt;РАЗБЛОКИРОВКА:&lt;/f&gt;&lt;f=Myriad Pro Light;44;1;0;0;0&gt;&lt;br&gt;у вас должно быть 3 выполненные цели.&lt;/f&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=66&gt;&lt;f=Myriad Pro;44;1;0;0;0&gt;РАЗБЛОКИРОВКА:&lt;/f&gt;&lt;f=Myriad Pro Light;44;1;0;0;0&gt;&lt;br&gt;у вас должно быть 3&lt;br&gt;выполненные цели.&lt;/f&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>&lt;ls=75&gt;&lt;f=Myriad Pro;50;1;0;0;0&gt;После того как вы выиграли бой:&lt;/f&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt;Можете изгнать эту карту, чтобы выбрать 1 из реликвий вашего противника и взять её себе. Затем,&lt;br&gt;за каждую подконтрольную вам легендарную планету или планету с технологической специализацией, получите 1 жетон приказа.&lt;/f&gt;&lt;/ls&gt;</t>
@@ -3932,7 +3932,7 @@
     <t>&lt;ls=75&gt;&lt;f=Myriad Pro;50;1;0;0;0&gt;После того как вы разведали планету:&lt;/f&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt;Можете разместить 1 отряд пехоты из вашего снабжения на этой планете.&lt;/f&gt;&lt;/ls&gt;</t>
   </si>
   <si>
-    <t>&lt;f=Myriad Pro Light;44;1;0;1;0&gt;&lt;ls=68&gt;«Ненавижу всё это старьё, оно просто собирает здесь пыль. Мы должны что-то с этим сделать!»&lt;/ls&gt;&lt;/f&gt;</t>
+    <t>&lt;f=Myriad Pro Light;44;1;0;1;0&gt;&lt;ls=68&gt;«Ненавижу всё это старьё,&lt;br&gt;оно просто собирает здесь&lt;br&gt;пыль. Мы должны что-то&lt;br&gt;с этим сделать!»&lt;/ls&gt;&lt;/f&gt;</t>
   </si>
   <si>
     <t>&lt;fs=64&gt;Каскадный резонанс&lt;/fs&gt;</t>
@@ -3986,7 +3986,7 @@
     <t>&lt;fc=FCAD04&gt;&lt;fs=40&gt;Безжалостный стратег&lt;/fs&gt;&lt;/fc&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=75&gt;&lt;f=Myriad Pro;50;1;0;0;0&gt;РАЗБЛОКИРОВКА:&lt;/f&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt; у вас должно быть на игровом поле хотя бы 4 прикреп-&lt;br&gt;лённых карты ловушек.&lt;/f&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=75&gt;&lt;f=Myriad Pro;50;1;0;0;0&gt;РАЗБЛОКИРОВКА:&lt;/f&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt; у вас должно быть на игровом поле хотя бы 4 прикреплённых карты ловушек.&lt;/f&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>&lt;ls=75&gt;&lt;f=Myriad Pro;50;1;0;0;0&gt;Во время раунда боя, в котором участвует не более 1 вашего корабля (кроме истребителей) или 1&lt;br&gt;вашего отряда пехоты:&lt;/f&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt;Можете выбрать 1 ваш отряд&lt;br&gt;в этом бою; этот отряд бро-&lt;br&gt;сает 1 дополнительный кубик.&lt;/f&gt;&lt;/ls&gt;</t>
@@ -4046,7 +4046,7 @@
     <t>&lt;fc=05F9F6&gt;&lt;fs=40&gt;Кристаллический Друид&lt;/fs&gt;&lt;/fc&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=75&gt;&lt;f=Myriad Pro;50;1;0;0;0&gt;РАЗБЛОКИРОВКА:&lt;/f&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt; выиграйте наземный бой на неподконтрольной вам планете.&lt;/f&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=75&gt;&lt;f=Myriad Pro;50;1;0;0;0&gt;РАЗБЛОКИРОВКА:&lt;/f&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt;&lt;br&gt;выиграйте наземный бой на неподконтрольной вам планете.&lt;/f&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>&lt;ls=75&gt;&lt;f=Myriad Pro;50;1;0;0;0&gt;В начале вторжения:&lt;/f&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt;Можете разместить 1 отряд пехоты из вашего снабже-&lt;br&gt;ния в космосе этой системы, если у вас есть неиспользо-&lt;br&gt;ванные места в активной системе.&lt;/f&gt;&lt;/ls&gt;</t>
@@ -4112,7 +4112,7 @@
     <t>&lt;ls=63&gt;&lt;f=Myriad Pro Light;42;1;0;0;0&gt;Во время шага «Передвижение» ваших тактических действий вы можете заменить любое коли-&lt;br&gt;чество перевозимых отрядов пехоты на такое же количество истребителей.&lt;/ls&gt;&lt;ls=50&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;&lt;ls=63&gt;Вы можете использовать способ-&lt;br&gt;ность &lt;/f&gt;&lt;push=0;14&gt;&lt;f=Russo One;34;0;0;0;0&gt;«КОСМИЧЕСКАЯ ПУШКА»&lt;/f&gt;&lt;push=0;-14&gt;&lt;f=Myriad Pro Light;42;1;0;0;0&gt; одного из ваших отрядов против отрядов в смежных системах.&lt;/f&gt;&lt;/ls&gt;</t>
   </si>
   <si>
-    <t>&lt;f=Myriad Pro Light;40;1;0;1;0&gt;&lt;ls=62&gt;Мирведа давно освоила техно-&lt;br&gt;логию боевого схода с орбиты, но лишь недавно её ИИ, судя по всему, нашёл способ модернизировать эти штурмовые аппараты для сражения в космосе после продол-&lt;br&gt;жительных операций на планетах.&lt;/ls&gt;&lt;/f&gt;</t>
+    <t>&lt;f=Myriad Pro Light;40;1;0;1;0&gt;&lt;ls=62&gt;Мирведа давно освоила техно-&lt;br&gt;логию боевого схода с орбиты, но лишь недавно её ИИ, судя по всему, нашёл способ модернизировать эти штурмовые аппараты для сражения в космосе после продолжитель-&lt;br&gt;ных операций на планетах.&lt;/ls&gt;&lt;/f&gt;</t>
   </si>
   <si>
     <t>&lt;fs=64&gt;Молот Дхора&lt;/fs&gt;</t>
@@ -4130,7 +4130,7 @@
     <t>&lt;ls=66&gt;&lt;f=Myriad Pro Light;44;1;0;0;0&gt;&lt;f=Myriad Pro;44;1;0;0;0&gt;ДЕЙСТВИЕ: &lt;/f&gt;разместите до 3 ПСО из вашего снабжения на подконтрольных вам планетах. Выберите 1 систему; ваши ПСО могут использовать свою способность &lt;/f&gt;&lt;push=0;15&gt;&lt;f=Russo One;35;0;0;0;0&gt;«КОСМИЧЕСКАЯ ПУШКА»&lt;/f&gt;&lt;push=0;-15&gt;&lt;f=Myriad Pro Light;44;1;0;0;0&gt; против кораблей в этой системе и способность &lt;/f&gt;&lt;push=0;15&gt;&lt;f=Russo One;35;0;0;0;0&gt;«БОМБАРДИ-&lt;br&gt;РОВКА»&lt;/f&gt;&lt;push=0;-15&gt;&lt;f=Myriad Pro Light;44;1;0;0;0&gt; против отрядов на одной планете&lt;br&gt;в этой системе.&lt;/ls&gt;&lt;ls=53&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;&lt;ls=66&gt;Затем изгоните эту карту.&lt;/f&gt;&lt;/ls&gt;</t>
   </si>
   <si>
-    <t>&lt;f=Myriad Pro Light;38;1;0;1;0&gt;&lt;ls=59&gt;ИИ Мирведы на самом деле представляет собой кластер интеллектов, каждый из которых обладает личностью и специализацией. Одни сохраняют безупречный контроль, другие — совершенно безумны, и с ними консультируются только в случае крайней необходимости. &lt;/ls&gt;&lt;/f&gt;</t>
+    <t>&lt;f=Myriad Pro Light;38;1;0;1;0&gt;&lt;ls=59&gt;ИИ Мирведы на самом деле представ-&lt;br&gt;ляет собой кластер интеллектов, каждый из которых обладает личностью и специализацией. Одни сохраняют безупречный контроль, другие — совершенно безумны, и с ними консультируются только в случае крайней необходимости. &lt;/ls&gt;&lt;/f&gt;</t>
   </si>
   <si>
     <t>Mortheus</t>
@@ -4175,7 +4175,7 @@
     <t>&lt;ls=75&gt;&lt;f=Myriad Pro;50;1;0;0;0&gt;В начале космического боя, если вы не являетесь активным игроком:&lt;/f&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt;Выберите 1 ваш корабль (кроме истребителей) в активной системе. Во время этого боя он получает спо-&lt;br&gt;собность &lt;/f&gt;&lt;push=0;17&gt;&lt;f=Russo One;40;0;0;0;0&gt;«ПОГЛОЩЕНИЕ УРОНА»&lt;/f&gt;&lt;push=0;-17&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt;.&lt;/f&gt;&lt;/ls&gt;</t>
   </si>
   <si>
-    <t>&lt;f=Myriad Pro Light;44;1;0;1;0&gt;&lt;ls=68&gt;«Как высокомерно полагать, что ваши простые чувства позволяют вам познать пределы этой реальности».&lt;/ls&gt;&lt;/f&gt;</t>
+    <t>&lt;f=Myriad Pro Light;44;1;0;1;0&gt;&lt;ls=68&gt;«Как высокомерно полагать, что ваши простые чувства позво-&lt;br&gt;ляют вам познать пределы этой реальности».&lt;/ls&gt;&lt;/f&gt;</t>
   </si>
   <si>
     <t>&lt;fs=56&gt;Репликатор Переплетений&lt;/fs&gt;</t>
@@ -4472,7 +4472,7 @@
     <t>&lt;ls=75&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt;Когда вы исследуете техно-&lt;br&gt;логию, можете использовать технологическую специали-&lt;br&gt;зацию 1 подконтрольной вам планеты, чтобы проигнори-&lt;br&gt;ровать 1 любое требование.&lt;/f&gt;&lt;/ls&gt;</t>
   </si>
   <si>
-    <t>&lt;f=Myriad Pro Light;44;1;0;1;0&gt;&lt;ls=68&gt;«Эти священные миры и хранящиеся в них сокровища — не просто короткий путь к знаниям. Это дары для нас, достойных, от тех, кто был&lt;br&gt;до нас».&lt;/ls&gt;&lt;/f&gt;</t>
+    <t>&lt;f=Myriad Pro Light;44;1;0;1;0&gt;&lt;ls=68&gt;«Эти священные миры и хранящиеся в них сокровища — не просто короткий путь к знаниям. Это дары для нас, достойных, от тех, кто был до нас».&lt;/ls&gt;&lt;/f&gt;</t>
   </si>
   <si>
     <t>&lt;fs=64&gt;Благословение Древних&lt;/fs&gt;</t>
@@ -4523,7 +4523,7 @@
     <t>&lt;fc=8D8971&gt;&lt;fs=40&gt;Доминирующий Конструктор&lt;/fs&gt;&lt;/fc&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=75&gt;&lt;f=Myriad Pro;50;1;0;0;0&gt;РАЗБЛОКИРОВКА:&lt;/f&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt; у вас должны быть отряды в одной системе с суммарным значением &lt;/f&gt;&lt;push=0;17&gt;&lt;f=Russo One;40;0;0;0;0&gt;«ПРОИЗВОДСТВА»&lt;/f&gt;&lt;push=0;-17&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt; 8 или больше.&lt;/f&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=75&gt;&lt;f=Myriad Pro;50;1;0;0;0&gt;РАЗБЛОКИРОВКА:&lt;/f&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt; у вас должны быть отряды в одной системе с суммарным значе-&lt;br&gt;нием &lt;/f&gt;&lt;push=0;17&gt;&lt;f=Russo One;40;0;0;0;0&gt;«ПРОИЗВОДСТВА»&lt;/f&gt;&lt;push=0;-17&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt; 8 или больше.&lt;/f&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>&lt;ls=75&gt;&lt;f=Myriad Pro;50;1;0;0;0&gt;Когда вы тратите жетон приказа, чтобы применить второстепенную способ-&lt;br&gt;ность карты стратегии «Строительство»:&lt;/f&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt;Можете вместо этого применить основную способность.&lt;/f&gt;&lt;/ls&gt;</t>
@@ -4625,7 +4625,7 @@
     <t>&lt;ls=66&gt;&lt;f=Myriad Pro;44;1;0;0;0&gt;В начале хода любого игрока:&lt;/f&gt;&lt;ls=53&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;&lt;f=Myriad Pro Light;44;1;0;0;0&gt;Можете перевернуть эту карту, чтобы позволить этому игроку выбрать подконтрольную ему планету; этот игрок получает количество продукции, равное значению влияния этой планеты.&lt;/f&gt;&lt;/ls&gt;</t>
   </si>
   <si>
-    <t>&lt;f=Myriad Pro Light;44;1;0;1;0&gt;&lt;ls=68&gt;Юдри Сухов — специалист по «переговорам» с упрямыми местными жителями, препят-&lt;br&gt;ствующими деятельности Банковских кланов. Он и его отряд хорошо вооружённых «консультантов» редко уходят с таких «переговоров» с пустыми руками.&lt;/ls&gt;&lt;/f&gt;</t>
+    <t>&lt;f=Myriad Pro Light;44;1;0;1;0&gt;&lt;ls=68&gt;Юдри Сухов — специалист по «переговорам» с упрямыми местными жителями, препят-&lt;br&gt;ствующими деятельности Банковских кланов. Он и его отряд хорошо вооружённых «консуль-&lt;br&gt;тантов» редко уходят с таких «переговоров» с пустыми руками.&lt;/ls&gt;&lt;/f&gt;</t>
   </si>
   <si>
     <t>E7F002</t>
@@ -4643,7 +4643,7 @@
     <t>&lt;fc=D6EF3D&gt;&lt;fs=40&gt;Банкир&lt;/fs&gt;&lt;/fc&gt;</t>
   </si>
   <si>
-    <t>&lt;ls=60&gt;&lt;f=Myriad Pro;40;1;0;0;0&gt;РАЗБЛОКИРОВКА:&lt;/f&gt;&lt;f=Myriad Pro Light;40;1;0;0;0&gt; на вашем планшете фракции должны быть жетоны контроля хотя бы половины от общего числа игроков (с округлением вниз).&lt;/f&gt;&lt;/ls&gt;</t>
+    <t>&lt;ls=60&gt;&lt;f=Myriad Pro;40;1;0;0;0&gt;РАЗБЛОКИРОВКА:&lt;/f&gt;&lt;f=Myriad Pro Light;40;1;0;0;0&gt; на вашем планшете фракции должны быть жетоны контроля хотя бы половины от общего числа игроков&lt;br&gt;(с округлением вниз).&lt;/f&gt;&lt;/ls&gt;</t>
   </si>
   <si>
     <t>&lt;ls=75&gt;&lt;f=Myriad Pro;50;1;0;0;0&gt;В начале фазы статуса:&lt;/f&gt;&lt;ls=60&gt;&lt;br&gt;&lt;br&gt;&lt;/ls&gt;&lt;f=Myriad Pro Light;50;1;0;0;0&gt;Получите 1 товар за каждую выполненную секретную цель и 1 продукцию за каждую выполненную&lt;br&gt;общую цель.&lt;/f&gt;&lt;/ls&gt;</t>
@@ -10653,10 +10653,10 @@
   <sheetPr/>
   <dimension ref="A1:S189"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A65" activePane="bottomLeft" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="C1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A59" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="D105" sqref="D105"/>
+      <selection pane="bottomLeft" activeCell="K94" sqref="K94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15"/>

</xml_diff>

<commit_message>
action & agenda fixes
</commit_message>
<xml_diff>
--- a/Template_Data.xlsx
+++ b/Template_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12885" tabRatio="796"/>
+    <workbookView windowWidth="14745" windowHeight="11880" tabRatio="796"/>
   </bookViews>
   <sheets>
     <sheet name="Actions" sheetId="14" r:id="rId1"/>
@@ -70,7 +70,7 @@
     <t>Images\Logo_Uncharted_Space.png</t>
   </si>
   <si>
-    <t>Images\Action\Action_Background.png</t>
+    <t>Images\Action\Action_Front.png</t>
   </si>
   <si>
     <t>&lt;fs=56&gt;Дипломатическое давление&lt;/fs&gt;</t>
@@ -9559,9 +9559,9 @@
   <dimension ref="A1:F61"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A35" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="C52" sqref="C52"/>
+      <selection pane="bottomLeft" activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="5"/>

</xml_diff>